<commit_message>
Diagrama de Gantt modificado - fechas actualizadas
</commit_message>
<xml_diff>
--- a/Análisis/Diagrama de Gantt.xlsx
+++ b/Análisis/Diagrama de Gantt.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EEDAFE-E1FF-4AD5-97D4-0D509B92738A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D75649-A6EE-458B-808B-2CCF86D5997A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CalendarioProyecto" sheetId="11" r:id="rId1"/>
@@ -28,7 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -5355,11 +5357,11 @@
   <dimension ref="A1:DW42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="29.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="27" customWidth="1"/>
     <col min="2" max="2" width="38.21875" customWidth="1"/>
@@ -5405,7 +5407,7 @@
     <col min="126" max="127" width="3.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:127" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -5419,7 +5421,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="10"/>
     </row>
-    <row r="2" spans="1:127" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
@@ -5428,7 +5430,7 @@
       </c>
       <c r="I2" s="29"/>
     </row>
-    <row r="3" spans="1:127" ht="29.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:127" ht="29.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>2</v>
       </c>
@@ -5442,7 +5444,7 @@
       </c>
       <c r="F3" s="113"/>
     </row>
-    <row r="4" spans="1:127" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="28" t="s">
         <v>35</v>
       </c>
@@ -6111,7 +6113,7 @@
         <v>44010</v>
       </c>
     </row>
-    <row r="6" spans="1:127" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:127" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="28" t="s">
         <v>4</v>
       </c>
@@ -6609,7 +6611,7 @@
         <v>d</v>
       </c>
     </row>
-    <row r="7" spans="1:127" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:127" ht="29.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="27" t="s">
         <v>5</v>
       </c>
@@ -6739,7 +6741,7 @@
       <c r="DV7" s="16"/>
       <c r="DW7" s="16"/>
     </row>
-    <row r="8" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="28" t="s">
         <v>6</v>
       </c>
@@ -6875,7 +6877,7 @@
       <c r="DV8" s="16"/>
       <c r="DW8" s="16"/>
     </row>
-    <row r="9" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="28" t="s">
         <v>7</v>
       </c>
@@ -7017,7 +7019,7 @@
       <c r="DV9" s="16"/>
       <c r="DW9" s="16"/>
     </row>
-    <row r="10" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="28" t="s">
         <v>8</v>
       </c>
@@ -7153,7 +7155,7 @@
       <c r="DV10" s="16"/>
       <c r="DW10" s="16"/>
     </row>
-    <row r="11" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="27"/>
       <c r="B11" s="43" t="s">
         <v>53</v>
@@ -7293,7 +7295,7 @@
       <c r="DV11" s="16"/>
       <c r="DW11" s="16"/>
     </row>
-    <row r="12" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="27"/>
       <c r="B12" s="43" t="s">
         <v>54</v>
@@ -7431,7 +7433,7 @@
       <c r="DV12" s="16"/>
       <c r="DW12" s="16"/>
     </row>
-    <row r="13" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="27"/>
       <c r="B13" s="14" t="s">
         <v>40</v>
@@ -7565,7 +7567,7 @@
       <c r="DV13" s="16"/>
       <c r="DW13" s="16"/>
     </row>
-    <row r="14" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
         <v>9</v>
       </c>
@@ -7705,7 +7707,7 @@
       <c r="DV14" s="16"/>
       <c r="DW14" s="16"/>
     </row>
-    <row r="15" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="28"/>
       <c r="B15" s="44" t="s">
         <v>45</v>
@@ -7843,7 +7845,7 @@
       <c r="DV15" s="16"/>
       <c r="DW15" s="16"/>
     </row>
-    <row r="16" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="27"/>
       <c r="B16" s="44" t="s">
         <v>46</v>
@@ -7981,7 +7983,7 @@
       <c r="DV16" s="16"/>
       <c r="DW16" s="16"/>
     </row>
-    <row r="17" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="27"/>
       <c r="B17" s="44" t="s">
         <v>47</v>
@@ -8119,7 +8121,7 @@
       <c r="DV17" s="16"/>
       <c r="DW17" s="16"/>
     </row>
-    <row r="18" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="27"/>
       <c r="B18" s="44" t="s">
         <v>48</v>
@@ -8257,7 +8259,7 @@
       <c r="DV18" s="16"/>
       <c r="DW18" s="16"/>
     </row>
-    <row r="19" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="27"/>
       <c r="B19" s="15" t="s">
         <v>41</v>
@@ -8391,7 +8393,7 @@
       <c r="DV19" s="16"/>
       <c r="DW19" s="16"/>
     </row>
-    <row r="20" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="27" t="s">
         <v>10</v>
       </c>
@@ -8401,15 +8403,15 @@
       <c r="C20" s="41"/>
       <c r="D20" s="58"/>
       <c r="E20" s="70">
-        <v>43923</v>
+        <v>43941</v>
       </c>
       <c r="F20" s="70">
-        <v>43925</v>
+        <v>43942</v>
       </c>
       <c r="G20" s="11"/>
       <c r="H20" s="11">
         <f t="shared" si="53"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
@@ -8531,7 +8533,7 @@
       <c r="DV20" s="16"/>
       <c r="DW20" s="16"/>
     </row>
-    <row r="21" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="27"/>
       <c r="B21" s="45" t="s">
         <v>50</v>
@@ -8669,7 +8671,7 @@
       <c r="DV21" s="16"/>
       <c r="DW21" s="16"/>
     </row>
-    <row r="22" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="27"/>
       <c r="B22" s="45" t="s">
         <v>46</v>
@@ -8677,15 +8679,15 @@
       <c r="C22" s="41"/>
       <c r="D22" s="58"/>
       <c r="E22" s="70">
-        <v>43926</v>
+        <v>43952</v>
       </c>
       <c r="F22" s="70">
-        <v>43938</v>
+        <v>43968</v>
       </c>
       <c r="G22" s="11"/>
       <c r="H22" s="11">
         <f t="shared" si="53"/>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I22" s="16"/>
       <c r="J22" s="16"/>
@@ -8807,7 +8809,7 @@
       <c r="DV22" s="16"/>
       <c r="DW22" s="16"/>
     </row>
-    <row r="23" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="27"/>
       <c r="B23" s="45" t="s">
         <v>51</v>
@@ -8945,7 +8947,7 @@
       <c r="DV23" s="16"/>
       <c r="DW23" s="16"/>
     </row>
-    <row r="24" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="27"/>
       <c r="B24" s="45" t="s">
         <v>48</v>
@@ -8953,16 +8955,16 @@
       <c r="C24" s="41"/>
       <c r="D24" s="58"/>
       <c r="E24" s="70">
-        <f>F21</f>
-        <v>43933</v>
+        <f>E22</f>
+        <v>43952</v>
       </c>
       <c r="F24" s="70">
-        <v>43939</v>
+        <v>43969</v>
       </c>
       <c r="G24" s="11"/>
       <c r="H24" s="11">
         <f t="shared" si="53"/>
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="I24" s="16"/>
       <c r="J24" s="16"/>
@@ -9084,7 +9086,7 @@
       <c r="DV24" s="16"/>
       <c r="DW24" s="16"/>
     </row>
-    <row r="25" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="27"/>
       <c r="B25" s="45" t="s">
         <v>47</v>
@@ -9092,16 +9094,16 @@
       <c r="C25" s="41"/>
       <c r="D25" s="58"/>
       <c r="E25" s="70">
-        <f>F21</f>
-        <v>43933</v>
+        <f>E23</f>
+        <v>43926</v>
       </c>
       <c r="F25" s="70">
-        <v>43939</v>
+        <v>43969</v>
       </c>
       <c r="G25" s="11"/>
       <c r="H25" s="11">
         <f t="shared" si="53"/>
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="I25" s="16"/>
       <c r="J25" s="16"/>
@@ -9223,7 +9225,7 @@
       <c r="DV25" s="16"/>
       <c r="DW25" s="16"/>
     </row>
-    <row r="26" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="27" t="s">
         <v>10</v>
       </c>
@@ -9236,12 +9238,12 @@
         <v>43941</v>
       </c>
       <c r="F26" s="70">
-        <v>43949</v>
+        <v>43971</v>
       </c>
       <c r="G26" s="11"/>
       <c r="H26" s="11">
         <f t="shared" si="53"/>
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="I26" s="16"/>
       <c r="J26" s="16"/>
@@ -9363,7 +9365,7 @@
       <c r="DV26" s="16"/>
       <c r="DW26" s="16"/>
     </row>
-    <row r="27" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="27"/>
       <c r="B27" s="71" t="s">
         <v>42</v>
@@ -9497,7 +9499,7 @@
       <c r="DV27" s="16"/>
       <c r="DW27" s="16"/>
     </row>
-    <row r="28" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="27"/>
       <c r="B28" s="76" t="s">
         <v>55</v>
@@ -9505,11 +9507,11 @@
       <c r="C28" s="77"/>
       <c r="D28" s="78"/>
       <c r="E28" s="79">
-        <v>43950</v>
+        <v>43972</v>
       </c>
       <c r="F28" s="79">
         <f>E28+5</f>
-        <v>43955</v>
+        <v>43977</v>
       </c>
       <c r="G28" s="11"/>
       <c r="H28" s="11">
@@ -9636,7 +9638,7 @@
       <c r="DV28" s="16"/>
       <c r="DW28" s="16"/>
     </row>
-    <row r="29" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="27"/>
       <c r="B29" s="76" t="s">
         <v>56</v>
@@ -9644,11 +9646,11 @@
       <c r="C29" s="77"/>
       <c r="D29" s="78"/>
       <c r="E29" s="79">
-        <v>43950</v>
+        <v>43972</v>
       </c>
       <c r="F29" s="79">
         <f>E29+5</f>
-        <v>43955</v>
+        <v>43977</v>
       </c>
       <c r="G29" s="11"/>
       <c r="H29" s="11">
@@ -9775,7 +9777,7 @@
       <c r="DV29" s="16"/>
       <c r="DW29" s="16"/>
     </row>
-    <row r="30" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="27"/>
       <c r="B30" s="76" t="s">
         <v>57</v>
@@ -9783,11 +9785,11 @@
       <c r="C30" s="77"/>
       <c r="D30" s="78"/>
       <c r="E30" s="79">
-        <v>43950</v>
+        <v>43972</v>
       </c>
       <c r="F30" s="79">
         <f>E30+5</f>
-        <v>43955</v>
+        <v>43977</v>
       </c>
       <c r="G30" s="11"/>
       <c r="H30" s="11">
@@ -9914,7 +9916,7 @@
       <c r="DV30" s="16"/>
       <c r="DW30" s="16"/>
     </row>
-    <row r="31" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="27"/>
       <c r="B31" s="76" t="s">
         <v>58</v>
@@ -9923,11 +9925,11 @@
       <c r="D31" s="78"/>
       <c r="E31" s="79">
         <f>F30+1</f>
-        <v>43956</v>
+        <v>43978</v>
       </c>
       <c r="F31" s="79">
         <f>E31+6</f>
-        <v>43962</v>
+        <v>43984</v>
       </c>
       <c r="G31" s="11"/>
       <c r="H31" s="11">
@@ -10054,7 +10056,7 @@
       <c r="DV31" s="16"/>
       <c r="DW31" s="16"/>
     </row>
-    <row r="32" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="27" t="s">
         <v>11</v>
       </c>
@@ -10065,11 +10067,11 @@
       <c r="D32" s="78"/>
       <c r="E32" s="79">
         <f>F30+1</f>
-        <v>43956</v>
+        <v>43978</v>
       </c>
       <c r="F32" s="79">
         <f>E32+6</f>
-        <v>43962</v>
+        <v>43984</v>
       </c>
       <c r="G32" s="11"/>
       <c r="H32" s="11">
@@ -10196,7 +10198,7 @@
       <c r="DV32" s="16"/>
       <c r="DW32" s="16"/>
     </row>
-    <row r="33" spans="1:127" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="28" t="s">
         <v>12</v>
       </c>
@@ -10332,19 +10334,19 @@
       <c r="DV33" s="16"/>
       <c r="DW33" s="16"/>
     </row>
-    <row r="34" spans="1:127" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="85" t="s">
         <v>44</v>
       </c>
       <c r="C34" s="86"/>
       <c r="D34" s="87"/>
       <c r="E34" s="88">
-        <f>F32+1</f>
-        <v>43963</v>
+        <f>F32+F361</f>
+        <v>43984</v>
       </c>
       <c r="F34" s="88">
         <f>E34+1</f>
-        <v>43964</v>
+        <v>43985</v>
       </c>
       <c r="G34" s="89"/>
       <c r="H34" s="89">
@@ -10471,7 +10473,7 @@
       <c r="DV34" s="90"/>
       <c r="DW34" s="90"/>
     </row>
-    <row r="35" spans="1:127" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="97"/>
       <c r="C35" s="98"/>
       <c r="D35" s="99"/>
@@ -10599,7 +10601,7 @@
       <c r="DV35" s="96"/>
       <c r="DW35" s="96"/>
     </row>
-    <row r="36" spans="1:127" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="101"/>
       <c r="C36" s="92"/>
       <c r="D36" s="93"/>
@@ -10727,7 +10729,7 @@
       <c r="DV36" s="96"/>
       <c r="DW36" s="96"/>
     </row>
-    <row r="37" spans="1:127" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="91"/>
       <c r="C37" s="92"/>
       <c r="D37" s="93"/>
@@ -10855,7 +10857,7 @@
       <c r="DV37" s="96"/>
       <c r="DW37" s="96"/>
     </row>
-    <row r="38" spans="1:127" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="91"/>
       <c r="C38" s="92"/>
       <c r="D38" s="93"/>
@@ -10983,7 +10985,7 @@
       <c r="DV38" s="96"/>
       <c r="DW38" s="96"/>
     </row>
-    <row r="39" spans="1:127" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="91"/>
       <c r="C39" s="92"/>
       <c r="D39" s="93"/>
@@ -11111,7 +11113,7 @@
       <c r="DV39" s="96"/>
       <c r="DW39" s="96"/>
     </row>
-    <row r="40" spans="1:127" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="104"/>
       <c r="C40" s="104"/>
       <c r="D40" s="104"/>
@@ -11239,7 +11241,7 @@
       <c r="DV40" s="104"/>
       <c r="DW40" s="104"/>
     </row>
-    <row r="42" spans="1:127" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="106"/>
     </row>
   </sheetData>
@@ -12925,26 +12927,26 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.95" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="87.109375" style="19" customWidth="1"/>
     <col min="2" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:2" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="46.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:2" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="20"/>
     </row>
-    <row r="3" spans="1:2" s="25" customFormat="1" ht="27.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="25" customFormat="1" ht="27.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="26"/>
     </row>
-    <row r="4" spans="1:2" s="22" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" s="22" customFormat="1" ht="26.05" x14ac:dyDescent="0.5">
       <c r="A4" s="23" t="s">
         <v>22</v>
       </c>
@@ -12954,57 +12956,57 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="26.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="19" customFormat="1" ht="223.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" s="19" customFormat="1" ht="223.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="46" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="22" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:2" s="22" customFormat="1" ht="26.05" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="58.1" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="19" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" s="19" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="22" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:2" s="22" customFormat="1" ht="26.05" x14ac:dyDescent="0.5">
       <c r="A11" s="23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="29.05" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="19" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" s="19" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="47" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="22" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:2" s="22" customFormat="1" ht="26.05" x14ac:dyDescent="0.5">
       <c r="A14" s="23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="91.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="91.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="87.15" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Cronograma de actividades actualizado
</commit_message>
<xml_diff>
--- a/Análisis/Diagrama de Gantt.xlsx
+++ b/Análisis/Diagrama de Gantt.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D75649-A6EE-458B-808B-2CCF86D5997A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D32B5B-7B2A-467D-AA18-D67DE2ADF7C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
   <si>
     <t>Cree una programación para un proyecto en esta hoja de cálculo.
 Escriba el título de este proyecto en la celda B1. 
@@ -117,10 +117,6 @@
   </si>
   <si>
     <t>Semana para mostrar:</t>
-  </si>
-  <si>
-    <t>ASIGNADO
-A</t>
   </si>
   <si>
     <t>INICIO</t>
@@ -262,6 +258,12 @@
   <si>
     <t>Equipo de desarrollo ADILD</t>
   </si>
+  <si>
+    <t>Realizado</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
 </sst>
 </file>
 
@@ -278,7 +280,7 @@
     <numFmt numFmtId="171" formatCode="d"/>
     <numFmt numFmtId="172" formatCode="ddd\,\ d/m/yyyy"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -517,6 +519,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Wingdings 2"/>
+      <family val="1"/>
+      <charset val="2"/>
     </font>
   </fonts>
   <fills count="49">
@@ -1090,7 +1099,7 @@
     <xf numFmtId="0" fontId="7" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1181,22 +1190,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="7">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="11" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="11" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="11" applyFill="1">
@@ -1415,6 +1412,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="172" fontId="7" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="9" borderId="2" xfId="11" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5357,8 +5369,8 @@
   <dimension ref="A1:DW42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="29.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5412,7 +5424,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -5426,7 +5438,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I2" s="29"/>
     </row>
@@ -5435,680 +5447,680 @@
         <v>2</v>
       </c>
       <c r="B3" s="33"/>
-      <c r="C3" s="110" t="s">
+      <c r="C3" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="111"/>
-      <c r="E3" s="113">
+      <c r="D3" s="107"/>
+      <c r="E3" s="109">
         <v>43892</v>
       </c>
-      <c r="F3" s="113"/>
+      <c r="F3" s="109"/>
     </row>
     <row r="4" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="110" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="111"/>
+      <c r="D4" s="107"/>
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="107">
+      <c r="I4" s="103">
         <f>I5</f>
         <v>43892</v>
       </c>
-      <c r="J4" s="108"/>
-      <c r="K4" s="108"/>
-      <c r="L4" s="108"/>
-      <c r="M4" s="108"/>
-      <c r="N4" s="108"/>
-      <c r="O4" s="109"/>
-      <c r="P4" s="107">
+      <c r="J4" s="104"/>
+      <c r="K4" s="104"/>
+      <c r="L4" s="104"/>
+      <c r="M4" s="104"/>
+      <c r="N4" s="104"/>
+      <c r="O4" s="105"/>
+      <c r="P4" s="103">
         <f>P5</f>
         <v>43899</v>
       </c>
-      <c r="Q4" s="108"/>
-      <c r="R4" s="108"/>
-      <c r="S4" s="108"/>
-      <c r="T4" s="108"/>
-      <c r="U4" s="108"/>
-      <c r="V4" s="109"/>
-      <c r="W4" s="107">
+      <c r="Q4" s="104"/>
+      <c r="R4" s="104"/>
+      <c r="S4" s="104"/>
+      <c r="T4" s="104"/>
+      <c r="U4" s="104"/>
+      <c r="V4" s="105"/>
+      <c r="W4" s="103">
         <f>W5</f>
         <v>43906</v>
       </c>
-      <c r="X4" s="108"/>
-      <c r="Y4" s="108"/>
-      <c r="Z4" s="108"/>
-      <c r="AA4" s="108"/>
-      <c r="AB4" s="108"/>
-      <c r="AC4" s="109"/>
-      <c r="AD4" s="107">
+      <c r="X4" s="104"/>
+      <c r="Y4" s="104"/>
+      <c r="Z4" s="104"/>
+      <c r="AA4" s="104"/>
+      <c r="AB4" s="104"/>
+      <c r="AC4" s="105"/>
+      <c r="AD4" s="103">
         <f>AD5</f>
         <v>43913</v>
       </c>
-      <c r="AE4" s="108"/>
-      <c r="AF4" s="108"/>
-      <c r="AG4" s="108"/>
-      <c r="AH4" s="108"/>
-      <c r="AI4" s="108"/>
-      <c r="AJ4" s="109"/>
-      <c r="AK4" s="107">
+      <c r="AE4" s="104"/>
+      <c r="AF4" s="104"/>
+      <c r="AG4" s="104"/>
+      <c r="AH4" s="104"/>
+      <c r="AI4" s="104"/>
+      <c r="AJ4" s="105"/>
+      <c r="AK4" s="103">
         <f>AK5</f>
         <v>43920</v>
       </c>
-      <c r="AL4" s="108"/>
-      <c r="AM4" s="108"/>
-      <c r="AN4" s="108"/>
-      <c r="AO4" s="108"/>
-      <c r="AP4" s="108"/>
-      <c r="AQ4" s="109"/>
-      <c r="AR4" s="107">
+      <c r="AL4" s="104"/>
+      <c r="AM4" s="104"/>
+      <c r="AN4" s="104"/>
+      <c r="AO4" s="104"/>
+      <c r="AP4" s="104"/>
+      <c r="AQ4" s="105"/>
+      <c r="AR4" s="103">
         <f>AR5</f>
         <v>43927</v>
       </c>
-      <c r="AS4" s="108"/>
-      <c r="AT4" s="108"/>
-      <c r="AU4" s="108"/>
-      <c r="AV4" s="108"/>
-      <c r="AW4" s="108"/>
-      <c r="AX4" s="109"/>
-      <c r="AY4" s="107">
+      <c r="AS4" s="104"/>
+      <c r="AT4" s="104"/>
+      <c r="AU4" s="104"/>
+      <c r="AV4" s="104"/>
+      <c r="AW4" s="104"/>
+      <c r="AX4" s="105"/>
+      <c r="AY4" s="103">
         <f>AY5</f>
         <v>43934</v>
       </c>
-      <c r="AZ4" s="108"/>
-      <c r="BA4" s="108"/>
-      <c r="BB4" s="108"/>
-      <c r="BC4" s="108"/>
-      <c r="BD4" s="108"/>
-      <c r="BE4" s="109"/>
-      <c r="BF4" s="107">
+      <c r="AZ4" s="104"/>
+      <c r="BA4" s="104"/>
+      <c r="BB4" s="104"/>
+      <c r="BC4" s="104"/>
+      <c r="BD4" s="104"/>
+      <c r="BE4" s="105"/>
+      <c r="BF4" s="103">
         <f>BF5</f>
         <v>43941</v>
       </c>
-      <c r="BG4" s="108"/>
-      <c r="BH4" s="108"/>
-      <c r="BI4" s="108"/>
-      <c r="BJ4" s="108"/>
-      <c r="BK4" s="108"/>
-      <c r="BL4" s="109"/>
-      <c r="BM4" s="107">
+      <c r="BG4" s="104"/>
+      <c r="BH4" s="104"/>
+      <c r="BI4" s="104"/>
+      <c r="BJ4" s="104"/>
+      <c r="BK4" s="104"/>
+      <c r="BL4" s="105"/>
+      <c r="BM4" s="103">
         <f>BM5</f>
         <v>43948</v>
       </c>
-      <c r="BN4" s="108"/>
-      <c r="BO4" s="108"/>
-      <c r="BP4" s="108"/>
-      <c r="BQ4" s="108"/>
-      <c r="BR4" s="108"/>
-      <c r="BS4" s="109"/>
-      <c r="BT4" s="107">
+      <c r="BN4" s="104"/>
+      <c r="BO4" s="104"/>
+      <c r="BP4" s="104"/>
+      <c r="BQ4" s="104"/>
+      <c r="BR4" s="104"/>
+      <c r="BS4" s="105"/>
+      <c r="BT4" s="103">
         <f>BT5</f>
         <v>43955</v>
       </c>
-      <c r="BU4" s="108"/>
-      <c r="BV4" s="108"/>
-      <c r="BW4" s="108"/>
-      <c r="BX4" s="108"/>
-      <c r="BY4" s="108"/>
-      <c r="BZ4" s="109"/>
-      <c r="CA4" s="107">
+      <c r="BU4" s="104"/>
+      <c r="BV4" s="104"/>
+      <c r="BW4" s="104"/>
+      <c r="BX4" s="104"/>
+      <c r="BY4" s="104"/>
+      <c r="BZ4" s="105"/>
+      <c r="CA4" s="103">
         <f>CA5</f>
         <v>43962</v>
       </c>
-      <c r="CB4" s="108"/>
-      <c r="CC4" s="108"/>
-      <c r="CD4" s="108"/>
-      <c r="CE4" s="108"/>
-      <c r="CF4" s="108"/>
-      <c r="CG4" s="109"/>
-      <c r="CH4" s="107">
+      <c r="CB4" s="104"/>
+      <c r="CC4" s="104"/>
+      <c r="CD4" s="104"/>
+      <c r="CE4" s="104"/>
+      <c r="CF4" s="104"/>
+      <c r="CG4" s="105"/>
+      <c r="CH4" s="103">
         <f>CH5</f>
         <v>43969</v>
       </c>
-      <c r="CI4" s="108"/>
-      <c r="CJ4" s="108"/>
-      <c r="CK4" s="108"/>
-      <c r="CL4" s="108"/>
-      <c r="CM4" s="108"/>
-      <c r="CN4" s="109"/>
-      <c r="CO4" s="107">
+      <c r="CI4" s="104"/>
+      <c r="CJ4" s="104"/>
+      <c r="CK4" s="104"/>
+      <c r="CL4" s="104"/>
+      <c r="CM4" s="104"/>
+      <c r="CN4" s="105"/>
+      <c r="CO4" s="103">
         <f>CO5</f>
         <v>43976</v>
       </c>
-      <c r="CP4" s="108"/>
-      <c r="CQ4" s="108"/>
-      <c r="CR4" s="108"/>
-      <c r="CS4" s="108"/>
-      <c r="CT4" s="108"/>
-      <c r="CU4" s="109"/>
-      <c r="CV4" s="107">
+      <c r="CP4" s="104"/>
+      <c r="CQ4" s="104"/>
+      <c r="CR4" s="104"/>
+      <c r="CS4" s="104"/>
+      <c r="CT4" s="104"/>
+      <c r="CU4" s="105"/>
+      <c r="CV4" s="103">
         <f>CV5</f>
         <v>43983</v>
       </c>
-      <c r="CW4" s="108"/>
-      <c r="CX4" s="108"/>
-      <c r="CY4" s="108"/>
-      <c r="CZ4" s="108"/>
-      <c r="DA4" s="108"/>
-      <c r="DB4" s="109"/>
-      <c r="DC4" s="107">
+      <c r="CW4" s="104"/>
+      <c r="CX4" s="104"/>
+      <c r="CY4" s="104"/>
+      <c r="CZ4" s="104"/>
+      <c r="DA4" s="104"/>
+      <c r="DB4" s="105"/>
+      <c r="DC4" s="103">
         <f>DC5</f>
         <v>43990</v>
       </c>
-      <c r="DD4" s="108"/>
-      <c r="DE4" s="108"/>
-      <c r="DF4" s="108"/>
-      <c r="DG4" s="108"/>
-      <c r="DH4" s="108"/>
-      <c r="DI4" s="109"/>
-      <c r="DJ4" s="107">
+      <c r="DD4" s="104"/>
+      <c r="DE4" s="104"/>
+      <c r="DF4" s="104"/>
+      <c r="DG4" s="104"/>
+      <c r="DH4" s="104"/>
+      <c r="DI4" s="105"/>
+      <c r="DJ4" s="103">
         <f>DJ5</f>
         <v>43997</v>
       </c>
-      <c r="DK4" s="108"/>
-      <c r="DL4" s="108"/>
-      <c r="DM4" s="108"/>
-      <c r="DN4" s="108"/>
-      <c r="DO4" s="108"/>
-      <c r="DP4" s="109"/>
-      <c r="DQ4" s="107">
+      <c r="DK4" s="104"/>
+      <c r="DL4" s="104"/>
+      <c r="DM4" s="104"/>
+      <c r="DN4" s="104"/>
+      <c r="DO4" s="104"/>
+      <c r="DP4" s="105"/>
+      <c r="DQ4" s="103">
         <f>DQ5</f>
         <v>44004</v>
       </c>
-      <c r="DR4" s="108"/>
-      <c r="DS4" s="108"/>
-      <c r="DT4" s="108"/>
-      <c r="DU4" s="108"/>
-      <c r="DV4" s="108"/>
-      <c r="DW4" s="109"/>
+      <c r="DR4" s="104"/>
+      <c r="DS4" s="104"/>
+      <c r="DT4" s="104"/>
+      <c r="DU4" s="104"/>
+      <c r="DV4" s="104"/>
+      <c r="DW4" s="105"/>
     </row>
     <row r="5" spans="1:127" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="112"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
-      <c r="I5" s="48">
+      <c r="B5" s="108"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="108"/>
+      <c r="I5" s="44">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43892</v>
       </c>
-      <c r="J5" s="49">
+      <c r="J5" s="45">
         <f>I5+1</f>
         <v>43893</v>
       </c>
-      <c r="K5" s="49">
+      <c r="K5" s="45">
         <f t="shared" ref="K5:AX5" si="0">J5+1</f>
         <v>43894</v>
       </c>
-      <c r="L5" s="49">
+      <c r="L5" s="45">
         <f t="shared" si="0"/>
         <v>43895</v>
       </c>
-      <c r="M5" s="49">
+      <c r="M5" s="45">
         <f t="shared" si="0"/>
         <v>43896</v>
       </c>
-      <c r="N5" s="49">
+      <c r="N5" s="45">
         <f t="shared" si="0"/>
         <v>43897</v>
       </c>
-      <c r="O5" s="50">
+      <c r="O5" s="46">
         <f t="shared" si="0"/>
         <v>43898</v>
       </c>
-      <c r="P5" s="48">
+      <c r="P5" s="44">
         <f>O5+1</f>
         <v>43899</v>
       </c>
-      <c r="Q5" s="49">
+      <c r="Q5" s="45">
         <f>P5+1</f>
         <v>43900</v>
       </c>
-      <c r="R5" s="49">
+      <c r="R5" s="45">
         <f t="shared" si="0"/>
         <v>43901</v>
       </c>
-      <c r="S5" s="49">
+      <c r="S5" s="45">
         <f t="shared" si="0"/>
         <v>43902</v>
       </c>
-      <c r="T5" s="49">
+      <c r="T5" s="45">
         <f t="shared" si="0"/>
         <v>43903</v>
       </c>
-      <c r="U5" s="49">
+      <c r="U5" s="45">
         <f t="shared" si="0"/>
         <v>43904</v>
       </c>
-      <c r="V5" s="50">
+      <c r="V5" s="46">
         <f t="shared" si="0"/>
         <v>43905</v>
       </c>
-      <c r="W5" s="48">
+      <c r="W5" s="44">
         <f>V5+1</f>
         <v>43906</v>
       </c>
-      <c r="X5" s="49">
+      <c r="X5" s="45">
         <f>W5+1</f>
         <v>43907</v>
       </c>
-      <c r="Y5" s="49">
+      <c r="Y5" s="45">
         <f t="shared" si="0"/>
         <v>43908</v>
       </c>
-      <c r="Z5" s="49">
+      <c r="Z5" s="45">
         <f t="shared" si="0"/>
         <v>43909</v>
       </c>
-      <c r="AA5" s="49">
+      <c r="AA5" s="45">
         <f t="shared" si="0"/>
         <v>43910</v>
       </c>
-      <c r="AB5" s="49">
+      <c r="AB5" s="45">
         <f t="shared" si="0"/>
         <v>43911</v>
       </c>
-      <c r="AC5" s="50">
+      <c r="AC5" s="46">
         <f t="shared" si="0"/>
         <v>43912</v>
       </c>
-      <c r="AD5" s="48">
+      <c r="AD5" s="44">
         <f>AC5+1</f>
         <v>43913</v>
       </c>
-      <c r="AE5" s="49">
+      <c r="AE5" s="45">
         <f>AD5+1</f>
         <v>43914</v>
       </c>
-      <c r="AF5" s="49">
+      <c r="AF5" s="45">
         <f t="shared" si="0"/>
         <v>43915</v>
       </c>
-      <c r="AG5" s="49">
+      <c r="AG5" s="45">
         <f t="shared" si="0"/>
         <v>43916</v>
       </c>
-      <c r="AH5" s="49">
+      <c r="AH5" s="45">
         <f t="shared" si="0"/>
         <v>43917</v>
       </c>
-      <c r="AI5" s="49">
+      <c r="AI5" s="45">
         <f t="shared" si="0"/>
         <v>43918</v>
       </c>
-      <c r="AJ5" s="50">
+      <c r="AJ5" s="46">
         <f t="shared" si="0"/>
         <v>43919</v>
       </c>
-      <c r="AK5" s="48">
+      <c r="AK5" s="44">
         <f>AJ5+1</f>
         <v>43920</v>
       </c>
-      <c r="AL5" s="49">
+      <c r="AL5" s="45">
         <f>AK5+1</f>
         <v>43921</v>
       </c>
-      <c r="AM5" s="49">
+      <c r="AM5" s="45">
         <f t="shared" si="0"/>
         <v>43922</v>
       </c>
-      <c r="AN5" s="49">
+      <c r="AN5" s="45">
         <f t="shared" si="0"/>
         <v>43923</v>
       </c>
-      <c r="AO5" s="49">
+      <c r="AO5" s="45">
         <f t="shared" si="0"/>
         <v>43924</v>
       </c>
-      <c r="AP5" s="49">
+      <c r="AP5" s="45">
         <f t="shared" si="0"/>
         <v>43925</v>
       </c>
-      <c r="AQ5" s="50">
+      <c r="AQ5" s="46">
         <f t="shared" si="0"/>
         <v>43926</v>
       </c>
-      <c r="AR5" s="48">
+      <c r="AR5" s="44">
         <f>AQ5+1</f>
         <v>43927</v>
       </c>
-      <c r="AS5" s="49">
+      <c r="AS5" s="45">
         <f>AR5+1</f>
         <v>43928</v>
       </c>
-      <c r="AT5" s="49">
+      <c r="AT5" s="45">
         <f t="shared" si="0"/>
         <v>43929</v>
       </c>
-      <c r="AU5" s="49">
+      <c r="AU5" s="45">
         <f t="shared" si="0"/>
         <v>43930</v>
       </c>
-      <c r="AV5" s="49">
+      <c r="AV5" s="45">
         <f t="shared" si="0"/>
         <v>43931</v>
       </c>
-      <c r="AW5" s="49">
+      <c r="AW5" s="45">
         <f t="shared" si="0"/>
         <v>43932</v>
       </c>
-      <c r="AX5" s="50">
+      <c r="AX5" s="46">
         <f t="shared" si="0"/>
         <v>43933</v>
       </c>
-      <c r="AY5" s="48">
+      <c r="AY5" s="44">
         <f>AX5+1</f>
         <v>43934</v>
       </c>
-      <c r="AZ5" s="49">
+      <c r="AZ5" s="45">
         <f>AY5+1</f>
         <v>43935</v>
       </c>
-      <c r="BA5" s="49">
+      <c r="BA5" s="45">
         <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
         <v>43936</v>
       </c>
-      <c r="BB5" s="49">
+      <c r="BB5" s="45">
         <f t="shared" si="1"/>
         <v>43937</v>
       </c>
-      <c r="BC5" s="49">
+      <c r="BC5" s="45">
         <f t="shared" si="1"/>
         <v>43938</v>
       </c>
-      <c r="BD5" s="49">
+      <c r="BD5" s="45">
         <f t="shared" si="1"/>
         <v>43939</v>
       </c>
-      <c r="BE5" s="50">
+      <c r="BE5" s="46">
         <f t="shared" si="1"/>
         <v>43940</v>
       </c>
-      <c r="BF5" s="48">
+      <c r="BF5" s="44">
         <f>BE5+1</f>
         <v>43941</v>
       </c>
-      <c r="BG5" s="49">
+      <c r="BG5" s="45">
         <f>BF5+1</f>
         <v>43942</v>
       </c>
-      <c r="BH5" s="49">
+      <c r="BH5" s="45">
         <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
         <v>43943</v>
       </c>
-      <c r="BI5" s="49">
+      <c r="BI5" s="45">
         <f t="shared" si="2"/>
         <v>43944</v>
       </c>
-      <c r="BJ5" s="49">
+      <c r="BJ5" s="45">
         <f t="shared" si="2"/>
         <v>43945</v>
       </c>
-      <c r="BK5" s="49">
+      <c r="BK5" s="45">
         <f t="shared" si="2"/>
         <v>43946</v>
       </c>
-      <c r="BL5" s="50">
+      <c r="BL5" s="46">
         <f t="shared" si="2"/>
         <v>43947</v>
       </c>
-      <c r="BM5" s="48">
+      <c r="BM5" s="44">
         <f>BL5+1</f>
         <v>43948</v>
       </c>
-      <c r="BN5" s="49">
+      <c r="BN5" s="45">
         <f>BM5+1</f>
         <v>43949</v>
       </c>
-      <c r="BO5" s="49">
+      <c r="BO5" s="45">
         <f t="shared" ref="BO5" si="3">BN5+1</f>
         <v>43950</v>
       </c>
-      <c r="BP5" s="49">
+      <c r="BP5" s="45">
         <f t="shared" ref="BP5" si="4">BO5+1</f>
         <v>43951</v>
       </c>
-      <c r="BQ5" s="49">
+      <c r="BQ5" s="45">
         <f t="shared" ref="BQ5" si="5">BP5+1</f>
         <v>43952</v>
       </c>
-      <c r="BR5" s="49">
+      <c r="BR5" s="45">
         <f t="shared" ref="BR5" si="6">BQ5+1</f>
         <v>43953</v>
       </c>
-      <c r="BS5" s="50">
+      <c r="BS5" s="46">
         <f t="shared" ref="BS5" si="7">BR5+1</f>
         <v>43954</v>
       </c>
-      <c r="BT5" s="48">
+      <c r="BT5" s="44">
         <f>BS5+1</f>
         <v>43955</v>
       </c>
-      <c r="BU5" s="49">
+      <c r="BU5" s="45">
         <f>BT5+1</f>
         <v>43956</v>
       </c>
-      <c r="BV5" s="49">
+      <c r="BV5" s="45">
         <f t="shared" ref="BV5" si="8">BU5+1</f>
         <v>43957</v>
       </c>
-      <c r="BW5" s="49">
+      <c r="BW5" s="45">
         <f t="shared" ref="BW5" si="9">BV5+1</f>
         <v>43958</v>
       </c>
-      <c r="BX5" s="49">
+      <c r="BX5" s="45">
         <f t="shared" ref="BX5" si="10">BW5+1</f>
         <v>43959</v>
       </c>
-      <c r="BY5" s="49">
+      <c r="BY5" s="45">
         <f t="shared" ref="BY5" si="11">BX5+1</f>
         <v>43960</v>
       </c>
-      <c r="BZ5" s="50">
+      <c r="BZ5" s="46">
         <f t="shared" ref="BZ5" si="12">BY5+1</f>
         <v>43961</v>
       </c>
-      <c r="CA5" s="48">
+      <c r="CA5" s="44">
         <f>BZ5+1</f>
         <v>43962</v>
       </c>
-      <c r="CB5" s="49">
+      <c r="CB5" s="45">
         <f>CA5+1</f>
         <v>43963</v>
       </c>
-      <c r="CC5" s="49">
+      <c r="CC5" s="45">
         <f t="shared" ref="CC5" si="13">CB5+1</f>
         <v>43964</v>
       </c>
-      <c r="CD5" s="49">
+      <c r="CD5" s="45">
         <f t="shared" ref="CD5" si="14">CC5+1</f>
         <v>43965</v>
       </c>
-      <c r="CE5" s="49">
+      <c r="CE5" s="45">
         <f t="shared" ref="CE5" si="15">CD5+1</f>
         <v>43966</v>
       </c>
-      <c r="CF5" s="49">
+      <c r="CF5" s="45">
         <f t="shared" ref="CF5" si="16">CE5+1</f>
         <v>43967</v>
       </c>
-      <c r="CG5" s="50">
+      <c r="CG5" s="46">
         <f t="shared" ref="CG5" si="17">CF5+1</f>
         <v>43968</v>
       </c>
-      <c r="CH5" s="48">
+      <c r="CH5" s="44">
         <f>CG5+1</f>
         <v>43969</v>
       </c>
-      <c r="CI5" s="49">
+      <c r="CI5" s="45">
         <f>CH5+1</f>
         <v>43970</v>
       </c>
-      <c r="CJ5" s="49">
+      <c r="CJ5" s="45">
         <f t="shared" ref="CJ5" si="18">CI5+1</f>
         <v>43971</v>
       </c>
-      <c r="CK5" s="49">
+      <c r="CK5" s="45">
         <f t="shared" ref="CK5" si="19">CJ5+1</f>
         <v>43972</v>
       </c>
-      <c r="CL5" s="49">
+      <c r="CL5" s="45">
         <f t="shared" ref="CL5" si="20">CK5+1</f>
         <v>43973</v>
       </c>
-      <c r="CM5" s="49">
+      <c r="CM5" s="45">
         <f t="shared" ref="CM5" si="21">CL5+1</f>
         <v>43974</v>
       </c>
-      <c r="CN5" s="50">
+      <c r="CN5" s="46">
         <f t="shared" ref="CN5" si="22">CM5+1</f>
         <v>43975</v>
       </c>
-      <c r="CO5" s="48">
+      <c r="CO5" s="44">
         <f>CN5+1</f>
         <v>43976</v>
       </c>
-      <c r="CP5" s="49">
+      <c r="CP5" s="45">
         <f>CO5+1</f>
         <v>43977</v>
       </c>
-      <c r="CQ5" s="49">
+      <c r="CQ5" s="45">
         <f t="shared" ref="CQ5" si="23">CP5+1</f>
         <v>43978</v>
       </c>
-      <c r="CR5" s="49">
+      <c r="CR5" s="45">
         <f t="shared" ref="CR5" si="24">CQ5+1</f>
         <v>43979</v>
       </c>
-      <c r="CS5" s="49">
+      <c r="CS5" s="45">
         <f t="shared" ref="CS5" si="25">CR5+1</f>
         <v>43980</v>
       </c>
-      <c r="CT5" s="49">
+      <c r="CT5" s="45">
         <f t="shared" ref="CT5" si="26">CS5+1</f>
         <v>43981</v>
       </c>
-      <c r="CU5" s="50">
+      <c r="CU5" s="46">
         <f t="shared" ref="CU5" si="27">CT5+1</f>
         <v>43982</v>
       </c>
-      <c r="CV5" s="48">
+      <c r="CV5" s="44">
         <f>CU5+1</f>
         <v>43983</v>
       </c>
-      <c r="CW5" s="49">
+      <c r="CW5" s="45">
         <f>CV5+1</f>
         <v>43984</v>
       </c>
-      <c r="CX5" s="49">
+      <c r="CX5" s="45">
         <f t="shared" ref="CX5" si="28">CW5+1</f>
         <v>43985</v>
       </c>
-      <c r="CY5" s="49">
+      <c r="CY5" s="45">
         <f t="shared" ref="CY5" si="29">CX5+1</f>
         <v>43986</v>
       </c>
-      <c r="CZ5" s="49">
+      <c r="CZ5" s="45">
         <f t="shared" ref="CZ5" si="30">CY5+1</f>
         <v>43987</v>
       </c>
-      <c r="DA5" s="49">
+      <c r="DA5" s="45">
         <f t="shared" ref="DA5" si="31">CZ5+1</f>
         <v>43988</v>
       </c>
-      <c r="DB5" s="50">
+      <c r="DB5" s="46">
         <f t="shared" ref="DB5" si="32">DA5+1</f>
         <v>43989</v>
       </c>
-      <c r="DC5" s="48">
+      <c r="DC5" s="44">
         <f>DB5+1</f>
         <v>43990</v>
       </c>
-      <c r="DD5" s="49">
+      <c r="DD5" s="45">
         <f>DC5+1</f>
         <v>43991</v>
       </c>
-      <c r="DE5" s="49">
+      <c r="DE5" s="45">
         <f t="shared" ref="DE5" si="33">DD5+1</f>
         <v>43992</v>
       </c>
-      <c r="DF5" s="49">
+      <c r="DF5" s="45">
         <f t="shared" ref="DF5" si="34">DE5+1</f>
         <v>43993</v>
       </c>
-      <c r="DG5" s="49">
+      <c r="DG5" s="45">
         <f t="shared" ref="DG5" si="35">DF5+1</f>
         <v>43994</v>
       </c>
-      <c r="DH5" s="49">
+      <c r="DH5" s="45">
         <f t="shared" ref="DH5" si="36">DG5+1</f>
         <v>43995</v>
       </c>
-      <c r="DI5" s="50">
+      <c r="DI5" s="46">
         <f t="shared" ref="DI5" si="37">DH5+1</f>
         <v>43996</v>
       </c>
-      <c r="DJ5" s="48">
+      <c r="DJ5" s="44">
         <f>DI5+1</f>
         <v>43997</v>
       </c>
-      <c r="DK5" s="49">
+      <c r="DK5" s="45">
         <f>DJ5+1</f>
         <v>43998</v>
       </c>
-      <c r="DL5" s="49">
+      <c r="DL5" s="45">
         <f t="shared" ref="DL5" si="38">DK5+1</f>
         <v>43999</v>
       </c>
-      <c r="DM5" s="49">
+      <c r="DM5" s="45">
         <f t="shared" ref="DM5" si="39">DL5+1</f>
         <v>44000</v>
       </c>
-      <c r="DN5" s="49">
+      <c r="DN5" s="45">
         <f t="shared" ref="DN5" si="40">DM5+1</f>
         <v>44001</v>
       </c>
-      <c r="DO5" s="49">
+      <c r="DO5" s="45">
         <f t="shared" ref="DO5" si="41">DN5+1</f>
         <v>44002</v>
       </c>
-      <c r="DP5" s="50">
+      <c r="DP5" s="46">
         <f t="shared" ref="DP5" si="42">DO5+1</f>
         <v>44003</v>
       </c>
-      <c r="DQ5" s="48">
+      <c r="DQ5" s="44">
         <f>DP5+1</f>
         <v>44004</v>
       </c>
-      <c r="DR5" s="49">
+      <c r="DR5" s="45">
         <f>DQ5+1</f>
         <v>44005</v>
       </c>
-      <c r="DS5" s="49">
+      <c r="DS5" s="45">
         <f t="shared" ref="DS5" si="43">DR5+1</f>
         <v>44006</v>
       </c>
-      <c r="DT5" s="49">
+      <c r="DT5" s="45">
         <f t="shared" ref="DT5" si="44">DS5+1</f>
         <v>44007</v>
       </c>
-      <c r="DU5" s="49">
+      <c r="DU5" s="45">
         <f t="shared" ref="DU5" si="45">DT5+1</f>
         <v>44008</v>
       </c>
-      <c r="DV5" s="49">
+      <c r="DV5" s="45">
         <f t="shared" ref="DV5" si="46">DU5+1</f>
         <v>44009</v>
       </c>
-      <c r="DW5" s="50">
+      <c r="DW5" s="46">
         <f t="shared" ref="DW5" si="47">DV5+1</f>
         <v>44010</v>
       </c>
@@ -6121,18 +6133,18 @@
         <v>13</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>18</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I6" s="9" t="str">
         <f t="shared" ref="I6" si="48">LEFT(TEXT(I5,"ddd"),1)</f>
@@ -6746,12 +6758,12 @@
         <v>6</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60"/>
+        <v>36</v>
+      </c>
+      <c r="C8" s="110"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="56"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11" t="str">
         <f t="shared" ref="H8:H34" si="53">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
@@ -6881,16 +6893,18 @@
       <c r="A9" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="61">
+      <c r="B9" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="111" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="48"/>
+      <c r="E9" s="57">
         <f>Project_Start</f>
         <v>43892</v>
       </c>
-      <c r="F9" s="61">
+      <c r="F9" s="57">
         <f>E9+7</f>
         <v>43899</v>
       </c>
@@ -7024,12 +7038,12 @@
         <v>8</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="63"/>
+        <v>38</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="59"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11" t="str">
         <f t="shared" si="53"/>
@@ -7157,16 +7171,18 @@
     </row>
     <row r="11" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="27"/>
-      <c r="B11" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="64">
+      <c r="B11" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="112" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="50"/>
+      <c r="E11" s="60">
         <f>F9</f>
         <v>43899</v>
       </c>
-      <c r="F11" s="64">
+      <c r="F11" s="60">
         <f>E11+4</f>
         <v>43903</v>
       </c>
@@ -7297,15 +7313,17 @@
     </row>
     <row r="12" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="27"/>
-      <c r="B12" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="64">
+      <c r="B12" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="112" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="50"/>
+      <c r="E12" s="60">
         <v>43899</v>
       </c>
-      <c r="F12" s="64">
+      <c r="F12" s="60">
         <v>43899</v>
       </c>
       <c r="G12" s="11"/>
@@ -7436,12 +7454,12 @@
     <row r="13" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="27"/>
       <c r="B13" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="66"/>
+        <v>39</v>
+      </c>
+      <c r="C13" s="35"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="62"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11" t="str">
         <f t="shared" si="53"/>
@@ -7571,15 +7589,17 @@
       <c r="A14" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="67">
+      <c r="B14" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="113" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="52"/>
+      <c r="E14" s="63">
         <v>43913</v>
       </c>
-      <c r="F14" s="67">
+      <c r="F14" s="63">
         <v>43918</v>
       </c>
       <c r="G14" s="11"/>
@@ -7709,15 +7729,17 @@
     </row>
     <row r="15" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="28"/>
-      <c r="B15" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="67">
+      <c r="B15" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="113" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="52"/>
+      <c r="E15" s="63">
         <v>43913</v>
       </c>
-      <c r="F15" s="67">
+      <c r="F15" s="63">
         <v>43918</v>
       </c>
       <c r="G15" s="11"/>
@@ -7847,15 +7869,17 @@
     </row>
     <row r="16" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="27"/>
-      <c r="B16" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="67">
+      <c r="B16" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="113" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="52"/>
+      <c r="E16" s="63">
         <v>43913</v>
       </c>
-      <c r="F16" s="67">
+      <c r="F16" s="63">
         <v>43918</v>
       </c>
       <c r="G16" s="11"/>
@@ -7985,15 +8009,17 @@
     </row>
     <row r="17" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="27"/>
-      <c r="B17" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="67">
+      <c r="B17" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="113" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="52"/>
+      <c r="E17" s="63">
         <v>43919</v>
       </c>
-      <c r="F17" s="67">
+      <c r="F17" s="63">
         <v>43922</v>
       </c>
       <c r="G17" s="11"/>
@@ -8123,15 +8149,17 @@
     </row>
     <row r="18" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="27"/>
-      <c r="B18" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="67">
+      <c r="B18" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="113" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="52"/>
+      <c r="E18" s="63">
         <v>43919</v>
       </c>
-      <c r="F18" s="67">
+      <c r="F18" s="63">
         <v>43922</v>
       </c>
       <c r="G18" s="11"/>
@@ -8262,12 +8290,12 @@
     <row r="19" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="27"/>
       <c r="B19" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="69"/>
+        <v>40</v>
+      </c>
+      <c r="C19" s="36"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="65"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11" t="str">
         <f t="shared" si="53"/>
@@ -8397,15 +8425,17 @@
       <c r="A20" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="70">
+      <c r="B20" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="114" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="54"/>
+      <c r="E20" s="66">
         <v>43941</v>
       </c>
-      <c r="F20" s="70">
+      <c r="F20" s="66">
         <v>43942</v>
       </c>
       <c r="G20" s="11"/>
@@ -8535,15 +8565,17 @@
     </row>
     <row r="21" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="27"/>
-      <c r="B21" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="70">
+      <c r="B21" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="114" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="54"/>
+      <c r="E21" s="66">
         <v>43926</v>
       </c>
-      <c r="F21" s="70">
+      <c r="F21" s="66">
         <v>43933</v>
       </c>
       <c r="G21" s="11"/>
@@ -8673,15 +8705,15 @@
     </row>
     <row r="22" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="27"/>
-      <c r="B22" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="70">
+      <c r="B22" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="37"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="66">
         <v>43952</v>
       </c>
-      <c r="F22" s="70">
+      <c r="F22" s="66">
         <v>43968</v>
       </c>
       <c r="G22" s="11"/>
@@ -8811,15 +8843,17 @@
     </row>
     <row r="23" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="27"/>
-      <c r="B23" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="70">
+      <c r="B23" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="114" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="54"/>
+      <c r="E23" s="66">
         <v>43926</v>
       </c>
-      <c r="F23" s="70">
+      <c r="F23" s="66">
         <v>43931</v>
       </c>
       <c r="G23" s="11"/>
@@ -8949,16 +8983,16 @@
     </row>
     <row r="24" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="27"/>
-      <c r="B24" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="70">
+      <c r="B24" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="37"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="66">
         <f>E22</f>
         <v>43952</v>
       </c>
-      <c r="F24" s="70">
+      <c r="F24" s="66">
         <v>43969</v>
       </c>
       <c r="G24" s="11"/>
@@ -9088,16 +9122,16 @@
     </row>
     <row r="25" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="27"/>
-      <c r="B25" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="70">
+      <c r="B25" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="37"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="66">
         <f>E23</f>
         <v>43926</v>
       </c>
-      <c r="F25" s="70">
+      <c r="F25" s="66">
         <v>43969</v>
       </c>
       <c r="G25" s="11"/>
@@ -9229,15 +9263,15 @@
       <c r="A26" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="70">
+      <c r="B26" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="37"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="66">
         <v>43941</v>
       </c>
-      <c r="F26" s="70">
+      <c r="F26" s="66">
         <v>43971</v>
       </c>
       <c r="G26" s="11"/>
@@ -9367,13 +9401,13 @@
     </row>
     <row r="27" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="27"/>
-      <c r="B27" s="71" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="72"/>
-      <c r="D27" s="73"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="75"/>
+      <c r="B27" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="68"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="71"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11" t="str">
         <f t="shared" si="53"/>
@@ -9501,15 +9535,15 @@
     </row>
     <row r="28" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="27"/>
-      <c r="B28" s="76" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="77"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="79">
+      <c r="B28" s="72" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="73"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="75">
         <v>43972</v>
       </c>
-      <c r="F28" s="79">
+      <c r="F28" s="75">
         <f>E28+5</f>
         <v>43977</v>
       </c>
@@ -9640,15 +9674,15 @@
     </row>
     <row r="29" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="27"/>
-      <c r="B29" s="76" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="77"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="79">
+      <c r="B29" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="73"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="75">
         <v>43972</v>
       </c>
-      <c r="F29" s="79">
+      <c r="F29" s="75">
         <f>E29+5</f>
         <v>43977</v>
       </c>
@@ -9779,15 +9813,15 @@
     </row>
     <row r="30" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="27"/>
-      <c r="B30" s="76" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="77"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="79">
+      <c r="B30" s="72" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="73"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="75">
         <v>43972</v>
       </c>
-      <c r="F30" s="79">
+      <c r="F30" s="75">
         <f>E30+5</f>
         <v>43977</v>
       </c>
@@ -9918,16 +9952,16 @@
     </row>
     <row r="31" spans="1:127" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="27"/>
-      <c r="B31" s="76" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="77"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="79">
+      <c r="B31" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="73"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="75">
         <f>F30+1</f>
         <v>43978</v>
       </c>
-      <c r="F31" s="79">
+      <c r="F31" s="75">
         <f>E31+6</f>
         <v>43984</v>
       </c>
@@ -10060,16 +10094,16 @@
       <c r="A32" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="76" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" s="77"/>
-      <c r="D32" s="78"/>
-      <c r="E32" s="79">
+      <c r="B32" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="73"/>
+      <c r="D32" s="74"/>
+      <c r="E32" s="75">
         <f>F30+1</f>
         <v>43978</v>
       </c>
-      <c r="F32" s="79">
+      <c r="F32" s="75">
         <f>E32+6</f>
         <v>43984</v>
       </c>
@@ -10202,13 +10236,13 @@
       <c r="A33" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="80" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" s="81"/>
-      <c r="D33" s="82"/>
-      <c r="E33" s="83"/>
-      <c r="F33" s="84"/>
+      <c r="B33" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="77"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="79"/>
+      <c r="F33" s="80"/>
       <c r="G33" s="11"/>
       <c r="H33" s="11" t="str">
         <f t="shared" si="53"/>
@@ -10335,923 +10369,922 @@
       <c r="DW33" s="16"/>
     </row>
     <row r="34" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="85" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="86"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="88">
+      <c r="B34" s="81" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="82"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="84">
         <f>F32+F361</f>
         <v>43984</v>
       </c>
-      <c r="F34" s="88">
+      <c r="F34" s="84">
         <f>E34+1</f>
         <v>43985</v>
       </c>
-      <c r="G34" s="89"/>
-      <c r="H34" s="89">
+      <c r="G34" s="85"/>
+      <c r="H34" s="85">
         <f t="shared" si="53"/>
         <v>2</v>
       </c>
-      <c r="I34" s="90"/>
-      <c r="J34" s="90"/>
-      <c r="K34" s="90"/>
-      <c r="L34" s="90"/>
-      <c r="M34" s="90"/>
-      <c r="N34" s="90"/>
-      <c r="O34" s="90"/>
-      <c r="P34" s="90"/>
-      <c r="Q34" s="90"/>
-      <c r="R34" s="90"/>
-      <c r="S34" s="90"/>
-      <c r="T34" s="90"/>
-      <c r="U34" s="90"/>
-      <c r="V34" s="90"/>
-      <c r="W34" s="90"/>
-      <c r="X34" s="90"/>
-      <c r="Y34" s="90"/>
-      <c r="Z34" s="90"/>
-      <c r="AA34" s="90"/>
-      <c r="AB34" s="90"/>
-      <c r="AC34" s="90"/>
-      <c r="AD34" s="90"/>
-      <c r="AE34" s="90"/>
-      <c r="AF34" s="90"/>
-      <c r="AG34" s="90"/>
-      <c r="AH34" s="90"/>
-      <c r="AI34" s="90"/>
-      <c r="AJ34" s="90"/>
-      <c r="AK34" s="90"/>
-      <c r="AL34" s="90"/>
-      <c r="AM34" s="90"/>
-      <c r="AN34" s="90"/>
-      <c r="AO34" s="90"/>
-      <c r="AP34" s="90"/>
-      <c r="AQ34" s="90"/>
-      <c r="AR34" s="90"/>
-      <c r="AS34" s="90"/>
-      <c r="AT34" s="90"/>
-      <c r="AU34" s="90"/>
-      <c r="AV34" s="90"/>
-      <c r="AW34" s="90"/>
-      <c r="AX34" s="90"/>
-      <c r="AY34" s="90"/>
-      <c r="AZ34" s="90"/>
-      <c r="BA34" s="90"/>
-      <c r="BB34" s="90"/>
-      <c r="BC34" s="90"/>
-      <c r="BD34" s="90"/>
-      <c r="BE34" s="90"/>
-      <c r="BF34" s="90"/>
-      <c r="BG34" s="90"/>
-      <c r="BH34" s="90"/>
-      <c r="BI34" s="90"/>
-      <c r="BJ34" s="90"/>
-      <c r="BK34" s="90"/>
-      <c r="BL34" s="90"/>
-      <c r="BM34" s="90"/>
-      <c r="BN34" s="90"/>
-      <c r="BO34" s="90"/>
-      <c r="BP34" s="90"/>
-      <c r="BQ34" s="90"/>
-      <c r="BR34" s="90"/>
-      <c r="BS34" s="90"/>
-      <c r="BT34" s="90"/>
-      <c r="BU34" s="90"/>
-      <c r="BV34" s="90"/>
-      <c r="BW34" s="90"/>
-      <c r="BX34" s="90"/>
-      <c r="BY34" s="90"/>
-      <c r="BZ34" s="90"/>
-      <c r="CA34" s="90"/>
-      <c r="CB34" s="90"/>
-      <c r="CC34" s="90"/>
-      <c r="CD34" s="90"/>
-      <c r="CE34" s="90"/>
-      <c r="CF34" s="90"/>
-      <c r="CG34" s="90"/>
-      <c r="CH34" s="90"/>
-      <c r="CI34" s="90"/>
-      <c r="CJ34" s="90"/>
-      <c r="CK34" s="90"/>
-      <c r="CL34" s="90"/>
-      <c r="CM34" s="90"/>
-      <c r="CN34" s="90"/>
-      <c r="CO34" s="90"/>
-      <c r="CP34" s="90"/>
-      <c r="CQ34" s="90"/>
-      <c r="CR34" s="90"/>
-      <c r="CS34" s="90"/>
-      <c r="CT34" s="90"/>
-      <c r="CU34" s="90"/>
-      <c r="CV34" s="90"/>
-      <c r="CW34" s="90"/>
-      <c r="CX34" s="90"/>
-      <c r="CY34" s="90"/>
-      <c r="CZ34" s="90"/>
-      <c r="DA34" s="90"/>
-      <c r="DB34" s="90"/>
-      <c r="DC34" s="90"/>
-      <c r="DD34" s="90"/>
-      <c r="DE34" s="90"/>
-      <c r="DF34" s="90"/>
-      <c r="DG34" s="90"/>
-      <c r="DH34" s="90"/>
-      <c r="DI34" s="90"/>
-      <c r="DJ34" s="90"/>
-      <c r="DK34" s="90"/>
-      <c r="DL34" s="90"/>
-      <c r="DM34" s="90"/>
-      <c r="DN34" s="90"/>
-      <c r="DO34" s="90"/>
-      <c r="DP34" s="90"/>
-      <c r="DQ34" s="90"/>
-      <c r="DR34" s="90"/>
-      <c r="DS34" s="90"/>
-      <c r="DT34" s="90"/>
-      <c r="DU34" s="90"/>
-      <c r="DV34" s="90"/>
-      <c r="DW34" s="90"/>
+      <c r="I34" s="86"/>
+      <c r="J34" s="86"/>
+      <c r="K34" s="86"/>
+      <c r="L34" s="86"/>
+      <c r="M34" s="86"/>
+      <c r="N34" s="86"/>
+      <c r="O34" s="86"/>
+      <c r="P34" s="86"/>
+      <c r="Q34" s="86"/>
+      <c r="R34" s="86"/>
+      <c r="S34" s="86"/>
+      <c r="T34" s="86"/>
+      <c r="U34" s="86"/>
+      <c r="V34" s="86"/>
+      <c r="W34" s="86"/>
+      <c r="X34" s="86"/>
+      <c r="Y34" s="86"/>
+      <c r="Z34" s="86"/>
+      <c r="AA34" s="86"/>
+      <c r="AB34" s="86"/>
+      <c r="AC34" s="86"/>
+      <c r="AD34" s="86"/>
+      <c r="AE34" s="86"/>
+      <c r="AF34" s="86"/>
+      <c r="AG34" s="86"/>
+      <c r="AH34" s="86"/>
+      <c r="AI34" s="86"/>
+      <c r="AJ34" s="86"/>
+      <c r="AK34" s="86"/>
+      <c r="AL34" s="86"/>
+      <c r="AM34" s="86"/>
+      <c r="AN34" s="86"/>
+      <c r="AO34" s="86"/>
+      <c r="AP34" s="86"/>
+      <c r="AQ34" s="86"/>
+      <c r="AR34" s="86"/>
+      <c r="AS34" s="86"/>
+      <c r="AT34" s="86"/>
+      <c r="AU34" s="86"/>
+      <c r="AV34" s="86"/>
+      <c r="AW34" s="86"/>
+      <c r="AX34" s="86"/>
+      <c r="AY34" s="86"/>
+      <c r="AZ34" s="86"/>
+      <c r="BA34" s="86"/>
+      <c r="BB34" s="86"/>
+      <c r="BC34" s="86"/>
+      <c r="BD34" s="86"/>
+      <c r="BE34" s="86"/>
+      <c r="BF34" s="86"/>
+      <c r="BG34" s="86"/>
+      <c r="BH34" s="86"/>
+      <c r="BI34" s="86"/>
+      <c r="BJ34" s="86"/>
+      <c r="BK34" s="86"/>
+      <c r="BL34" s="86"/>
+      <c r="BM34" s="86"/>
+      <c r="BN34" s="86"/>
+      <c r="BO34" s="86"/>
+      <c r="BP34" s="86"/>
+      <c r="BQ34" s="86"/>
+      <c r="BR34" s="86"/>
+      <c r="BS34" s="86"/>
+      <c r="BT34" s="86"/>
+      <c r="BU34" s="86"/>
+      <c r="BV34" s="86"/>
+      <c r="BW34" s="86"/>
+      <c r="BX34" s="86"/>
+      <c r="BY34" s="86"/>
+      <c r="BZ34" s="86"/>
+      <c r="CA34" s="86"/>
+      <c r="CB34" s="86"/>
+      <c r="CC34" s="86"/>
+      <c r="CD34" s="86"/>
+      <c r="CE34" s="86"/>
+      <c r="CF34" s="86"/>
+      <c r="CG34" s="86"/>
+      <c r="CH34" s="86"/>
+      <c r="CI34" s="86"/>
+      <c r="CJ34" s="86"/>
+      <c r="CK34" s="86"/>
+      <c r="CL34" s="86"/>
+      <c r="CM34" s="86"/>
+      <c r="CN34" s="86"/>
+      <c r="CO34" s="86"/>
+      <c r="CP34" s="86"/>
+      <c r="CQ34" s="86"/>
+      <c r="CR34" s="86"/>
+      <c r="CS34" s="86"/>
+      <c r="CT34" s="86"/>
+      <c r="CU34" s="86"/>
+      <c r="CV34" s="86"/>
+      <c r="CW34" s="86"/>
+      <c r="CX34" s="86"/>
+      <c r="CY34" s="86"/>
+      <c r="CZ34" s="86"/>
+      <c r="DA34" s="86"/>
+      <c r="DB34" s="86"/>
+      <c r="DC34" s="86"/>
+      <c r="DD34" s="86"/>
+      <c r="DE34" s="86"/>
+      <c r="DF34" s="86"/>
+      <c r="DG34" s="86"/>
+      <c r="DH34" s="86"/>
+      <c r="DI34" s="86"/>
+      <c r="DJ34" s="86"/>
+      <c r="DK34" s="86"/>
+      <c r="DL34" s="86"/>
+      <c r="DM34" s="86"/>
+      <c r="DN34" s="86"/>
+      <c r="DO34" s="86"/>
+      <c r="DP34" s="86"/>
+      <c r="DQ34" s="86"/>
+      <c r="DR34" s="86"/>
+      <c r="DS34" s="86"/>
+      <c r="DT34" s="86"/>
+      <c r="DU34" s="86"/>
+      <c r="DV34" s="86"/>
+      <c r="DW34" s="86"/>
     </row>
     <row r="35" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="97"/>
-      <c r="C35" s="98"/>
-      <c r="D35" s="99"/>
-      <c r="E35" s="100"/>
-      <c r="F35" s="100"/>
-      <c r="G35" s="95"/>
-      <c r="H35" s="95"/>
-      <c r="I35" s="96"/>
-      <c r="J35" s="96"/>
-      <c r="K35" s="96"/>
-      <c r="L35" s="96"/>
-      <c r="M35" s="96"/>
-      <c r="N35" s="96"/>
-      <c r="O35" s="96"/>
-      <c r="P35" s="96"/>
-      <c r="Q35" s="96"/>
-      <c r="R35" s="96"/>
-      <c r="S35" s="96"/>
-      <c r="T35" s="96"/>
-      <c r="U35" s="96"/>
-      <c r="V35" s="96"/>
-      <c r="W35" s="96"/>
-      <c r="X35" s="96"/>
-      <c r="Y35" s="96"/>
-      <c r="Z35" s="96"/>
-      <c r="AA35" s="96"/>
-      <c r="AB35" s="96"/>
-      <c r="AC35" s="96"/>
-      <c r="AD35" s="96"/>
-      <c r="AE35" s="96"/>
-      <c r="AF35" s="96"/>
-      <c r="AG35" s="96"/>
-      <c r="AH35" s="96"/>
-      <c r="AI35" s="96"/>
-      <c r="AJ35" s="96"/>
-      <c r="AK35" s="96"/>
-      <c r="AL35" s="96"/>
-      <c r="AM35" s="96"/>
-      <c r="AN35" s="96"/>
-      <c r="AO35" s="96"/>
-      <c r="AP35" s="96"/>
-      <c r="AQ35" s="96"/>
-      <c r="AR35" s="96"/>
-      <c r="AS35" s="96"/>
-      <c r="AT35" s="96"/>
-      <c r="AU35" s="96"/>
-      <c r="AV35" s="96"/>
-      <c r="AW35" s="96"/>
-      <c r="AX35" s="96"/>
-      <c r="AY35" s="96"/>
-      <c r="AZ35" s="96"/>
-      <c r="BA35" s="96"/>
-      <c r="BB35" s="96"/>
-      <c r="BC35" s="96"/>
-      <c r="BD35" s="96"/>
-      <c r="BE35" s="96"/>
-      <c r="BF35" s="96"/>
-      <c r="BG35" s="96"/>
-      <c r="BH35" s="96"/>
-      <c r="BI35" s="96"/>
-      <c r="BJ35" s="96"/>
-      <c r="BK35" s="96"/>
-      <c r="BL35" s="96"/>
-      <c r="BM35" s="96"/>
-      <c r="BN35" s="96"/>
-      <c r="BO35" s="96"/>
-      <c r="BP35" s="96"/>
-      <c r="BQ35" s="96"/>
-      <c r="BR35" s="96"/>
-      <c r="BS35" s="96"/>
-      <c r="BT35" s="96"/>
-      <c r="BU35" s="96"/>
-      <c r="BV35" s="96"/>
-      <c r="BW35" s="96"/>
-      <c r="BX35" s="96"/>
-      <c r="BY35" s="96"/>
-      <c r="BZ35" s="96"/>
-      <c r="CA35" s="96"/>
-      <c r="CB35" s="96"/>
-      <c r="CC35" s="96"/>
-      <c r="CD35" s="96"/>
-      <c r="CE35" s="96"/>
-      <c r="CF35" s="96"/>
-      <c r="CG35" s="96"/>
-      <c r="CH35" s="96"/>
-      <c r="CI35" s="96"/>
-      <c r="CJ35" s="96"/>
-      <c r="CK35" s="96"/>
-      <c r="CL35" s="96"/>
-      <c r="CM35" s="96"/>
-      <c r="CN35" s="96"/>
-      <c r="CO35" s="96"/>
-      <c r="CP35" s="96"/>
-      <c r="CQ35" s="96"/>
-      <c r="CR35" s="96"/>
-      <c r="CS35" s="96"/>
-      <c r="CT35" s="96"/>
-      <c r="CU35" s="96"/>
-      <c r="CV35" s="96"/>
-      <c r="CW35" s="96"/>
-      <c r="CX35" s="96"/>
-      <c r="CY35" s="96"/>
-      <c r="CZ35" s="96"/>
-      <c r="DA35" s="96"/>
-      <c r="DB35" s="96"/>
-      <c r="DC35" s="96"/>
-      <c r="DD35" s="96"/>
-      <c r="DE35" s="96"/>
-      <c r="DF35" s="96"/>
-      <c r="DG35" s="96"/>
-      <c r="DH35" s="96"/>
-      <c r="DI35" s="96"/>
-      <c r="DJ35" s="96"/>
-      <c r="DK35" s="96"/>
-      <c r="DL35" s="96"/>
-      <c r="DM35" s="96"/>
-      <c r="DN35" s="96"/>
-      <c r="DO35" s="96"/>
-      <c r="DP35" s="96"/>
-      <c r="DQ35" s="96"/>
-      <c r="DR35" s="96"/>
-      <c r="DS35" s="96"/>
-      <c r="DT35" s="96"/>
-      <c r="DU35" s="96"/>
-      <c r="DV35" s="96"/>
-      <c r="DW35" s="96"/>
+      <c r="B35" s="93"/>
+      <c r="C35" s="94"/>
+      <c r="D35" s="95"/>
+      <c r="E35" s="96"/>
+      <c r="F35" s="96"/>
+      <c r="G35" s="91"/>
+      <c r="H35" s="91"/>
+      <c r="I35" s="92"/>
+      <c r="J35" s="92"/>
+      <c r="K35" s="92"/>
+      <c r="L35" s="92"/>
+      <c r="M35" s="92"/>
+      <c r="N35" s="92"/>
+      <c r="O35" s="92"/>
+      <c r="P35" s="92"/>
+      <c r="Q35" s="92"/>
+      <c r="R35" s="92"/>
+      <c r="S35" s="92"/>
+      <c r="T35" s="92"/>
+      <c r="U35" s="92"/>
+      <c r="V35" s="92"/>
+      <c r="W35" s="92"/>
+      <c r="X35" s="92"/>
+      <c r="Y35" s="92"/>
+      <c r="Z35" s="92"/>
+      <c r="AA35" s="92"/>
+      <c r="AB35" s="92"/>
+      <c r="AC35" s="92"/>
+      <c r="AD35" s="92"/>
+      <c r="AE35" s="92"/>
+      <c r="AF35" s="92"/>
+      <c r="AG35" s="92"/>
+      <c r="AH35" s="92"/>
+      <c r="AI35" s="92"/>
+      <c r="AJ35" s="92"/>
+      <c r="AK35" s="92"/>
+      <c r="AL35" s="92"/>
+      <c r="AM35" s="92"/>
+      <c r="AN35" s="92"/>
+      <c r="AO35" s="92"/>
+      <c r="AP35" s="92"/>
+      <c r="AQ35" s="92"/>
+      <c r="AR35" s="92"/>
+      <c r="AS35" s="92"/>
+      <c r="AT35" s="92"/>
+      <c r="AU35" s="92"/>
+      <c r="AV35" s="92"/>
+      <c r="AW35" s="92"/>
+      <c r="AX35" s="92"/>
+      <c r="AY35" s="92"/>
+      <c r="AZ35" s="92"/>
+      <c r="BA35" s="92"/>
+      <c r="BB35" s="92"/>
+      <c r="BC35" s="92"/>
+      <c r="BD35" s="92"/>
+      <c r="BE35" s="92"/>
+      <c r="BF35" s="92"/>
+      <c r="BG35" s="92"/>
+      <c r="BH35" s="92"/>
+      <c r="BI35" s="92"/>
+      <c r="BJ35" s="92"/>
+      <c r="BK35" s="92"/>
+      <c r="BL35" s="92"/>
+      <c r="BM35" s="92"/>
+      <c r="BN35" s="92"/>
+      <c r="BO35" s="92"/>
+      <c r="BP35" s="92"/>
+      <c r="BQ35" s="92"/>
+      <c r="BR35" s="92"/>
+      <c r="BS35" s="92"/>
+      <c r="BT35" s="92"/>
+      <c r="BU35" s="92"/>
+      <c r="BV35" s="92"/>
+      <c r="BW35" s="92"/>
+      <c r="BX35" s="92"/>
+      <c r="BY35" s="92"/>
+      <c r="BZ35" s="92"/>
+      <c r="CA35" s="92"/>
+      <c r="CB35" s="92"/>
+      <c r="CC35" s="92"/>
+      <c r="CD35" s="92"/>
+      <c r="CE35" s="92"/>
+      <c r="CF35" s="92"/>
+      <c r="CG35" s="92"/>
+      <c r="CH35" s="92"/>
+      <c r="CI35" s="92"/>
+      <c r="CJ35" s="92"/>
+      <c r="CK35" s="92"/>
+      <c r="CL35" s="92"/>
+      <c r="CM35" s="92"/>
+      <c r="CN35" s="92"/>
+      <c r="CO35" s="92"/>
+      <c r="CP35" s="92"/>
+      <c r="CQ35" s="92"/>
+      <c r="CR35" s="92"/>
+      <c r="CS35" s="92"/>
+      <c r="CT35" s="92"/>
+      <c r="CU35" s="92"/>
+      <c r="CV35" s="92"/>
+      <c r="CW35" s="92"/>
+      <c r="CX35" s="92"/>
+      <c r="CY35" s="92"/>
+      <c r="CZ35" s="92"/>
+      <c r="DA35" s="92"/>
+      <c r="DB35" s="92"/>
+      <c r="DC35" s="92"/>
+      <c r="DD35" s="92"/>
+      <c r="DE35" s="92"/>
+      <c r="DF35" s="92"/>
+      <c r="DG35" s="92"/>
+      <c r="DH35" s="92"/>
+      <c r="DI35" s="92"/>
+      <c r="DJ35" s="92"/>
+      <c r="DK35" s="92"/>
+      <c r="DL35" s="92"/>
+      <c r="DM35" s="92"/>
+      <c r="DN35" s="92"/>
+      <c r="DO35" s="92"/>
+      <c r="DP35" s="92"/>
+      <c r="DQ35" s="92"/>
+      <c r="DR35" s="92"/>
+      <c r="DS35" s="92"/>
+      <c r="DT35" s="92"/>
+      <c r="DU35" s="92"/>
+      <c r="DV35" s="92"/>
+      <c r="DW35" s="92"/>
     </row>
     <row r="36" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="101"/>
-      <c r="C36" s="92"/>
-      <c r="D36" s="93"/>
-      <c r="E36" s="102"/>
-      <c r="F36" s="103"/>
-      <c r="G36" s="95"/>
-      <c r="H36" s="95"/>
-      <c r="I36" s="96"/>
-      <c r="J36" s="96"/>
-      <c r="K36" s="96"/>
-      <c r="L36" s="96"/>
-      <c r="M36" s="96"/>
-      <c r="N36" s="96"/>
-      <c r="O36" s="96"/>
-      <c r="P36" s="96"/>
-      <c r="Q36" s="96"/>
-      <c r="R36" s="96"/>
-      <c r="S36" s="96"/>
-      <c r="T36" s="96"/>
-      <c r="U36" s="96"/>
-      <c r="V36" s="96"/>
-      <c r="W36" s="96"/>
-      <c r="X36" s="96"/>
-      <c r="Y36" s="96"/>
-      <c r="Z36" s="96"/>
-      <c r="AA36" s="96"/>
-      <c r="AB36" s="96"/>
-      <c r="AC36" s="96"/>
-      <c r="AD36" s="96"/>
-      <c r="AE36" s="96"/>
-      <c r="AF36" s="96"/>
-      <c r="AG36" s="96"/>
-      <c r="AH36" s="96"/>
-      <c r="AI36" s="96"/>
-      <c r="AJ36" s="96"/>
-      <c r="AK36" s="96"/>
-      <c r="AL36" s="96"/>
-      <c r="AM36" s="96"/>
-      <c r="AN36" s="96"/>
-      <c r="AO36" s="96"/>
-      <c r="AP36" s="96"/>
-      <c r="AQ36" s="96"/>
-      <c r="AR36" s="96"/>
-      <c r="AS36" s="96"/>
-      <c r="AT36" s="96"/>
-      <c r="AU36" s="96"/>
-      <c r="AV36" s="96"/>
-      <c r="AW36" s="96"/>
-      <c r="AX36" s="96"/>
-      <c r="AY36" s="96"/>
-      <c r="AZ36" s="96"/>
-      <c r="BA36" s="96"/>
-      <c r="BB36" s="96"/>
-      <c r="BC36" s="96"/>
-      <c r="BD36" s="96"/>
-      <c r="BE36" s="96"/>
-      <c r="BF36" s="96"/>
-      <c r="BG36" s="96"/>
-      <c r="BH36" s="96"/>
-      <c r="BI36" s="96"/>
-      <c r="BJ36" s="96"/>
-      <c r="BK36" s="96"/>
-      <c r="BL36" s="96"/>
-      <c r="BM36" s="96"/>
-      <c r="BN36" s="96"/>
-      <c r="BO36" s="96"/>
-      <c r="BP36" s="96"/>
-      <c r="BQ36" s="96"/>
-      <c r="BR36" s="96"/>
-      <c r="BS36" s="96"/>
-      <c r="BT36" s="96"/>
-      <c r="BU36" s="96"/>
-      <c r="BV36" s="96"/>
-      <c r="BW36" s="96"/>
-      <c r="BX36" s="96"/>
-      <c r="BY36" s="96"/>
-      <c r="BZ36" s="96"/>
-      <c r="CA36" s="96"/>
-      <c r="CB36" s="96"/>
-      <c r="CC36" s="96"/>
-      <c r="CD36" s="96"/>
-      <c r="CE36" s="96"/>
-      <c r="CF36" s="96"/>
-      <c r="CG36" s="96"/>
-      <c r="CH36" s="96"/>
-      <c r="CI36" s="96"/>
-      <c r="CJ36" s="96"/>
-      <c r="CK36" s="96"/>
-      <c r="CL36" s="96"/>
-      <c r="CM36" s="96"/>
-      <c r="CN36" s="96"/>
-      <c r="CO36" s="96"/>
-      <c r="CP36" s="96"/>
-      <c r="CQ36" s="96"/>
-      <c r="CR36" s="96"/>
-      <c r="CS36" s="96"/>
-      <c r="CT36" s="96"/>
-      <c r="CU36" s="96"/>
-      <c r="CV36" s="96"/>
-      <c r="CW36" s="96"/>
-      <c r="CX36" s="96"/>
-      <c r="CY36" s="96"/>
-      <c r="CZ36" s="96"/>
-      <c r="DA36" s="96"/>
-      <c r="DB36" s="96"/>
-      <c r="DC36" s="96"/>
-      <c r="DD36" s="96"/>
-      <c r="DE36" s="96"/>
-      <c r="DF36" s="96"/>
-      <c r="DG36" s="96"/>
-      <c r="DH36" s="96"/>
-      <c r="DI36" s="96"/>
-      <c r="DJ36" s="96"/>
-      <c r="DK36" s="96"/>
-      <c r="DL36" s="96"/>
-      <c r="DM36" s="96"/>
-      <c r="DN36" s="96"/>
-      <c r="DO36" s="96"/>
-      <c r="DP36" s="96"/>
-      <c r="DQ36" s="96"/>
-      <c r="DR36" s="96"/>
-      <c r="DS36" s="96"/>
-      <c r="DT36" s="96"/>
-      <c r="DU36" s="96"/>
-      <c r="DV36" s="96"/>
-      <c r="DW36" s="96"/>
+      <c r="B36" s="97"/>
+      <c r="C36" s="88"/>
+      <c r="D36" s="89"/>
+      <c r="E36" s="98"/>
+      <c r="F36" s="99"/>
+      <c r="G36" s="91"/>
+      <c r="H36" s="91"/>
+      <c r="I36" s="92"/>
+      <c r="J36" s="92"/>
+      <c r="K36" s="92"/>
+      <c r="L36" s="92"/>
+      <c r="M36" s="92"/>
+      <c r="N36" s="92"/>
+      <c r="O36" s="92"/>
+      <c r="P36" s="92"/>
+      <c r="Q36" s="92"/>
+      <c r="R36" s="92"/>
+      <c r="S36" s="92"/>
+      <c r="T36" s="92"/>
+      <c r="U36" s="92"/>
+      <c r="V36" s="92"/>
+      <c r="W36" s="92"/>
+      <c r="X36" s="92"/>
+      <c r="Y36" s="92"/>
+      <c r="Z36" s="92"/>
+      <c r="AA36" s="92"/>
+      <c r="AB36" s="92"/>
+      <c r="AC36" s="92"/>
+      <c r="AD36" s="92"/>
+      <c r="AE36" s="92"/>
+      <c r="AF36" s="92"/>
+      <c r="AG36" s="92"/>
+      <c r="AH36" s="92"/>
+      <c r="AI36" s="92"/>
+      <c r="AJ36" s="92"/>
+      <c r="AK36" s="92"/>
+      <c r="AL36" s="92"/>
+      <c r="AM36" s="92"/>
+      <c r="AN36" s="92"/>
+      <c r="AO36" s="92"/>
+      <c r="AP36" s="92"/>
+      <c r="AQ36" s="92"/>
+      <c r="AR36" s="92"/>
+      <c r="AS36" s="92"/>
+      <c r="AT36" s="92"/>
+      <c r="AU36" s="92"/>
+      <c r="AV36" s="92"/>
+      <c r="AW36" s="92"/>
+      <c r="AX36" s="92"/>
+      <c r="AY36" s="92"/>
+      <c r="AZ36" s="92"/>
+      <c r="BA36" s="92"/>
+      <c r="BB36" s="92"/>
+      <c r="BC36" s="92"/>
+      <c r="BD36" s="92"/>
+      <c r="BE36" s="92"/>
+      <c r="BF36" s="92"/>
+      <c r="BG36" s="92"/>
+      <c r="BH36" s="92"/>
+      <c r="BI36" s="92"/>
+      <c r="BJ36" s="92"/>
+      <c r="BK36" s="92"/>
+      <c r="BL36" s="92"/>
+      <c r="BM36" s="92"/>
+      <c r="BN36" s="92"/>
+      <c r="BO36" s="92"/>
+      <c r="BP36" s="92"/>
+      <c r="BQ36" s="92"/>
+      <c r="BR36" s="92"/>
+      <c r="BS36" s="92"/>
+      <c r="BT36" s="92"/>
+      <c r="BU36" s="92"/>
+      <c r="BV36" s="92"/>
+      <c r="BW36" s="92"/>
+      <c r="BX36" s="92"/>
+      <c r="BY36" s="92"/>
+      <c r="BZ36" s="92"/>
+      <c r="CA36" s="92"/>
+      <c r="CB36" s="92"/>
+      <c r="CC36" s="92"/>
+      <c r="CD36" s="92"/>
+      <c r="CE36" s="92"/>
+      <c r="CF36" s="92"/>
+      <c r="CG36" s="92"/>
+      <c r="CH36" s="92"/>
+      <c r="CI36" s="92"/>
+      <c r="CJ36" s="92"/>
+      <c r="CK36" s="92"/>
+      <c r="CL36" s="92"/>
+      <c r="CM36" s="92"/>
+      <c r="CN36" s="92"/>
+      <c r="CO36" s="92"/>
+      <c r="CP36" s="92"/>
+      <c r="CQ36" s="92"/>
+      <c r="CR36" s="92"/>
+      <c r="CS36" s="92"/>
+      <c r="CT36" s="92"/>
+      <c r="CU36" s="92"/>
+      <c r="CV36" s="92"/>
+      <c r="CW36" s="92"/>
+      <c r="CX36" s="92"/>
+      <c r="CY36" s="92"/>
+      <c r="CZ36" s="92"/>
+      <c r="DA36" s="92"/>
+      <c r="DB36" s="92"/>
+      <c r="DC36" s="92"/>
+      <c r="DD36" s="92"/>
+      <c r="DE36" s="92"/>
+      <c r="DF36" s="92"/>
+      <c r="DG36" s="92"/>
+      <c r="DH36" s="92"/>
+      <c r="DI36" s="92"/>
+      <c r="DJ36" s="92"/>
+      <c r="DK36" s="92"/>
+      <c r="DL36" s="92"/>
+      <c r="DM36" s="92"/>
+      <c r="DN36" s="92"/>
+      <c r="DO36" s="92"/>
+      <c r="DP36" s="92"/>
+      <c r="DQ36" s="92"/>
+      <c r="DR36" s="92"/>
+      <c r="DS36" s="92"/>
+      <c r="DT36" s="92"/>
+      <c r="DU36" s="92"/>
+      <c r="DV36" s="92"/>
+      <c r="DW36" s="92"/>
     </row>
     <row r="37" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="91"/>
-      <c r="C37" s="92"/>
-      <c r="D37" s="93"/>
-      <c r="E37" s="94"/>
-      <c r="F37" s="94"/>
-      <c r="G37" s="95"/>
-      <c r="H37" s="95"/>
-      <c r="I37" s="96"/>
-      <c r="J37" s="96"/>
-      <c r="K37" s="96"/>
-      <c r="L37" s="96"/>
-      <c r="M37" s="96"/>
-      <c r="N37" s="96"/>
-      <c r="O37" s="96"/>
-      <c r="P37" s="96"/>
-      <c r="Q37" s="96"/>
-      <c r="R37" s="96"/>
-      <c r="S37" s="96"/>
-      <c r="T37" s="96"/>
-      <c r="U37" s="96"/>
-      <c r="V37" s="96"/>
-      <c r="W37" s="96"/>
-      <c r="X37" s="96"/>
-      <c r="Y37" s="96"/>
-      <c r="Z37" s="96"/>
-      <c r="AA37" s="96"/>
-      <c r="AB37" s="96"/>
-      <c r="AC37" s="96"/>
-      <c r="AD37" s="96"/>
-      <c r="AE37" s="96"/>
-      <c r="AF37" s="96"/>
-      <c r="AG37" s="96"/>
-      <c r="AH37" s="96"/>
-      <c r="AI37" s="96"/>
-      <c r="AJ37" s="96"/>
-      <c r="AK37" s="96"/>
-      <c r="AL37" s="96"/>
-      <c r="AM37" s="96"/>
-      <c r="AN37" s="96"/>
-      <c r="AO37" s="96"/>
-      <c r="AP37" s="96"/>
-      <c r="AQ37" s="96"/>
-      <c r="AR37" s="96"/>
-      <c r="AS37" s="96"/>
-      <c r="AT37" s="96"/>
-      <c r="AU37" s="96"/>
-      <c r="AV37" s="96"/>
-      <c r="AW37" s="96"/>
-      <c r="AX37" s="96"/>
-      <c r="AY37" s="96"/>
-      <c r="AZ37" s="96"/>
-      <c r="BA37" s="96"/>
-      <c r="BB37" s="96"/>
-      <c r="BC37" s="96"/>
-      <c r="BD37" s="96"/>
-      <c r="BE37" s="96"/>
-      <c r="BF37" s="96"/>
-      <c r="BG37" s="96"/>
-      <c r="BH37" s="96"/>
-      <c r="BI37" s="96"/>
-      <c r="BJ37" s="96"/>
-      <c r="BK37" s="96"/>
-      <c r="BL37" s="96"/>
-      <c r="BM37" s="96"/>
-      <c r="BN37" s="96"/>
-      <c r="BO37" s="96"/>
-      <c r="BP37" s="96"/>
-      <c r="BQ37" s="96"/>
-      <c r="BR37" s="96"/>
-      <c r="BS37" s="96"/>
-      <c r="BT37" s="96"/>
-      <c r="BU37" s="96"/>
-      <c r="BV37" s="96"/>
-      <c r="BW37" s="96"/>
-      <c r="BX37" s="96"/>
-      <c r="BY37" s="96"/>
-      <c r="BZ37" s="96"/>
-      <c r="CA37" s="96"/>
-      <c r="CB37" s="96"/>
-      <c r="CC37" s="96"/>
-      <c r="CD37" s="96"/>
-      <c r="CE37" s="96"/>
-      <c r="CF37" s="96"/>
-      <c r="CG37" s="96"/>
-      <c r="CH37" s="96"/>
-      <c r="CI37" s="96"/>
-      <c r="CJ37" s="96"/>
-      <c r="CK37" s="96"/>
-      <c r="CL37" s="96"/>
-      <c r="CM37" s="96"/>
-      <c r="CN37" s="96"/>
-      <c r="CO37" s="96"/>
-      <c r="CP37" s="96"/>
-      <c r="CQ37" s="96"/>
-      <c r="CR37" s="96"/>
-      <c r="CS37" s="96"/>
-      <c r="CT37" s="96"/>
-      <c r="CU37" s="96"/>
-      <c r="CV37" s="96"/>
-      <c r="CW37" s="96"/>
-      <c r="CX37" s="96"/>
-      <c r="CY37" s="96"/>
-      <c r="CZ37" s="96"/>
-      <c r="DA37" s="96"/>
-      <c r="DB37" s="96"/>
-      <c r="DC37" s="96"/>
-      <c r="DD37" s="96"/>
-      <c r="DE37" s="96"/>
-      <c r="DF37" s="96"/>
-      <c r="DG37" s="96"/>
-      <c r="DH37" s="96"/>
-      <c r="DI37" s="96"/>
-      <c r="DJ37" s="96"/>
-      <c r="DK37" s="96"/>
-      <c r="DL37" s="96"/>
-      <c r="DM37" s="96"/>
-      <c r="DN37" s="96"/>
-      <c r="DO37" s="96"/>
-      <c r="DP37" s="96"/>
-      <c r="DQ37" s="96"/>
-      <c r="DR37" s="96"/>
-      <c r="DS37" s="96"/>
-      <c r="DT37" s="96"/>
-      <c r="DU37" s="96"/>
-      <c r="DV37" s="96"/>
-      <c r="DW37" s="96"/>
+      <c r="B37" s="87"/>
+      <c r="C37" s="88"/>
+      <c r="D37" s="89"/>
+      <c r="E37" s="90"/>
+      <c r="F37" s="90"/>
+      <c r="G37" s="91"/>
+      <c r="H37" s="91"/>
+      <c r="I37" s="92"/>
+      <c r="J37" s="92"/>
+      <c r="K37" s="92"/>
+      <c r="L37" s="92"/>
+      <c r="M37" s="92"/>
+      <c r="N37" s="92"/>
+      <c r="O37" s="92"/>
+      <c r="P37" s="92"/>
+      <c r="Q37" s="92"/>
+      <c r="R37" s="92"/>
+      <c r="S37" s="92"/>
+      <c r="T37" s="92"/>
+      <c r="U37" s="92"/>
+      <c r="V37" s="92"/>
+      <c r="W37" s="92"/>
+      <c r="X37" s="92"/>
+      <c r="Y37" s="92"/>
+      <c r="Z37" s="92"/>
+      <c r="AA37" s="92"/>
+      <c r="AB37" s="92"/>
+      <c r="AC37" s="92"/>
+      <c r="AD37" s="92"/>
+      <c r="AE37" s="92"/>
+      <c r="AF37" s="92"/>
+      <c r="AG37" s="92"/>
+      <c r="AH37" s="92"/>
+      <c r="AI37" s="92"/>
+      <c r="AJ37" s="92"/>
+      <c r="AK37" s="92"/>
+      <c r="AL37" s="92"/>
+      <c r="AM37" s="92"/>
+      <c r="AN37" s="92"/>
+      <c r="AO37" s="92"/>
+      <c r="AP37" s="92"/>
+      <c r="AQ37" s="92"/>
+      <c r="AR37" s="92"/>
+      <c r="AS37" s="92"/>
+      <c r="AT37" s="92"/>
+      <c r="AU37" s="92"/>
+      <c r="AV37" s="92"/>
+      <c r="AW37" s="92"/>
+      <c r="AX37" s="92"/>
+      <c r="AY37" s="92"/>
+      <c r="AZ37" s="92"/>
+      <c r="BA37" s="92"/>
+      <c r="BB37" s="92"/>
+      <c r="BC37" s="92"/>
+      <c r="BD37" s="92"/>
+      <c r="BE37" s="92"/>
+      <c r="BF37" s="92"/>
+      <c r="BG37" s="92"/>
+      <c r="BH37" s="92"/>
+      <c r="BI37" s="92"/>
+      <c r="BJ37" s="92"/>
+      <c r="BK37" s="92"/>
+      <c r="BL37" s="92"/>
+      <c r="BM37" s="92"/>
+      <c r="BN37" s="92"/>
+      <c r="BO37" s="92"/>
+      <c r="BP37" s="92"/>
+      <c r="BQ37" s="92"/>
+      <c r="BR37" s="92"/>
+      <c r="BS37" s="92"/>
+      <c r="BT37" s="92"/>
+      <c r="BU37" s="92"/>
+      <c r="BV37" s="92"/>
+      <c r="BW37" s="92"/>
+      <c r="BX37" s="92"/>
+      <c r="BY37" s="92"/>
+      <c r="BZ37" s="92"/>
+      <c r="CA37" s="92"/>
+      <c r="CB37" s="92"/>
+      <c r="CC37" s="92"/>
+      <c r="CD37" s="92"/>
+      <c r="CE37" s="92"/>
+      <c r="CF37" s="92"/>
+      <c r="CG37" s="92"/>
+      <c r="CH37" s="92"/>
+      <c r="CI37" s="92"/>
+      <c r="CJ37" s="92"/>
+      <c r="CK37" s="92"/>
+      <c r="CL37" s="92"/>
+      <c r="CM37" s="92"/>
+      <c r="CN37" s="92"/>
+      <c r="CO37" s="92"/>
+      <c r="CP37" s="92"/>
+      <c r="CQ37" s="92"/>
+      <c r="CR37" s="92"/>
+      <c r="CS37" s="92"/>
+      <c r="CT37" s="92"/>
+      <c r="CU37" s="92"/>
+      <c r="CV37" s="92"/>
+      <c r="CW37" s="92"/>
+      <c r="CX37" s="92"/>
+      <c r="CY37" s="92"/>
+      <c r="CZ37" s="92"/>
+      <c r="DA37" s="92"/>
+      <c r="DB37" s="92"/>
+      <c r="DC37" s="92"/>
+      <c r="DD37" s="92"/>
+      <c r="DE37" s="92"/>
+      <c r="DF37" s="92"/>
+      <c r="DG37" s="92"/>
+      <c r="DH37" s="92"/>
+      <c r="DI37" s="92"/>
+      <c r="DJ37" s="92"/>
+      <c r="DK37" s="92"/>
+      <c r="DL37" s="92"/>
+      <c r="DM37" s="92"/>
+      <c r="DN37" s="92"/>
+      <c r="DO37" s="92"/>
+      <c r="DP37" s="92"/>
+      <c r="DQ37" s="92"/>
+      <c r="DR37" s="92"/>
+      <c r="DS37" s="92"/>
+      <c r="DT37" s="92"/>
+      <c r="DU37" s="92"/>
+      <c r="DV37" s="92"/>
+      <c r="DW37" s="92"/>
     </row>
     <row r="38" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="91"/>
-      <c r="C38" s="92"/>
-      <c r="D38" s="93"/>
-      <c r="E38" s="94"/>
-      <c r="F38" s="94"/>
-      <c r="G38" s="95"/>
-      <c r="H38" s="95"/>
-      <c r="I38" s="96"/>
-      <c r="J38" s="96"/>
-      <c r="K38" s="96"/>
-      <c r="L38" s="96"/>
-      <c r="M38" s="96"/>
-      <c r="N38" s="96"/>
-      <c r="O38" s="96"/>
-      <c r="P38" s="96"/>
-      <c r="Q38" s="96"/>
-      <c r="R38" s="96"/>
-      <c r="S38" s="96"/>
-      <c r="T38" s="96"/>
-      <c r="U38" s="96"/>
-      <c r="V38" s="96"/>
-      <c r="W38" s="96"/>
-      <c r="X38" s="96"/>
-      <c r="Y38" s="96"/>
-      <c r="Z38" s="96"/>
-      <c r="AA38" s="96"/>
-      <c r="AB38" s="96"/>
-      <c r="AC38" s="96"/>
-      <c r="AD38" s="96"/>
-      <c r="AE38" s="96"/>
-      <c r="AF38" s="96"/>
-      <c r="AG38" s="96"/>
-      <c r="AH38" s="96"/>
-      <c r="AI38" s="96"/>
-      <c r="AJ38" s="96"/>
-      <c r="AK38" s="96"/>
-      <c r="AL38" s="96"/>
-      <c r="AM38" s="96"/>
-      <c r="AN38" s="96"/>
-      <c r="AO38" s="96"/>
-      <c r="AP38" s="96"/>
-      <c r="AQ38" s="96"/>
-      <c r="AR38" s="96"/>
-      <c r="AS38" s="96"/>
-      <c r="AT38" s="96"/>
-      <c r="AU38" s="96"/>
-      <c r="AV38" s="96"/>
-      <c r="AW38" s="96"/>
-      <c r="AX38" s="96"/>
-      <c r="AY38" s="96"/>
-      <c r="AZ38" s="96"/>
-      <c r="BA38" s="96"/>
-      <c r="BB38" s="96"/>
-      <c r="BC38" s="96"/>
-      <c r="BD38" s="96"/>
-      <c r="BE38" s="96"/>
-      <c r="BF38" s="96"/>
-      <c r="BG38" s="96"/>
-      <c r="BH38" s="96"/>
-      <c r="BI38" s="96"/>
-      <c r="BJ38" s="96"/>
-      <c r="BK38" s="96"/>
-      <c r="BL38" s="96"/>
-      <c r="BM38" s="96"/>
-      <c r="BN38" s="96"/>
-      <c r="BO38" s="96"/>
-      <c r="BP38" s="96"/>
-      <c r="BQ38" s="96"/>
-      <c r="BR38" s="96"/>
-      <c r="BS38" s="96"/>
-      <c r="BT38" s="96"/>
-      <c r="BU38" s="96"/>
-      <c r="BV38" s="96"/>
-      <c r="BW38" s="96"/>
-      <c r="BX38" s="96"/>
-      <c r="BY38" s="96"/>
-      <c r="BZ38" s="96"/>
-      <c r="CA38" s="96"/>
-      <c r="CB38" s="96"/>
-      <c r="CC38" s="96"/>
-      <c r="CD38" s="96"/>
-      <c r="CE38" s="96"/>
-      <c r="CF38" s="96"/>
-      <c r="CG38" s="96"/>
-      <c r="CH38" s="96"/>
-      <c r="CI38" s="96"/>
-      <c r="CJ38" s="96"/>
-      <c r="CK38" s="96"/>
-      <c r="CL38" s="96"/>
-      <c r="CM38" s="96"/>
-      <c r="CN38" s="96"/>
-      <c r="CO38" s="96"/>
-      <c r="CP38" s="96"/>
-      <c r="CQ38" s="96"/>
-      <c r="CR38" s="96"/>
-      <c r="CS38" s="96"/>
-      <c r="CT38" s="96"/>
-      <c r="CU38" s="96"/>
-      <c r="CV38" s="96"/>
-      <c r="CW38" s="96"/>
-      <c r="CX38" s="96"/>
-      <c r="CY38" s="96"/>
-      <c r="CZ38" s="96"/>
-      <c r="DA38" s="96"/>
-      <c r="DB38" s="96"/>
-      <c r="DC38" s="96"/>
-      <c r="DD38" s="96"/>
-      <c r="DE38" s="96"/>
-      <c r="DF38" s="96"/>
-      <c r="DG38" s="96"/>
-      <c r="DH38" s="96"/>
-      <c r="DI38" s="96"/>
-      <c r="DJ38" s="96"/>
-      <c r="DK38" s="96"/>
-      <c r="DL38" s="96"/>
-      <c r="DM38" s="96"/>
-      <c r="DN38" s="96"/>
-      <c r="DO38" s="96"/>
-      <c r="DP38" s="96"/>
-      <c r="DQ38" s="96"/>
-      <c r="DR38" s="96"/>
-      <c r="DS38" s="96"/>
-      <c r="DT38" s="96"/>
-      <c r="DU38" s="96"/>
-      <c r="DV38" s="96"/>
-      <c r="DW38" s="96"/>
+      <c r="B38" s="87"/>
+      <c r="C38" s="88"/>
+      <c r="D38" s="89"/>
+      <c r="E38" s="90"/>
+      <c r="F38" s="90"/>
+      <c r="G38" s="91"/>
+      <c r="H38" s="91"/>
+      <c r="I38" s="92"/>
+      <c r="J38" s="92"/>
+      <c r="K38" s="92"/>
+      <c r="L38" s="92"/>
+      <c r="M38" s="92"/>
+      <c r="N38" s="92"/>
+      <c r="O38" s="92"/>
+      <c r="P38" s="92"/>
+      <c r="Q38" s="92"/>
+      <c r="R38" s="92"/>
+      <c r="S38" s="92"/>
+      <c r="T38" s="92"/>
+      <c r="U38" s="92"/>
+      <c r="V38" s="92"/>
+      <c r="W38" s="92"/>
+      <c r="X38" s="92"/>
+      <c r="Y38" s="92"/>
+      <c r="Z38" s="92"/>
+      <c r="AA38" s="92"/>
+      <c r="AB38" s="92"/>
+      <c r="AC38" s="92"/>
+      <c r="AD38" s="92"/>
+      <c r="AE38" s="92"/>
+      <c r="AF38" s="92"/>
+      <c r="AG38" s="92"/>
+      <c r="AH38" s="92"/>
+      <c r="AI38" s="92"/>
+      <c r="AJ38" s="92"/>
+      <c r="AK38" s="92"/>
+      <c r="AL38" s="92"/>
+      <c r="AM38" s="92"/>
+      <c r="AN38" s="92"/>
+      <c r="AO38" s="92"/>
+      <c r="AP38" s="92"/>
+      <c r="AQ38" s="92"/>
+      <c r="AR38" s="92"/>
+      <c r="AS38" s="92"/>
+      <c r="AT38" s="92"/>
+      <c r="AU38" s="92"/>
+      <c r="AV38" s="92"/>
+      <c r="AW38" s="92"/>
+      <c r="AX38" s="92"/>
+      <c r="AY38" s="92"/>
+      <c r="AZ38" s="92"/>
+      <c r="BA38" s="92"/>
+      <c r="BB38" s="92"/>
+      <c r="BC38" s="92"/>
+      <c r="BD38" s="92"/>
+      <c r="BE38" s="92"/>
+      <c r="BF38" s="92"/>
+      <c r="BG38" s="92"/>
+      <c r="BH38" s="92"/>
+      <c r="BI38" s="92"/>
+      <c r="BJ38" s="92"/>
+      <c r="BK38" s="92"/>
+      <c r="BL38" s="92"/>
+      <c r="BM38" s="92"/>
+      <c r="BN38" s="92"/>
+      <c r="BO38" s="92"/>
+      <c r="BP38" s="92"/>
+      <c r="BQ38" s="92"/>
+      <c r="BR38" s="92"/>
+      <c r="BS38" s="92"/>
+      <c r="BT38" s="92"/>
+      <c r="BU38" s="92"/>
+      <c r="BV38" s="92"/>
+      <c r="BW38" s="92"/>
+      <c r="BX38" s="92"/>
+      <c r="BY38" s="92"/>
+      <c r="BZ38" s="92"/>
+      <c r="CA38" s="92"/>
+      <c r="CB38" s="92"/>
+      <c r="CC38" s="92"/>
+      <c r="CD38" s="92"/>
+      <c r="CE38" s="92"/>
+      <c r="CF38" s="92"/>
+      <c r="CG38" s="92"/>
+      <c r="CH38" s="92"/>
+      <c r="CI38" s="92"/>
+      <c r="CJ38" s="92"/>
+      <c r="CK38" s="92"/>
+      <c r="CL38" s="92"/>
+      <c r="CM38" s="92"/>
+      <c r="CN38" s="92"/>
+      <c r="CO38" s="92"/>
+      <c r="CP38" s="92"/>
+      <c r="CQ38" s="92"/>
+      <c r="CR38" s="92"/>
+      <c r="CS38" s="92"/>
+      <c r="CT38" s="92"/>
+      <c r="CU38" s="92"/>
+      <c r="CV38" s="92"/>
+      <c r="CW38" s="92"/>
+      <c r="CX38" s="92"/>
+      <c r="CY38" s="92"/>
+      <c r="CZ38" s="92"/>
+      <c r="DA38" s="92"/>
+      <c r="DB38" s="92"/>
+      <c r="DC38" s="92"/>
+      <c r="DD38" s="92"/>
+      <c r="DE38" s="92"/>
+      <c r="DF38" s="92"/>
+      <c r="DG38" s="92"/>
+      <c r="DH38" s="92"/>
+      <c r="DI38" s="92"/>
+      <c r="DJ38" s="92"/>
+      <c r="DK38" s="92"/>
+      <c r="DL38" s="92"/>
+      <c r="DM38" s="92"/>
+      <c r="DN38" s="92"/>
+      <c r="DO38" s="92"/>
+      <c r="DP38" s="92"/>
+      <c r="DQ38" s="92"/>
+      <c r="DR38" s="92"/>
+      <c r="DS38" s="92"/>
+      <c r="DT38" s="92"/>
+      <c r="DU38" s="92"/>
+      <c r="DV38" s="92"/>
+      <c r="DW38" s="92"/>
     </row>
     <row r="39" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="91"/>
-      <c r="C39" s="92"/>
-      <c r="D39" s="93"/>
-      <c r="E39" s="94"/>
-      <c r="F39" s="94"/>
-      <c r="G39" s="95"/>
-      <c r="H39" s="95"/>
-      <c r="I39" s="96"/>
-      <c r="J39" s="96"/>
-      <c r="K39" s="96"/>
-      <c r="L39" s="96"/>
-      <c r="M39" s="96"/>
-      <c r="N39" s="96"/>
-      <c r="O39" s="96"/>
-      <c r="P39" s="96"/>
-      <c r="Q39" s="96"/>
-      <c r="R39" s="96"/>
-      <c r="S39" s="96"/>
-      <c r="T39" s="96"/>
-      <c r="U39" s="96"/>
-      <c r="V39" s="96"/>
-      <c r="W39" s="96"/>
-      <c r="X39" s="96"/>
-      <c r="Y39" s="96"/>
-      <c r="Z39" s="96"/>
-      <c r="AA39" s="96"/>
-      <c r="AB39" s="96"/>
-      <c r="AC39" s="96"/>
-      <c r="AD39" s="96"/>
-      <c r="AE39" s="96"/>
-      <c r="AF39" s="96"/>
-      <c r="AG39" s="96"/>
-      <c r="AH39" s="96"/>
-      <c r="AI39" s="96"/>
-      <c r="AJ39" s="96"/>
-      <c r="AK39" s="96"/>
-      <c r="AL39" s="96"/>
-      <c r="AM39" s="96"/>
-      <c r="AN39" s="96"/>
-      <c r="AO39" s="96"/>
-      <c r="AP39" s="96"/>
-      <c r="AQ39" s="96"/>
-      <c r="AR39" s="96"/>
-      <c r="AS39" s="96"/>
-      <c r="AT39" s="96"/>
-      <c r="AU39" s="96"/>
-      <c r="AV39" s="96"/>
-      <c r="AW39" s="96"/>
-      <c r="AX39" s="96"/>
-      <c r="AY39" s="96"/>
-      <c r="AZ39" s="96"/>
-      <c r="BA39" s="96"/>
-      <c r="BB39" s="96"/>
-      <c r="BC39" s="96"/>
-      <c r="BD39" s="96"/>
-      <c r="BE39" s="96"/>
-      <c r="BF39" s="96"/>
-      <c r="BG39" s="96"/>
-      <c r="BH39" s="96"/>
-      <c r="BI39" s="96"/>
-      <c r="BJ39" s="96"/>
-      <c r="BK39" s="96"/>
-      <c r="BL39" s="96"/>
-      <c r="BM39" s="96"/>
-      <c r="BN39" s="96"/>
-      <c r="BO39" s="96"/>
-      <c r="BP39" s="96"/>
-      <c r="BQ39" s="96"/>
-      <c r="BR39" s="96"/>
-      <c r="BS39" s="96"/>
-      <c r="BT39" s="96"/>
-      <c r="BU39" s="96"/>
-      <c r="BV39" s="96"/>
-      <c r="BW39" s="96"/>
-      <c r="BX39" s="96"/>
-      <c r="BY39" s="96"/>
-      <c r="BZ39" s="96"/>
-      <c r="CA39" s="96"/>
-      <c r="CB39" s="96"/>
-      <c r="CC39" s="96"/>
-      <c r="CD39" s="96"/>
-      <c r="CE39" s="96"/>
-      <c r="CF39" s="96"/>
-      <c r="CG39" s="96"/>
-      <c r="CH39" s="96"/>
-      <c r="CI39" s="96"/>
-      <c r="CJ39" s="96"/>
-      <c r="CK39" s="96"/>
-      <c r="CL39" s="96"/>
-      <c r="CM39" s="96"/>
-      <c r="CN39" s="96"/>
-      <c r="CO39" s="96"/>
-      <c r="CP39" s="96"/>
-      <c r="CQ39" s="96"/>
-      <c r="CR39" s="96"/>
-      <c r="CS39" s="96"/>
-      <c r="CT39" s="96"/>
-      <c r="CU39" s="96"/>
-      <c r="CV39" s="96"/>
-      <c r="CW39" s="96"/>
-      <c r="CX39" s="96"/>
-      <c r="CY39" s="96"/>
-      <c r="CZ39" s="96"/>
-      <c r="DA39" s="96"/>
-      <c r="DB39" s="96"/>
-      <c r="DC39" s="96"/>
-      <c r="DD39" s="96"/>
-      <c r="DE39" s="96"/>
-      <c r="DF39" s="96"/>
-      <c r="DG39" s="96"/>
-      <c r="DH39" s="96"/>
-      <c r="DI39" s="96"/>
-      <c r="DJ39" s="96"/>
-      <c r="DK39" s="96"/>
-      <c r="DL39" s="96"/>
-      <c r="DM39" s="96"/>
-      <c r="DN39" s="96"/>
-      <c r="DO39" s="96"/>
-      <c r="DP39" s="96"/>
-      <c r="DQ39" s="96"/>
-      <c r="DR39" s="96"/>
-      <c r="DS39" s="96"/>
-      <c r="DT39" s="96"/>
-      <c r="DU39" s="96"/>
-      <c r="DV39" s="96"/>
-      <c r="DW39" s="96"/>
+      <c r="B39" s="87"/>
+      <c r="C39" s="88"/>
+      <c r="D39" s="89"/>
+      <c r="E39" s="90"/>
+      <c r="F39" s="90"/>
+      <c r="G39" s="91"/>
+      <c r="H39" s="91"/>
+      <c r="I39" s="92"/>
+      <c r="J39" s="92"/>
+      <c r="K39" s="92"/>
+      <c r="L39" s="92"/>
+      <c r="M39" s="92"/>
+      <c r="N39" s="92"/>
+      <c r="O39" s="92"/>
+      <c r="P39" s="92"/>
+      <c r="Q39" s="92"/>
+      <c r="R39" s="92"/>
+      <c r="S39" s="92"/>
+      <c r="T39" s="92"/>
+      <c r="U39" s="92"/>
+      <c r="V39" s="92"/>
+      <c r="W39" s="92"/>
+      <c r="X39" s="92"/>
+      <c r="Y39" s="92"/>
+      <c r="Z39" s="92"/>
+      <c r="AA39" s="92"/>
+      <c r="AB39" s="92"/>
+      <c r="AC39" s="92"/>
+      <c r="AD39" s="92"/>
+      <c r="AE39" s="92"/>
+      <c r="AF39" s="92"/>
+      <c r="AG39" s="92"/>
+      <c r="AH39" s="92"/>
+      <c r="AI39" s="92"/>
+      <c r="AJ39" s="92"/>
+      <c r="AK39" s="92"/>
+      <c r="AL39" s="92"/>
+      <c r="AM39" s="92"/>
+      <c r="AN39" s="92"/>
+      <c r="AO39" s="92"/>
+      <c r="AP39" s="92"/>
+      <c r="AQ39" s="92"/>
+      <c r="AR39" s="92"/>
+      <c r="AS39" s="92"/>
+      <c r="AT39" s="92"/>
+      <c r="AU39" s="92"/>
+      <c r="AV39" s="92"/>
+      <c r="AW39" s="92"/>
+      <c r="AX39" s="92"/>
+      <c r="AY39" s="92"/>
+      <c r="AZ39" s="92"/>
+      <c r="BA39" s="92"/>
+      <c r="BB39" s="92"/>
+      <c r="BC39" s="92"/>
+      <c r="BD39" s="92"/>
+      <c r="BE39" s="92"/>
+      <c r="BF39" s="92"/>
+      <c r="BG39" s="92"/>
+      <c r="BH39" s="92"/>
+      <c r="BI39" s="92"/>
+      <c r="BJ39" s="92"/>
+      <c r="BK39" s="92"/>
+      <c r="BL39" s="92"/>
+      <c r="BM39" s="92"/>
+      <c r="BN39" s="92"/>
+      <c r="BO39" s="92"/>
+      <c r="BP39" s="92"/>
+      <c r="BQ39" s="92"/>
+      <c r="BR39" s="92"/>
+      <c r="BS39" s="92"/>
+      <c r="BT39" s="92"/>
+      <c r="BU39" s="92"/>
+      <c r="BV39" s="92"/>
+      <c r="BW39" s="92"/>
+      <c r="BX39" s="92"/>
+      <c r="BY39" s="92"/>
+      <c r="BZ39" s="92"/>
+      <c r="CA39" s="92"/>
+      <c r="CB39" s="92"/>
+      <c r="CC39" s="92"/>
+      <c r="CD39" s="92"/>
+      <c r="CE39" s="92"/>
+      <c r="CF39" s="92"/>
+      <c r="CG39" s="92"/>
+      <c r="CH39" s="92"/>
+      <c r="CI39" s="92"/>
+      <c r="CJ39" s="92"/>
+      <c r="CK39" s="92"/>
+      <c r="CL39" s="92"/>
+      <c r="CM39" s="92"/>
+      <c r="CN39" s="92"/>
+      <c r="CO39" s="92"/>
+      <c r="CP39" s="92"/>
+      <c r="CQ39" s="92"/>
+      <c r="CR39" s="92"/>
+      <c r="CS39" s="92"/>
+      <c r="CT39" s="92"/>
+      <c r="CU39" s="92"/>
+      <c r="CV39" s="92"/>
+      <c r="CW39" s="92"/>
+      <c r="CX39" s="92"/>
+      <c r="CY39" s="92"/>
+      <c r="CZ39" s="92"/>
+      <c r="DA39" s="92"/>
+      <c r="DB39" s="92"/>
+      <c r="DC39" s="92"/>
+      <c r="DD39" s="92"/>
+      <c r="DE39" s="92"/>
+      <c r="DF39" s="92"/>
+      <c r="DG39" s="92"/>
+      <c r="DH39" s="92"/>
+      <c r="DI39" s="92"/>
+      <c r="DJ39" s="92"/>
+      <c r="DK39" s="92"/>
+      <c r="DL39" s="92"/>
+      <c r="DM39" s="92"/>
+      <c r="DN39" s="92"/>
+      <c r="DO39" s="92"/>
+      <c r="DP39" s="92"/>
+      <c r="DQ39" s="92"/>
+      <c r="DR39" s="92"/>
+      <c r="DS39" s="92"/>
+      <c r="DT39" s="92"/>
+      <c r="DU39" s="92"/>
+      <c r="DV39" s="92"/>
+      <c r="DW39" s="92"/>
     </row>
     <row r="40" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="104"/>
-      <c r="C40" s="104"/>
-      <c r="D40" s="104"/>
-      <c r="E40" s="105"/>
-      <c r="F40" s="104"/>
-      <c r="G40" s="104"/>
-      <c r="H40" s="104"/>
-      <c r="I40" s="104"/>
-      <c r="J40" s="104"/>
-      <c r="K40" s="104"/>
-      <c r="L40" s="104"/>
-      <c r="M40" s="104"/>
-      <c r="N40" s="104"/>
-      <c r="O40" s="104"/>
-      <c r="P40" s="104"/>
-      <c r="Q40" s="104"/>
-      <c r="R40" s="104"/>
-      <c r="S40" s="104"/>
-      <c r="T40" s="104"/>
-      <c r="U40" s="104"/>
-      <c r="V40" s="104"/>
-      <c r="W40" s="104"/>
-      <c r="X40" s="104"/>
-      <c r="Y40" s="104"/>
-      <c r="Z40" s="104"/>
-      <c r="AA40" s="104"/>
-      <c r="AB40" s="104"/>
-      <c r="AC40" s="104"/>
-      <c r="AD40" s="104"/>
-      <c r="AE40" s="104"/>
-      <c r="AF40" s="104"/>
-      <c r="AG40" s="104"/>
-      <c r="AH40" s="104"/>
-      <c r="AI40" s="104"/>
-      <c r="AJ40" s="104"/>
-      <c r="AK40" s="104"/>
-      <c r="AL40" s="104"/>
-      <c r="AM40" s="104"/>
-      <c r="AN40" s="104"/>
-      <c r="AO40" s="104"/>
-      <c r="AP40" s="104"/>
-      <c r="AQ40" s="104"/>
-      <c r="AR40" s="104"/>
-      <c r="AS40" s="104"/>
-      <c r="AT40" s="104"/>
-      <c r="AU40" s="104"/>
-      <c r="AV40" s="104"/>
-      <c r="AW40" s="104"/>
-      <c r="AX40" s="104"/>
-      <c r="AY40" s="104"/>
-      <c r="AZ40" s="104"/>
-      <c r="BA40" s="104"/>
-      <c r="BB40" s="104"/>
-      <c r="BC40" s="104"/>
-      <c r="BD40" s="104"/>
-      <c r="BE40" s="104"/>
-      <c r="BF40" s="104"/>
-      <c r="BG40" s="104"/>
-      <c r="BH40" s="104"/>
-      <c r="BI40" s="104"/>
-      <c r="BJ40" s="104"/>
-      <c r="BK40" s="104"/>
-      <c r="BL40" s="104"/>
-      <c r="BM40" s="104"/>
-      <c r="BN40" s="104"/>
-      <c r="BO40" s="104"/>
-      <c r="BP40" s="104"/>
-      <c r="BQ40" s="104"/>
-      <c r="BR40" s="104"/>
-      <c r="BS40" s="104"/>
-      <c r="BT40" s="104"/>
-      <c r="BU40" s="104"/>
-      <c r="BV40" s="104"/>
-      <c r="BW40" s="104"/>
-      <c r="BX40" s="104"/>
-      <c r="BY40" s="104"/>
-      <c r="BZ40" s="104"/>
-      <c r="CA40" s="104"/>
-      <c r="CB40" s="104"/>
-      <c r="CC40" s="104"/>
-      <c r="CD40" s="104"/>
-      <c r="CE40" s="104"/>
-      <c r="CF40" s="104"/>
-      <c r="CG40" s="104"/>
-      <c r="CH40" s="104"/>
-      <c r="CI40" s="104"/>
-      <c r="CJ40" s="104"/>
-      <c r="CK40" s="104"/>
-      <c r="CL40" s="104"/>
-      <c r="CM40" s="104"/>
-      <c r="CN40" s="104"/>
-      <c r="CO40" s="104"/>
-      <c r="CP40" s="104"/>
-      <c r="CQ40" s="104"/>
-      <c r="CR40" s="104"/>
-      <c r="CS40" s="104"/>
-      <c r="CT40" s="104"/>
-      <c r="CU40" s="104"/>
-      <c r="CV40" s="104"/>
-      <c r="CW40" s="104"/>
-      <c r="CX40" s="104"/>
-      <c r="CY40" s="104"/>
-      <c r="CZ40" s="104"/>
-      <c r="DA40" s="104"/>
-      <c r="DB40" s="104"/>
-      <c r="DC40" s="104"/>
-      <c r="DD40" s="104"/>
-      <c r="DE40" s="104"/>
-      <c r="DF40" s="104"/>
-      <c r="DG40" s="104"/>
-      <c r="DH40" s="104"/>
-      <c r="DI40" s="104"/>
-      <c r="DJ40" s="104"/>
-      <c r="DK40" s="104"/>
-      <c r="DL40" s="104"/>
-      <c r="DM40" s="104"/>
-      <c r="DN40" s="104"/>
-      <c r="DO40" s="104"/>
-      <c r="DP40" s="104"/>
-      <c r="DQ40" s="104"/>
-      <c r="DR40" s="104"/>
-      <c r="DS40" s="104"/>
-      <c r="DT40" s="104"/>
-      <c r="DU40" s="104"/>
-      <c r="DV40" s="104"/>
-      <c r="DW40" s="104"/>
+      <c r="B40" s="100"/>
+      <c r="C40" s="100"/>
+      <c r="D40" s="100"/>
+      <c r="E40" s="101"/>
+      <c r="F40" s="100"/>
+      <c r="G40" s="100"/>
+      <c r="H40" s="100"/>
+      <c r="I40" s="100"/>
+      <c r="J40" s="100"/>
+      <c r="K40" s="100"/>
+      <c r="L40" s="100"/>
+      <c r="M40" s="100"/>
+      <c r="N40" s="100"/>
+      <c r="O40" s="100"/>
+      <c r="P40" s="100"/>
+      <c r="Q40" s="100"/>
+      <c r="R40" s="100"/>
+      <c r="S40" s="100"/>
+      <c r="T40" s="100"/>
+      <c r="U40" s="100"/>
+      <c r="V40" s="100"/>
+      <c r="W40" s="100"/>
+      <c r="X40" s="100"/>
+      <c r="Y40" s="100"/>
+      <c r="Z40" s="100"/>
+      <c r="AA40" s="100"/>
+      <c r="AB40" s="100"/>
+      <c r="AC40" s="100"/>
+      <c r="AD40" s="100"/>
+      <c r="AE40" s="100"/>
+      <c r="AF40" s="100"/>
+      <c r="AG40" s="100"/>
+      <c r="AH40" s="100"/>
+      <c r="AI40" s="100"/>
+      <c r="AJ40" s="100"/>
+      <c r="AK40" s="100"/>
+      <c r="AL40" s="100"/>
+      <c r="AM40" s="100"/>
+      <c r="AN40" s="100"/>
+      <c r="AO40" s="100"/>
+      <c r="AP40" s="100"/>
+      <c r="AQ40" s="100"/>
+      <c r="AR40" s="100"/>
+      <c r="AS40" s="100"/>
+      <c r="AT40" s="100"/>
+      <c r="AU40" s="100"/>
+      <c r="AV40" s="100"/>
+      <c r="AW40" s="100"/>
+      <c r="AX40" s="100"/>
+      <c r="AY40" s="100"/>
+      <c r="AZ40" s="100"/>
+      <c r="BA40" s="100"/>
+      <c r="BB40" s="100"/>
+      <c r="BC40" s="100"/>
+      <c r="BD40" s="100"/>
+      <c r="BE40" s="100"/>
+      <c r="BF40" s="100"/>
+      <c r="BG40" s="100"/>
+      <c r="BH40" s="100"/>
+      <c r="BI40" s="100"/>
+      <c r="BJ40" s="100"/>
+      <c r="BK40" s="100"/>
+      <c r="BL40" s="100"/>
+      <c r="BM40" s="100"/>
+      <c r="BN40" s="100"/>
+      <c r="BO40" s="100"/>
+      <c r="BP40" s="100"/>
+      <c r="BQ40" s="100"/>
+      <c r="BR40" s="100"/>
+      <c r="BS40" s="100"/>
+      <c r="BT40" s="100"/>
+      <c r="BU40" s="100"/>
+      <c r="BV40" s="100"/>
+      <c r="BW40" s="100"/>
+      <c r="BX40" s="100"/>
+      <c r="BY40" s="100"/>
+      <c r="BZ40" s="100"/>
+      <c r="CA40" s="100"/>
+      <c r="CB40" s="100"/>
+      <c r="CC40" s="100"/>
+      <c r="CD40" s="100"/>
+      <c r="CE40" s="100"/>
+      <c r="CF40" s="100"/>
+      <c r="CG40" s="100"/>
+      <c r="CH40" s="100"/>
+      <c r="CI40" s="100"/>
+      <c r="CJ40" s="100"/>
+      <c r="CK40" s="100"/>
+      <c r="CL40" s="100"/>
+      <c r="CM40" s="100"/>
+      <c r="CN40" s="100"/>
+      <c r="CO40" s="100"/>
+      <c r="CP40" s="100"/>
+      <c r="CQ40" s="100"/>
+      <c r="CR40" s="100"/>
+      <c r="CS40" s="100"/>
+      <c r="CT40" s="100"/>
+      <c r="CU40" s="100"/>
+      <c r="CV40" s="100"/>
+      <c r="CW40" s="100"/>
+      <c r="CX40" s="100"/>
+      <c r="CY40" s="100"/>
+      <c r="CZ40" s="100"/>
+      <c r="DA40" s="100"/>
+      <c r="DB40" s="100"/>
+      <c r="DC40" s="100"/>
+      <c r="DD40" s="100"/>
+      <c r="DE40" s="100"/>
+      <c r="DF40" s="100"/>
+      <c r="DG40" s="100"/>
+      <c r="DH40" s="100"/>
+      <c r="DI40" s="100"/>
+      <c r="DJ40" s="100"/>
+      <c r="DK40" s="100"/>
+      <c r="DL40" s="100"/>
+      <c r="DM40" s="100"/>
+      <c r="DN40" s="100"/>
+      <c r="DO40" s="100"/>
+      <c r="DP40" s="100"/>
+      <c r="DQ40" s="100"/>
+      <c r="DR40" s="100"/>
+      <c r="DS40" s="100"/>
+      <c r="DT40" s="100"/>
+      <c r="DU40" s="100"/>
+      <c r="DV40" s="100"/>
+      <c r="DW40" s="100"/>
     </row>
     <row r="42" spans="1:127" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="106"/>
+      <c r="B42" s="102"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="DQ4:DW4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="CV4:DB4"/>
-    <mergeCell ref="DC4:DI4"/>
-    <mergeCell ref="DJ4:DP4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B5:G5"/>
@@ -11262,11 +11295,12 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="DQ4:DW4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="CV4:DB4"/>
+    <mergeCell ref="DC4:DI4"/>
+    <mergeCell ref="DJ4:DP4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D27">
     <cfRule type="dataBar" priority="352">
@@ -12936,79 +12970,79 @@
     <row r="1" spans="1:2" ht="46.45" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:2" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="20"/>
     </row>
     <row r="3" spans="1:2" s="25" customFormat="1" ht="27.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="26"/>
     </row>
     <row r="4" spans="1:2" s="22" customFormat="1" ht="26.05" x14ac:dyDescent="0.5">
       <c r="A4" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="87" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="19" customFormat="1" ht="223.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="46" t="s">
-        <v>25</v>
+      <c r="A7" s="42" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="22" customFormat="1" ht="26.05" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="58.1" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="19" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="47" t="s">
-        <v>28</v>
+      <c r="A10" s="43" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="22" customFormat="1" ht="26.05" x14ac:dyDescent="0.5">
       <c r="A11" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="29.05" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="19" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="47" t="s">
-        <v>31</v>
+      <c r="A13" s="43" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="22" customFormat="1" ht="26.05" x14ac:dyDescent="0.5">
       <c r="A14" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="91.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="87.15" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Diagrama de Gantt modificado
</commit_message>
<xml_diff>
--- a/Análisis/Diagrama de Gantt.xlsx
+++ b/Análisis/Diagrama de Gantt.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE96778-2479-435D-AD59-B3ADACD99880}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAED2F5-26AC-401A-99CD-CE6D17A5292E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CalendarioProyecto" sheetId="11" r:id="rId1"/>
-    <sheet name="Acerca de" sheetId="12" r:id="rId2"/>
+    <sheet name="Portada" sheetId="12" r:id="rId1"/>
+    <sheet name="CalendarioProyecto" sheetId="11" r:id="rId2"/>
+    <sheet name="Acerca de" sheetId="14" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Display_Week">CalendarioProyecto!$E$4</definedName>
-    <definedName name="hoy" localSheetId="0">TODAY()</definedName>
+    <definedName name="hoy" localSheetId="1">TODAY()</definedName>
     <definedName name="Project_Start">CalendarioProyecto!$E$3</definedName>
-    <definedName name="task_end" localSheetId="0">CalendarioProyecto!$F1</definedName>
-    <definedName name="task_progress" localSheetId="0">CalendarioProyecto!$D1</definedName>
-    <definedName name="task_start" localSheetId="0">CalendarioProyecto!$E1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">CalendarioProyecto!$4:$6</definedName>
+    <definedName name="task_end" localSheetId="1">CalendarioProyecto!$F1</definedName>
+    <definedName name="task_progress" localSheetId="1">CalendarioProyecto!$D1</definedName>
+    <definedName name="task_start" localSheetId="1">CalendarioProyecto!$E1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">CalendarioProyecto!$4:$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
   <si>
     <t>Cree una programación para un proyecto en esta hoja de cálculo.
 Escriba el título de este proyecto en la celda B1. 
@@ -128,56 +129,6 @@
     <t>DÍAS</t>
   </si>
   <si>
-    <t>GRÁFICO GANTT SIMPLE de Vertex42.com</t>
-  </si>
-  <si>
-    <t>https://www.vertex42.com/ExcelTemplates/simple-gantt-chart.html</t>
-  </si>
-  <si>
-    <t>Información sobre esta plantilla</t>
-  </si>
-  <si>
-    <t>Esta plantilla proporciona una forma sencilla de crear un diagrama de Gantt para ayudarle a visualizar su proyecto y realizar un seguimiento de este. Simplemente escriba sus tareas y fechas de inicio y finalización, no necesita fórmulas. Las barras del gráfico de Gantt representan la duración de la tarea y se muestran con formato condicional. Para insertar nuevas tareas, inserte filas nuevas.</t>
-  </si>
-  <si>
-    <t>Guía para lectores de pantalla</t>
-  </si>
-  <si>
-    <t>Hay dos hojas de cálculo en este libro. 
-ProjectSchedule
-Acerca de
-Las instrucciones de las hojas de cálculo se encuentran en la columna A de cada hoja, a partir de la celda A1. Están escritas con texto oculto. Cada paso le guiará a través de la información de esa fila. Los pasos posteriores continúan en la celda A2, A3, y así sucesivamente, a menos que se indique de forma explícita. Por ejemplo, el texto de una instrucción podría ser “Vaya a la celda A6” para continuar con el siguiente paso. 
-Este texto oculto no se imprimirá.
-Para quitar las instrucciones de la hoja de cálculo, es suficiente con eliminar la columna A.</t>
-  </si>
-  <si>
-    <t>Ayuda adicional</t>
-  </si>
-  <si>
-    <t>Haga clic en el vínculo siguiente para visitar vertex42.com y obtener más información sobre cómo usar esta plantilla, como la forma de calcular los días laborales, crear dependencias de tareas, cambiar los colores de las barras, agregar una barra de desplazamiento para que sea más fácil cambiar la semana que se muestra, ampliar el intervalo de fechas que se muestran en el gráfico, etcétera.</t>
-  </si>
-  <si>
-    <t>Cómo usar el gráfico de Gantt simple</t>
-  </si>
-  <si>
-    <t>Más plantillas de administración de proyectos</t>
-  </si>
-  <si>
-    <t>Visite Vertex42.com para descargar otras plantillas de administración de proyectos, como distintas programaciones de proyectos, diagramas de Gantt, listas de tareas, etcétera.</t>
-  </si>
-  <si>
-    <t>Plantillas de administración de proyectos</t>
-  </si>
-  <si>
-    <t>Información sobre Vertex42</t>
-  </si>
-  <si>
-    <t>Vertex42.com ofrece más de 300 plantillas de hojas de cálculo de diseño profesional para empresas, hogares y centros educativos (la mayoría se puede descargar de forma gratuita). Su colección incluye una amplia variedad de calendarios, planificadores y programaciones, así como hojas de cálculo para las finanzas personales: para la administración de presupuestos, la reducción de deudas y la amortización de préstamos.</t>
-  </si>
-  <si>
-    <t>Las empresas encontrarán plantillas de facturas, partes de horas, informes financieros, planificación de proyectos y plantillas para hacer un seguimiento del inventario. Los profesores y los estudiantes encontrarán recursos como programaciones de clases, libros de calificaciones y hojas de asistencia. Organice su vida familiar con planificadores de comidas, listas y registros de ejercicio. Cada plantilla ha sido cuidadosamente diseñada, perfeccionada y mejorada a lo largo del tiempo gracias a los comentarios de miles de usuarios.</t>
-  </si>
-  <si>
     <t>La Semana para mostrar en la celda E4 representa la semana inicial para mostrar en la programación del proyecto en la celda I4. La fecha de inicio del proyecto se considera la semana 1. Para cambiar semana que se muestra, simplemente escriba un número de semana nuevo en la celda E4.
 La fecha de inicio de cada semana, comenzando por la Semana para mostrar en la celda E4, comienza en la celda I4 y se calcula automáticamente. Hay 8 semanas representadas en esta vista desde la celda I4 hasta la celda BF4.
 No debería modificar estas celdas.
@@ -264,6 +215,57 @@
   <si>
     <t>P</t>
   </si>
+  <si>
+    <t>Información sobre este diagrama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enlaces </t>
+  </si>
+  <si>
+    <t>Este diagrama proporciona el calendario del proceso de desarrollo de la aplicación web Uventos, la cual es una aplicación que ayudara a manejar mejor las organizaciones de los eventos en la facultad de negocios y tecnologias en el campus Ixtaczoquitlan desarrollada por Empresaurios</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD VERACRUZANA</t>
+  </si>
+  <si>
+    <t>FACULTAD DE NEGOCIOS Y TECNOLOGIAS</t>
+  </si>
+  <si>
+    <t>PROGRAMA EDUCATIVO</t>
+  </si>
+  <si>
+    <t>INGENIERÍA DE SOFTWARE</t>
+  </si>
+  <si>
+    <t>EXPERIENCIA EDUCATIVA</t>
+  </si>
+  <si>
+    <t>DESARROLLO DE SOFTWARE</t>
+  </si>
+  <si>
+    <t>INTEGRANTES DE EQUIPO</t>
+  </si>
+  <si>
+    <t>DIAZ TORRES ALDO FRANCISCO</t>
+  </si>
+  <si>
+    <t>NOLASCO ALVARADO DANIEL ANTONIO</t>
+  </si>
+  <si>
+    <t>ORTIZ HERNADEZ IBET</t>
+  </si>
+  <si>
+    <t>ROMERO REYES LUIS ANGEL</t>
+  </si>
+  <si>
+    <t>BLOQUE Y SECCIÓN</t>
+  </si>
+  <si>
+    <t>601-ISW</t>
+  </si>
+  <si>
+    <t>“DIAGRAMA DE GANTT”</t>
+  </si>
 </sst>
 </file>
 
@@ -280,7 +282,7 @@
     <numFmt numFmtId="171" formatCode="d"/>
     <numFmt numFmtId="172" formatCode="ddd\,\ d/m/yyyy"/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,6 +528,26 @@
       <name val="Wingdings 2"/>
       <family val="1"/>
       <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="49">
@@ -1112,7 +1134,7 @@
     <xf numFmtId="0" fontId="7" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1210,9 +1232,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="11" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="12" applyFill="1">
@@ -1417,6 +1436,12 @@
     <xf numFmtId="0" fontId="33" fillId="9" borderId="2" xfId="11" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="170" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1436,11 +1461,20 @@
     <xf numFmtId="172" fontId="7" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -5479,26 +5513,141 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>284309</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>64348</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectángulo 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48C6116D-E24F-46DA-AE95-DF90CB26D876}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="14499771" cy="648335"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rot="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" anchorCtr="0" upright="1">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>7684</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>122945</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>284308</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>18245</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectángulo 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7A24634-A5F2-47AF-8514-FEBB87BEC5AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7684" y="4779469"/>
+          <a:ext cx="15767636" cy="778964"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rot="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" anchorCtr="0" upright="1">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>192100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>92208</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1905000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>523875</xdr:rowOff>
+      <xdr:colOff>645459</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>147219</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1" descr="Logotipo de Vertex42">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        <xdr:cNvPr id="9" name="Imagen 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF4CDF2F-69B6-4A9F-BF78-24A04F843F19}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5507,7 +5656,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5520,8 +5669,215 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="190500" y="95250"/>
-          <a:ext cx="1905000" cy="428625"/>
+          <a:off x="192100" y="676195"/>
+          <a:ext cx="453359" cy="592893"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>183136</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>83244</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>6404</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>138255</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagen 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F02ADDBB-C09D-44DE-9ED9-5F3825649877}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13783875" y="667231"/>
+          <a:ext cx="453359" cy="592893"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1498388</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4787154</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>51201</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5B6E7E2-4C70-4F6C-B4D5-0B8C87F65153}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1498388" y="0"/>
+          <a:ext cx="3288766" cy="635188"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2168742</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1106501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9267B88-74FF-46E0-8BBD-BB3F3D97B05C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2520363"/>
+          <a:ext cx="2168742" cy="1106501"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2274474</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>124386</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3883852</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1029661</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDA5B2C7-965B-4F43-97E1-E1C0D23B9666}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2274474" y="2644749"/>
+          <a:ext cx="1609378" cy="905275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5795,14 +6151,118 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Hoja2">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.95" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="87.109375" style="19" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="2"/>
+    <col min="3" max="3" width="4.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.21875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="46.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:9" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+    </row>
+    <row r="3" spans="1:9" s="25" customFormat="1" ht="27.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3"/>
+      <c r="B3" s="26"/>
+    </row>
+    <row r="4" spans="1:9" s="22" customFormat="1" ht="26.05" x14ac:dyDescent="0.5">
+      <c r="C4" s="116" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="21.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="116" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="117"/>
+    </row>
+    <row r="7" spans="1:9" s="19" customFormat="1" ht="24.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="118" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="118" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="22" customFormat="1" ht="26.05" x14ac:dyDescent="0.5">
+      <c r="A8" s="116" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="116" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="24.85" x14ac:dyDescent="0.3">
+      <c r="C9" s="116" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="116" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="19" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="118" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="116" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="22" customFormat="1" ht="26.05" x14ac:dyDescent="0.5">
+      <c r="A11" s="116" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="116" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="19" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:9" s="22" customFormat="1" ht="26.05" x14ac:dyDescent="0.5">
+      <c r="I14" s="118" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I15" s="116" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <headerFooter differentFirst="1" scaleWithDoc="0">
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:EY41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
@@ -5880,7 +6340,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -5894,7 +6354,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="I2" s="29"/>
     </row>
@@ -5903,832 +6363,832 @@
         <v>2</v>
       </c>
       <c r="B3" s="33"/>
-      <c r="C3" s="109" t="s">
+      <c r="C3" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="110"/>
-      <c r="E3" s="112">
+      <c r="D3" s="111"/>
+      <c r="E3" s="113">
         <v>43892</v>
       </c>
-      <c r="F3" s="112"/>
+      <c r="F3" s="113"/>
     </row>
     <row r="4" spans="1:155" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="110"/>
+      <c r="D4" s="111"/>
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="106">
+      <c r="I4" s="107">
         <f>I5</f>
         <v>43892</v>
       </c>
-      <c r="J4" s="107"/>
-      <c r="K4" s="107"/>
-      <c r="L4" s="107"/>
-      <c r="M4" s="107"/>
-      <c r="N4" s="107"/>
-      <c r="O4" s="108"/>
-      <c r="P4" s="106">
+      <c r="J4" s="108"/>
+      <c r="K4" s="108"/>
+      <c r="L4" s="108"/>
+      <c r="M4" s="108"/>
+      <c r="N4" s="108"/>
+      <c r="O4" s="109"/>
+      <c r="P4" s="107">
         <f>P5</f>
         <v>43899</v>
       </c>
-      <c r="Q4" s="107"/>
-      <c r="R4" s="107"/>
-      <c r="S4" s="107"/>
-      <c r="T4" s="107"/>
-      <c r="U4" s="107"/>
-      <c r="V4" s="108"/>
-      <c r="W4" s="106">
+      <c r="Q4" s="108"/>
+      <c r="R4" s="108"/>
+      <c r="S4" s="108"/>
+      <c r="T4" s="108"/>
+      <c r="U4" s="108"/>
+      <c r="V4" s="109"/>
+      <c r="W4" s="107">
         <f>W5</f>
         <v>43906</v>
       </c>
-      <c r="X4" s="107"/>
-      <c r="Y4" s="107"/>
-      <c r="Z4" s="107"/>
-      <c r="AA4" s="107"/>
-      <c r="AB4" s="107"/>
-      <c r="AC4" s="108"/>
-      <c r="AD4" s="106">
+      <c r="X4" s="108"/>
+      <c r="Y4" s="108"/>
+      <c r="Z4" s="108"/>
+      <c r="AA4" s="108"/>
+      <c r="AB4" s="108"/>
+      <c r="AC4" s="109"/>
+      <c r="AD4" s="107">
         <f>AD5</f>
         <v>43913</v>
       </c>
-      <c r="AE4" s="107"/>
-      <c r="AF4" s="107"/>
-      <c r="AG4" s="107"/>
-      <c r="AH4" s="107"/>
-      <c r="AI4" s="107"/>
-      <c r="AJ4" s="108"/>
-      <c r="AK4" s="106">
+      <c r="AE4" s="108"/>
+      <c r="AF4" s="108"/>
+      <c r="AG4" s="108"/>
+      <c r="AH4" s="108"/>
+      <c r="AI4" s="108"/>
+      <c r="AJ4" s="109"/>
+      <c r="AK4" s="107">
         <f>AK5</f>
         <v>43920</v>
       </c>
-      <c r="AL4" s="107"/>
-      <c r="AM4" s="107"/>
-      <c r="AN4" s="107"/>
-      <c r="AO4" s="107"/>
-      <c r="AP4" s="107"/>
-      <c r="AQ4" s="108"/>
-      <c r="AR4" s="106">
+      <c r="AL4" s="108"/>
+      <c r="AM4" s="108"/>
+      <c r="AN4" s="108"/>
+      <c r="AO4" s="108"/>
+      <c r="AP4" s="108"/>
+      <c r="AQ4" s="109"/>
+      <c r="AR4" s="107">
         <f>AR5</f>
         <v>43927</v>
       </c>
-      <c r="AS4" s="107"/>
-      <c r="AT4" s="107"/>
-      <c r="AU4" s="107"/>
-      <c r="AV4" s="107"/>
-      <c r="AW4" s="107"/>
-      <c r="AX4" s="108"/>
-      <c r="AY4" s="106">
+      <c r="AS4" s="108"/>
+      <c r="AT4" s="108"/>
+      <c r="AU4" s="108"/>
+      <c r="AV4" s="108"/>
+      <c r="AW4" s="108"/>
+      <c r="AX4" s="109"/>
+      <c r="AY4" s="107">
         <f>AY5</f>
         <v>43934</v>
       </c>
-      <c r="AZ4" s="107"/>
-      <c r="BA4" s="107"/>
-      <c r="BB4" s="107"/>
-      <c r="BC4" s="107"/>
-      <c r="BD4" s="107"/>
-      <c r="BE4" s="108"/>
-      <c r="BF4" s="106">
+      <c r="AZ4" s="108"/>
+      <c r="BA4" s="108"/>
+      <c r="BB4" s="108"/>
+      <c r="BC4" s="108"/>
+      <c r="BD4" s="108"/>
+      <c r="BE4" s="109"/>
+      <c r="BF4" s="107">
         <f>BF5</f>
         <v>43941</v>
       </c>
-      <c r="BG4" s="107"/>
-      <c r="BH4" s="107"/>
-      <c r="BI4" s="107"/>
-      <c r="BJ4" s="107"/>
-      <c r="BK4" s="107"/>
-      <c r="BL4" s="108"/>
-      <c r="BM4" s="106">
+      <c r="BG4" s="108"/>
+      <c r="BH4" s="108"/>
+      <c r="BI4" s="108"/>
+      <c r="BJ4" s="108"/>
+      <c r="BK4" s="108"/>
+      <c r="BL4" s="109"/>
+      <c r="BM4" s="107">
         <f>BM5</f>
         <v>43948</v>
       </c>
-      <c r="BN4" s="107"/>
-      <c r="BO4" s="107"/>
-      <c r="BP4" s="107"/>
-      <c r="BQ4" s="107"/>
-      <c r="BR4" s="107"/>
-      <c r="BS4" s="108"/>
-      <c r="BT4" s="106">
+      <c r="BN4" s="108"/>
+      <c r="BO4" s="108"/>
+      <c r="BP4" s="108"/>
+      <c r="BQ4" s="108"/>
+      <c r="BR4" s="108"/>
+      <c r="BS4" s="109"/>
+      <c r="BT4" s="107">
         <f>BT5</f>
         <v>43955</v>
       </c>
-      <c r="BU4" s="107"/>
-      <c r="BV4" s="107"/>
-      <c r="BW4" s="107"/>
-      <c r="BX4" s="107"/>
-      <c r="BY4" s="107"/>
-      <c r="BZ4" s="108"/>
-      <c r="CA4" s="106">
+      <c r="BU4" s="108"/>
+      <c r="BV4" s="108"/>
+      <c r="BW4" s="108"/>
+      <c r="BX4" s="108"/>
+      <c r="BY4" s="108"/>
+      <c r="BZ4" s="109"/>
+      <c r="CA4" s="107">
         <f>CA5</f>
         <v>43962</v>
       </c>
-      <c r="CB4" s="107"/>
-      <c r="CC4" s="107"/>
-      <c r="CD4" s="107"/>
-      <c r="CE4" s="107"/>
-      <c r="CF4" s="107"/>
-      <c r="CG4" s="108"/>
-      <c r="CH4" s="106">
+      <c r="CB4" s="108"/>
+      <c r="CC4" s="108"/>
+      <c r="CD4" s="108"/>
+      <c r="CE4" s="108"/>
+      <c r="CF4" s="108"/>
+      <c r="CG4" s="109"/>
+      <c r="CH4" s="107">
         <f>CH5</f>
         <v>43969</v>
       </c>
-      <c r="CI4" s="107"/>
-      <c r="CJ4" s="107"/>
-      <c r="CK4" s="107"/>
-      <c r="CL4" s="107"/>
-      <c r="CM4" s="107"/>
-      <c r="CN4" s="108"/>
-      <c r="CO4" s="106">
+      <c r="CI4" s="108"/>
+      <c r="CJ4" s="108"/>
+      <c r="CK4" s="108"/>
+      <c r="CL4" s="108"/>
+      <c r="CM4" s="108"/>
+      <c r="CN4" s="109"/>
+      <c r="CO4" s="107">
         <f>CO5</f>
         <v>43976</v>
       </c>
-      <c r="CP4" s="107"/>
-      <c r="CQ4" s="107"/>
-      <c r="CR4" s="107"/>
-      <c r="CS4" s="107"/>
-      <c r="CT4" s="107"/>
-      <c r="CU4" s="108"/>
-      <c r="CV4" s="106">
+      <c r="CP4" s="108"/>
+      <c r="CQ4" s="108"/>
+      <c r="CR4" s="108"/>
+      <c r="CS4" s="108"/>
+      <c r="CT4" s="108"/>
+      <c r="CU4" s="109"/>
+      <c r="CV4" s="107">
         <f>CV5</f>
         <v>43983</v>
       </c>
-      <c r="CW4" s="107"/>
-      <c r="CX4" s="107"/>
-      <c r="CY4" s="107"/>
-      <c r="CZ4" s="107"/>
-      <c r="DA4" s="107"/>
-      <c r="DB4" s="108"/>
-      <c r="DC4" s="106">
+      <c r="CW4" s="108"/>
+      <c r="CX4" s="108"/>
+      <c r="CY4" s="108"/>
+      <c r="CZ4" s="108"/>
+      <c r="DA4" s="108"/>
+      <c r="DB4" s="109"/>
+      <c r="DC4" s="107">
         <f>DC5</f>
         <v>43990</v>
       </c>
-      <c r="DD4" s="107"/>
-      <c r="DE4" s="107"/>
-      <c r="DF4" s="107"/>
-      <c r="DG4" s="107"/>
-      <c r="DH4" s="107"/>
-      <c r="DI4" s="108"/>
-      <c r="DJ4" s="106">
+      <c r="DD4" s="108"/>
+      <c r="DE4" s="108"/>
+      <c r="DF4" s="108"/>
+      <c r="DG4" s="108"/>
+      <c r="DH4" s="108"/>
+      <c r="DI4" s="109"/>
+      <c r="DJ4" s="107">
         <f>DJ5</f>
         <v>43997</v>
       </c>
-      <c r="DK4" s="107"/>
-      <c r="DL4" s="107"/>
-      <c r="DM4" s="107"/>
-      <c r="DN4" s="107"/>
-      <c r="DO4" s="107"/>
-      <c r="DP4" s="108"/>
-      <c r="DQ4" s="106">
+      <c r="DK4" s="108"/>
+      <c r="DL4" s="108"/>
+      <c r="DM4" s="108"/>
+      <c r="DN4" s="108"/>
+      <c r="DO4" s="108"/>
+      <c r="DP4" s="109"/>
+      <c r="DQ4" s="107">
         <f>DQ5</f>
         <v>44004</v>
       </c>
-      <c r="DR4" s="107"/>
-      <c r="DS4" s="107"/>
-      <c r="DT4" s="107"/>
-      <c r="DU4" s="107"/>
-      <c r="DV4" s="107"/>
-      <c r="DW4" s="108"/>
-      <c r="DX4" s="106">
+      <c r="DR4" s="108"/>
+      <c r="DS4" s="108"/>
+      <c r="DT4" s="108"/>
+      <c r="DU4" s="108"/>
+      <c r="DV4" s="108"/>
+      <c r="DW4" s="109"/>
+      <c r="DX4" s="107">
         <f>DX5</f>
         <v>44011</v>
       </c>
-      <c r="DY4" s="107"/>
-      <c r="DZ4" s="107"/>
-      <c r="EA4" s="107"/>
-      <c r="EB4" s="107"/>
-      <c r="EC4" s="107"/>
-      <c r="ED4" s="108"/>
-      <c r="EE4" s="106">
+      <c r="DY4" s="108"/>
+      <c r="DZ4" s="108"/>
+      <c r="EA4" s="108"/>
+      <c r="EB4" s="108"/>
+      <c r="EC4" s="108"/>
+      <c r="ED4" s="109"/>
+      <c r="EE4" s="107">
         <f>EE5</f>
         <v>44018</v>
       </c>
-      <c r="EF4" s="107"/>
-      <c r="EG4" s="107"/>
-      <c r="EH4" s="107"/>
-      <c r="EI4" s="107"/>
-      <c r="EJ4" s="107"/>
-      <c r="EK4" s="108"/>
-      <c r="EL4" s="106">
+      <c r="EF4" s="108"/>
+      <c r="EG4" s="108"/>
+      <c r="EH4" s="108"/>
+      <c r="EI4" s="108"/>
+      <c r="EJ4" s="108"/>
+      <c r="EK4" s="109"/>
+      <c r="EL4" s="107">
         <f>EL5</f>
         <v>44025</v>
       </c>
-      <c r="EM4" s="107"/>
-      <c r="EN4" s="107"/>
-      <c r="EO4" s="107"/>
-      <c r="EP4" s="107"/>
-      <c r="EQ4" s="107"/>
-      <c r="ER4" s="108"/>
-      <c r="ES4" s="106">
+      <c r="EM4" s="108"/>
+      <c r="EN4" s="108"/>
+      <c r="EO4" s="108"/>
+      <c r="EP4" s="108"/>
+      <c r="EQ4" s="108"/>
+      <c r="ER4" s="109"/>
+      <c r="ES4" s="107">
         <f>ES5</f>
         <v>44032</v>
       </c>
-      <c r="ET4" s="107"/>
-      <c r="EU4" s="107"/>
-      <c r="EV4" s="107"/>
-      <c r="EW4" s="107"/>
-      <c r="EX4" s="107"/>
-      <c r="EY4" s="108"/>
+      <c r="ET4" s="108"/>
+      <c r="EU4" s="108"/>
+      <c r="EV4" s="108"/>
+      <c r="EW4" s="108"/>
+      <c r="EX4" s="108"/>
+      <c r="EY4" s="109"/>
     </row>
     <row r="5" spans="1:155" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="111"/>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
-      <c r="G5" s="111"/>
-      <c r="I5" s="44">
+      <c r="B5" s="112"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
+      <c r="I5" s="43">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43892</v>
       </c>
-      <c r="J5" s="45">
+      <c r="J5" s="44">
         <f>I5+1</f>
         <v>43893</v>
       </c>
-      <c r="K5" s="45">
+      <c r="K5" s="44">
         <f t="shared" ref="K5:AX5" si="0">J5+1</f>
         <v>43894</v>
       </c>
-      <c r="L5" s="45">
+      <c r="L5" s="44">
         <f t="shared" si="0"/>
         <v>43895</v>
       </c>
-      <c r="M5" s="45">
+      <c r="M5" s="44">
         <f t="shared" si="0"/>
         <v>43896</v>
       </c>
-      <c r="N5" s="45">
+      <c r="N5" s="44">
         <f t="shared" si="0"/>
         <v>43897</v>
       </c>
-      <c r="O5" s="46">
+      <c r="O5" s="45">
         <f t="shared" si="0"/>
         <v>43898</v>
       </c>
-      <c r="P5" s="44">
+      <c r="P5" s="43">
         <f>O5+1</f>
         <v>43899</v>
       </c>
-      <c r="Q5" s="45">
+      <c r="Q5" s="44">
         <f>P5+1</f>
         <v>43900</v>
       </c>
-      <c r="R5" s="45">
+      <c r="R5" s="44">
         <f t="shared" si="0"/>
         <v>43901</v>
       </c>
-      <c r="S5" s="45">
+      <c r="S5" s="44">
         <f t="shared" si="0"/>
         <v>43902</v>
       </c>
-      <c r="T5" s="45">
+      <c r="T5" s="44">
         <f t="shared" si="0"/>
         <v>43903</v>
       </c>
-      <c r="U5" s="45">
+      <c r="U5" s="44">
         <f t="shared" si="0"/>
         <v>43904</v>
       </c>
-      <c r="V5" s="46">
+      <c r="V5" s="45">
         <f t="shared" si="0"/>
         <v>43905</v>
       </c>
-      <c r="W5" s="44">
+      <c r="W5" s="43">
         <f>V5+1</f>
         <v>43906</v>
       </c>
-      <c r="X5" s="45">
+      <c r="X5" s="44">
         <f>W5+1</f>
         <v>43907</v>
       </c>
-      <c r="Y5" s="45">
+      <c r="Y5" s="44">
         <f t="shared" si="0"/>
         <v>43908</v>
       </c>
-      <c r="Z5" s="45">
+      <c r="Z5" s="44">
         <f t="shared" si="0"/>
         <v>43909</v>
       </c>
-      <c r="AA5" s="45">
+      <c r="AA5" s="44">
         <f t="shared" si="0"/>
         <v>43910</v>
       </c>
-      <c r="AB5" s="45">
+      <c r="AB5" s="44">
         <f t="shared" si="0"/>
         <v>43911</v>
       </c>
-      <c r="AC5" s="46">
+      <c r="AC5" s="45">
         <f t="shared" si="0"/>
         <v>43912</v>
       </c>
-      <c r="AD5" s="44">
+      <c r="AD5" s="43">
         <f>AC5+1</f>
         <v>43913</v>
       </c>
-      <c r="AE5" s="45">
+      <c r="AE5" s="44">
         <f>AD5+1</f>
         <v>43914</v>
       </c>
-      <c r="AF5" s="45">
+      <c r="AF5" s="44">
         <f t="shared" si="0"/>
         <v>43915</v>
       </c>
-      <c r="AG5" s="45">
+      <c r="AG5" s="44">
         <f t="shared" si="0"/>
         <v>43916</v>
       </c>
-      <c r="AH5" s="45">
+      <c r="AH5" s="44">
         <f t="shared" si="0"/>
         <v>43917</v>
       </c>
-      <c r="AI5" s="45">
+      <c r="AI5" s="44">
         <f t="shared" si="0"/>
         <v>43918</v>
       </c>
-      <c r="AJ5" s="46">
+      <c r="AJ5" s="45">
         <f t="shared" si="0"/>
         <v>43919</v>
       </c>
-      <c r="AK5" s="44">
+      <c r="AK5" s="43">
         <f>AJ5+1</f>
         <v>43920</v>
       </c>
-      <c r="AL5" s="45">
+      <c r="AL5" s="44">
         <f>AK5+1</f>
         <v>43921</v>
       </c>
-      <c r="AM5" s="45">
+      <c r="AM5" s="44">
         <f t="shared" si="0"/>
         <v>43922</v>
       </c>
-      <c r="AN5" s="45">
+      <c r="AN5" s="44">
         <f t="shared" si="0"/>
         <v>43923</v>
       </c>
-      <c r="AO5" s="45">
+      <c r="AO5" s="44">
         <f t="shared" si="0"/>
         <v>43924</v>
       </c>
-      <c r="AP5" s="45">
+      <c r="AP5" s="44">
         <f t="shared" si="0"/>
         <v>43925</v>
       </c>
-      <c r="AQ5" s="46">
+      <c r="AQ5" s="45">
         <f t="shared" si="0"/>
         <v>43926</v>
       </c>
-      <c r="AR5" s="44">
+      <c r="AR5" s="43">
         <f>AQ5+1</f>
         <v>43927</v>
       </c>
-      <c r="AS5" s="45">
+      <c r="AS5" s="44">
         <f>AR5+1</f>
         <v>43928</v>
       </c>
-      <c r="AT5" s="45">
+      <c r="AT5" s="44">
         <f t="shared" si="0"/>
         <v>43929</v>
       </c>
-      <c r="AU5" s="45">
+      <c r="AU5" s="44">
         <f t="shared" si="0"/>
         <v>43930</v>
       </c>
-      <c r="AV5" s="45">
+      <c r="AV5" s="44">
         <f t="shared" si="0"/>
         <v>43931</v>
       </c>
-      <c r="AW5" s="45">
+      <c r="AW5" s="44">
         <f t="shared" si="0"/>
         <v>43932</v>
       </c>
-      <c r="AX5" s="46">
+      <c r="AX5" s="45">
         <f t="shared" si="0"/>
         <v>43933</v>
       </c>
-      <c r="AY5" s="44">
+      <c r="AY5" s="43">
         <f>AX5+1</f>
         <v>43934</v>
       </c>
-      <c r="AZ5" s="45">
+      <c r="AZ5" s="44">
         <f>AY5+1</f>
         <v>43935</v>
       </c>
-      <c r="BA5" s="45">
+      <c r="BA5" s="44">
         <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
         <v>43936</v>
       </c>
-      <c r="BB5" s="45">
+      <c r="BB5" s="44">
         <f t="shared" si="1"/>
         <v>43937</v>
       </c>
-      <c r="BC5" s="45">
+      <c r="BC5" s="44">
         <f t="shared" si="1"/>
         <v>43938</v>
       </c>
-      <c r="BD5" s="45">
+      <c r="BD5" s="44">
         <f t="shared" si="1"/>
         <v>43939</v>
       </c>
-      <c r="BE5" s="46">
+      <c r="BE5" s="45">
         <f t="shared" si="1"/>
         <v>43940</v>
       </c>
-      <c r="BF5" s="44">
+      <c r="BF5" s="43">
         <f>BE5+1</f>
         <v>43941</v>
       </c>
-      <c r="BG5" s="45">
+      <c r="BG5" s="44">
         <f>BF5+1</f>
         <v>43942</v>
       </c>
-      <c r="BH5" s="45">
+      <c r="BH5" s="44">
         <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
         <v>43943</v>
       </c>
-      <c r="BI5" s="45">
+      <c r="BI5" s="44">
         <f t="shared" si="2"/>
         <v>43944</v>
       </c>
-      <c r="BJ5" s="45">
+      <c r="BJ5" s="44">
         <f t="shared" si="2"/>
         <v>43945</v>
       </c>
-      <c r="BK5" s="45">
+      <c r="BK5" s="44">
         <f t="shared" si="2"/>
         <v>43946</v>
       </c>
-      <c r="BL5" s="46">
+      <c r="BL5" s="45">
         <f t="shared" si="2"/>
         <v>43947</v>
       </c>
-      <c r="BM5" s="44">
+      <c r="BM5" s="43">
         <f>BL5+1</f>
         <v>43948</v>
       </c>
-      <c r="BN5" s="45">
+      <c r="BN5" s="44">
         <f>BM5+1</f>
         <v>43949</v>
       </c>
-      <c r="BO5" s="45">
+      <c r="BO5" s="44">
         <f t="shared" ref="BO5" si="3">BN5+1</f>
         <v>43950</v>
       </c>
-      <c r="BP5" s="45">
+      <c r="BP5" s="44">
         <f t="shared" ref="BP5" si="4">BO5+1</f>
         <v>43951</v>
       </c>
-      <c r="BQ5" s="45">
+      <c r="BQ5" s="44">
         <f t="shared" ref="BQ5" si="5">BP5+1</f>
         <v>43952</v>
       </c>
-      <c r="BR5" s="45">
+      <c r="BR5" s="44">
         <f t="shared" ref="BR5" si="6">BQ5+1</f>
         <v>43953</v>
       </c>
-      <c r="BS5" s="46">
+      <c r="BS5" s="45">
         <f t="shared" ref="BS5" si="7">BR5+1</f>
         <v>43954</v>
       </c>
-      <c r="BT5" s="44">
+      <c r="BT5" s="43">
         <f>BS5+1</f>
         <v>43955</v>
       </c>
-      <c r="BU5" s="45">
+      <c r="BU5" s="44">
         <f>BT5+1</f>
         <v>43956</v>
       </c>
-      <c r="BV5" s="45">
+      <c r="BV5" s="44">
         <f t="shared" ref="BV5" si="8">BU5+1</f>
         <v>43957</v>
       </c>
-      <c r="BW5" s="45">
+      <c r="BW5" s="44">
         <f t="shared" ref="BW5" si="9">BV5+1</f>
         <v>43958</v>
       </c>
-      <c r="BX5" s="45">
+      <c r="BX5" s="44">
         <f t="shared" ref="BX5" si="10">BW5+1</f>
         <v>43959</v>
       </c>
-      <c r="BY5" s="45">
+      <c r="BY5" s="44">
         <f t="shared" ref="BY5" si="11">BX5+1</f>
         <v>43960</v>
       </c>
-      <c r="BZ5" s="46">
+      <c r="BZ5" s="45">
         <f t="shared" ref="BZ5" si="12">BY5+1</f>
         <v>43961</v>
       </c>
-      <c r="CA5" s="44">
+      <c r="CA5" s="43">
         <f>BZ5+1</f>
         <v>43962</v>
       </c>
-      <c r="CB5" s="45">
+      <c r="CB5" s="44">
         <f>CA5+1</f>
         <v>43963</v>
       </c>
-      <c r="CC5" s="45">
+      <c r="CC5" s="44">
         <f t="shared" ref="CC5" si="13">CB5+1</f>
         <v>43964</v>
       </c>
-      <c r="CD5" s="45">
+      <c r="CD5" s="44">
         <f t="shared" ref="CD5" si="14">CC5+1</f>
         <v>43965</v>
       </c>
-      <c r="CE5" s="45">
+      <c r="CE5" s="44">
         <f t="shared" ref="CE5" si="15">CD5+1</f>
         <v>43966</v>
       </c>
-      <c r="CF5" s="45">
+      <c r="CF5" s="44">
         <f t="shared" ref="CF5" si="16">CE5+1</f>
         <v>43967</v>
       </c>
-      <c r="CG5" s="46">
+      <c r="CG5" s="45">
         <f t="shared" ref="CG5" si="17">CF5+1</f>
         <v>43968</v>
       </c>
-      <c r="CH5" s="44">
+      <c r="CH5" s="43">
         <f>CG5+1</f>
         <v>43969</v>
       </c>
-      <c r="CI5" s="45">
+      <c r="CI5" s="44">
         <f>CH5+1</f>
         <v>43970</v>
       </c>
-      <c r="CJ5" s="45">
+      <c r="CJ5" s="44">
         <f t="shared" ref="CJ5" si="18">CI5+1</f>
         <v>43971</v>
       </c>
-      <c r="CK5" s="45">
+      <c r="CK5" s="44">
         <f t="shared" ref="CK5" si="19">CJ5+1</f>
         <v>43972</v>
       </c>
-      <c r="CL5" s="45">
+      <c r="CL5" s="44">
         <f t="shared" ref="CL5" si="20">CK5+1</f>
         <v>43973</v>
       </c>
-      <c r="CM5" s="45">
+      <c r="CM5" s="44">
         <f t="shared" ref="CM5" si="21">CL5+1</f>
         <v>43974</v>
       </c>
-      <c r="CN5" s="46">
+      <c r="CN5" s="45">
         <f t="shared" ref="CN5" si="22">CM5+1</f>
         <v>43975</v>
       </c>
-      <c r="CO5" s="44">
+      <c r="CO5" s="43">
         <f>CN5+1</f>
         <v>43976</v>
       </c>
-      <c r="CP5" s="45">
+      <c r="CP5" s="44">
         <f>CO5+1</f>
         <v>43977</v>
       </c>
-      <c r="CQ5" s="45">
+      <c r="CQ5" s="44">
         <f t="shared" ref="CQ5" si="23">CP5+1</f>
         <v>43978</v>
       </c>
-      <c r="CR5" s="45">
+      <c r="CR5" s="44">
         <f t="shared" ref="CR5" si="24">CQ5+1</f>
         <v>43979</v>
       </c>
-      <c r="CS5" s="45">
+      <c r="CS5" s="44">
         <f t="shared" ref="CS5" si="25">CR5+1</f>
         <v>43980</v>
       </c>
-      <c r="CT5" s="45">
+      <c r="CT5" s="44">
         <f t="shared" ref="CT5" si="26">CS5+1</f>
         <v>43981</v>
       </c>
-      <c r="CU5" s="46">
+      <c r="CU5" s="45">
         <f t="shared" ref="CU5" si="27">CT5+1</f>
         <v>43982</v>
       </c>
-      <c r="CV5" s="44">
+      <c r="CV5" s="43">
         <f>CU5+1</f>
         <v>43983</v>
       </c>
-      <c r="CW5" s="45">
+      <c r="CW5" s="44">
         <f>CV5+1</f>
         <v>43984</v>
       </c>
-      <c r="CX5" s="45">
+      <c r="CX5" s="44">
         <f t="shared" ref="CX5" si="28">CW5+1</f>
         <v>43985</v>
       </c>
-      <c r="CY5" s="45">
+      <c r="CY5" s="44">
         <f t="shared" ref="CY5" si="29">CX5+1</f>
         <v>43986</v>
       </c>
-      <c r="CZ5" s="45">
+      <c r="CZ5" s="44">
         <f t="shared" ref="CZ5" si="30">CY5+1</f>
         <v>43987</v>
       </c>
-      <c r="DA5" s="45">
+      <c r="DA5" s="44">
         <f t="shared" ref="DA5" si="31">CZ5+1</f>
         <v>43988</v>
       </c>
-      <c r="DB5" s="46">
+      <c r="DB5" s="45">
         <f t="shared" ref="DB5" si="32">DA5+1</f>
         <v>43989</v>
       </c>
-      <c r="DC5" s="44">
+      <c r="DC5" s="43">
         <f>DB5+1</f>
         <v>43990</v>
       </c>
-      <c r="DD5" s="45">
+      <c r="DD5" s="44">
         <f>DC5+1</f>
         <v>43991</v>
       </c>
-      <c r="DE5" s="45">
+      <c r="DE5" s="44">
         <f t="shared" ref="DE5" si="33">DD5+1</f>
         <v>43992</v>
       </c>
-      <c r="DF5" s="45">
+      <c r="DF5" s="44">
         <f t="shared" ref="DF5" si="34">DE5+1</f>
         <v>43993</v>
       </c>
-      <c r="DG5" s="45">
+      <c r="DG5" s="44">
         <f t="shared" ref="DG5" si="35">DF5+1</f>
         <v>43994</v>
       </c>
-      <c r="DH5" s="45">
+      <c r="DH5" s="44">
         <f t="shared" ref="DH5" si="36">DG5+1</f>
         <v>43995</v>
       </c>
-      <c r="DI5" s="46">
+      <c r="DI5" s="45">
         <f t="shared" ref="DI5" si="37">DH5+1</f>
         <v>43996</v>
       </c>
-      <c r="DJ5" s="44">
+      <c r="DJ5" s="43">
         <f>DI5+1</f>
         <v>43997</v>
       </c>
-      <c r="DK5" s="45">
+      <c r="DK5" s="44">
         <f>DJ5+1</f>
         <v>43998</v>
       </c>
-      <c r="DL5" s="45">
+      <c r="DL5" s="44">
         <f t="shared" ref="DL5" si="38">DK5+1</f>
         <v>43999</v>
       </c>
-      <c r="DM5" s="45">
+      <c r="DM5" s="44">
         <f t="shared" ref="DM5" si="39">DL5+1</f>
         <v>44000</v>
       </c>
-      <c r="DN5" s="45">
+      <c r="DN5" s="44">
         <f t="shared" ref="DN5" si="40">DM5+1</f>
         <v>44001</v>
       </c>
-      <c r="DO5" s="45">
+      <c r="DO5" s="44">
         <f t="shared" ref="DO5" si="41">DN5+1</f>
         <v>44002</v>
       </c>
-      <c r="DP5" s="46">
+      <c r="DP5" s="45">
         <f t="shared" ref="DP5" si="42">DO5+1</f>
         <v>44003</v>
       </c>
-      <c r="DQ5" s="44">
+      <c r="DQ5" s="43">
         <f>DP5+1</f>
         <v>44004</v>
       </c>
-      <c r="DR5" s="45">
+      <c r="DR5" s="44">
         <f>DQ5+1</f>
         <v>44005</v>
       </c>
-      <c r="DS5" s="45">
+      <c r="DS5" s="44">
         <f t="shared" ref="DS5" si="43">DR5+1</f>
         <v>44006</v>
       </c>
-      <c r="DT5" s="45">
+      <c r="DT5" s="44">
         <f t="shared" ref="DT5" si="44">DS5+1</f>
         <v>44007</v>
       </c>
-      <c r="DU5" s="45">
+      <c r="DU5" s="44">
         <f t="shared" ref="DU5" si="45">DT5+1</f>
         <v>44008</v>
       </c>
-      <c r="DV5" s="45">
+      <c r="DV5" s="44">
         <f t="shared" ref="DV5" si="46">DU5+1</f>
         <v>44009</v>
       </c>
-      <c r="DW5" s="46">
+      <c r="DW5" s="45">
         <f t="shared" ref="DW5" si="47">DV5+1</f>
         <v>44010</v>
       </c>
-      <c r="DX5" s="44">
+      <c r="DX5" s="43">
         <f>DW5+1</f>
         <v>44011</v>
       </c>
-      <c r="DY5" s="45">
+      <c r="DY5" s="44">
         <f>DX5+1</f>
         <v>44012</v>
       </c>
-      <c r="DZ5" s="45">
+      <c r="DZ5" s="44">
         <f t="shared" ref="DZ5" si="48">DY5+1</f>
         <v>44013</v>
       </c>
-      <c r="EA5" s="45">
+      <c r="EA5" s="44">
         <f t="shared" ref="EA5" si="49">DZ5+1</f>
         <v>44014</v>
       </c>
-      <c r="EB5" s="45">
+      <c r="EB5" s="44">
         <f t="shared" ref="EB5" si="50">EA5+1</f>
         <v>44015</v>
       </c>
-      <c r="EC5" s="45">
+      <c r="EC5" s="44">
         <f t="shared" ref="EC5" si="51">EB5+1</f>
         <v>44016</v>
       </c>
-      <c r="ED5" s="46">
+      <c r="ED5" s="45">
         <f t="shared" ref="ED5" si="52">EC5+1</f>
         <v>44017</v>
       </c>
-      <c r="EE5" s="44">
+      <c r="EE5" s="43">
         <f>ED5+1</f>
         <v>44018</v>
       </c>
-      <c r="EF5" s="45">
+      <c r="EF5" s="44">
         <f>EE5+1</f>
         <v>44019</v>
       </c>
-      <c r="EG5" s="45">
+      <c r="EG5" s="44">
         <f t="shared" ref="EG5" si="53">EF5+1</f>
         <v>44020</v>
       </c>
-      <c r="EH5" s="45">
+      <c r="EH5" s="44">
         <f t="shared" ref="EH5" si="54">EG5+1</f>
         <v>44021</v>
       </c>
-      <c r="EI5" s="45">
+      <c r="EI5" s="44">
         <f t="shared" ref="EI5" si="55">EH5+1</f>
         <v>44022</v>
       </c>
-      <c r="EJ5" s="45">
+      <c r="EJ5" s="44">
         <f t="shared" ref="EJ5" si="56">EI5+1</f>
         <v>44023</v>
       </c>
-      <c r="EK5" s="46">
+      <c r="EK5" s="45">
         <f t="shared" ref="EK5" si="57">EJ5+1</f>
         <v>44024</v>
       </c>
-      <c r="EL5" s="44">
+      <c r="EL5" s="43">
         <f>EK5+1</f>
         <v>44025</v>
       </c>
-      <c r="EM5" s="45">
+      <c r="EM5" s="44">
         <f>EL5+1</f>
         <v>44026</v>
       </c>
-      <c r="EN5" s="45">
+      <c r="EN5" s="44">
         <f t="shared" ref="EN5" si="58">EM5+1</f>
         <v>44027</v>
       </c>
-      <c r="EO5" s="45">
+      <c r="EO5" s="44">
         <f t="shared" ref="EO5" si="59">EN5+1</f>
         <v>44028</v>
       </c>
-      <c r="EP5" s="45">
+      <c r="EP5" s="44">
         <f t="shared" ref="EP5" si="60">EO5+1</f>
         <v>44029</v>
       </c>
-      <c r="EQ5" s="45">
+      <c r="EQ5" s="44">
         <f t="shared" ref="EQ5" si="61">EP5+1</f>
         <v>44030</v>
       </c>
-      <c r="ER5" s="46">
+      <c r="ER5" s="45">
         <f t="shared" ref="ER5" si="62">EQ5+1</f>
         <v>44031</v>
       </c>
-      <c r="ES5" s="44">
+      <c r="ES5" s="43">
         <f>ER5+1</f>
         <v>44032</v>
       </c>
-      <c r="ET5" s="45">
+      <c r="ET5" s="44">
         <f>ES5+1</f>
         <v>44033</v>
       </c>
-      <c r="EU5" s="45">
+      <c r="EU5" s="44">
         <f t="shared" ref="EU5" si="63">ET5+1</f>
         <v>44034</v>
       </c>
-      <c r="EV5" s="45">
+      <c r="EV5" s="44">
         <f t="shared" ref="EV5" si="64">EU5+1</f>
         <v>44035</v>
       </c>
-      <c r="EW5" s="45">
+      <c r="EW5" s="44">
         <f t="shared" ref="EW5" si="65">EV5+1</f>
         <v>44036</v>
       </c>
-      <c r="EX5" s="45">
+      <c r="EX5" s="44">
         <f t="shared" ref="EX5" si="66">EW5+1</f>
         <v>44037</v>
       </c>
-      <c r="EY5" s="46">
+      <c r="EY5" s="45">
         <f t="shared" ref="EY5" si="67">EX5+1</f>
         <v>44038</v>
       </c>
@@ -6741,7 +7201,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
@@ -7506,12 +7966,12 @@
         <v>6</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="101"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="56"/>
+        <v>21</v>
+      </c>
+      <c r="C8" s="100"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="55"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11" t="str">
         <f t="shared" ref="H8:H33" si="75">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
@@ -7669,18 +8129,18 @@
       <c r="A9" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="102" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="57">
+      <c r="B9" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="101" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="47"/>
+      <c r="E9" s="56">
         <f>Project_Start</f>
         <v>43892</v>
       </c>
-      <c r="F9" s="57">
+      <c r="F9" s="56">
         <f>E9+7</f>
         <v>43899</v>
       </c>
@@ -7842,12 +8302,12 @@
         <v>8</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C10" s="34"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="59"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="58"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11" t="str">
         <f t="shared" si="75"/>
@@ -8003,18 +8463,18 @@
     </row>
     <row r="11" spans="1:155" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="27"/>
-      <c r="B11" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="103" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="60">
+      <c r="B11" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="102" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="49"/>
+      <c r="E11" s="59">
         <f>F9</f>
         <v>43899</v>
       </c>
-      <c r="F11" s="60">
+      <c r="F11" s="59">
         <f>E11+4</f>
         <v>43903</v>
       </c>
@@ -8173,17 +8633,17 @@
     </row>
     <row r="12" spans="1:155" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="27"/>
-      <c r="B12" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="103" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="60">
+      <c r="B12" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="102" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="49"/>
+      <c r="E12" s="59">
         <v>43899</v>
       </c>
-      <c r="F12" s="60">
+      <c r="F12" s="59">
         <v>43899</v>
       </c>
       <c r="G12" s="11"/>
@@ -8342,12 +8802,12 @@
     <row r="13" spans="1:155" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="27"/>
       <c r="B13" s="14" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C13" s="35"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="62"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="61"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11" t="str">
         <f t="shared" si="75"/>
@@ -8505,17 +8965,17 @@
       <c r="A14" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="104" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="52"/>
-      <c r="E14" s="63">
+      <c r="B14" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="103" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="51"/>
+      <c r="E14" s="62">
         <v>43913</v>
       </c>
-      <c r="F14" s="63">
+      <c r="F14" s="62">
         <v>43918</v>
       </c>
       <c r="G14" s="11"/>
@@ -8673,17 +9133,17 @@
     </row>
     <row r="15" spans="1:155" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="28"/>
-      <c r="B15" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="104" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="52"/>
-      <c r="E15" s="63">
+      <c r="B15" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="103" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="51"/>
+      <c r="E15" s="62">
         <v>43913</v>
       </c>
-      <c r="F15" s="63">
+      <c r="F15" s="62">
         <v>43918</v>
       </c>
       <c r="G15" s="11"/>
@@ -8841,17 +9301,17 @@
     </row>
     <row r="16" spans="1:155" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="27"/>
-      <c r="B16" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="104" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="52"/>
-      <c r="E16" s="63">
+      <c r="B16" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="103" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="51"/>
+      <c r="E16" s="62">
         <v>43913</v>
       </c>
-      <c r="F16" s="63">
+      <c r="F16" s="62">
         <v>43918</v>
       </c>
       <c r="G16" s="11"/>
@@ -9009,17 +9469,17 @@
     </row>
     <row r="17" spans="1:155" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="27"/>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="104" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="52"/>
-      <c r="E17" s="63">
+      <c r="D17" s="51"/>
+      <c r="E17" s="62">
         <v>43919</v>
       </c>
-      <c r="F17" s="63">
+      <c r="F17" s="62">
         <v>43922</v>
       </c>
       <c r="G17" s="11"/>
@@ -9177,17 +9637,17 @@
     </row>
     <row r="18" spans="1:155" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="27"/>
-      <c r="B18" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="104" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="52"/>
-      <c r="E18" s="63">
+      <c r="B18" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="103" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="51"/>
+      <c r="E18" s="62">
         <v>43919</v>
       </c>
-      <c r="F18" s="63">
+      <c r="F18" s="62">
         <v>43922</v>
       </c>
       <c r="G18" s="11"/>
@@ -9346,12 +9806,12 @@
     <row r="19" spans="1:155" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="27"/>
       <c r="B19" s="15" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C19" s="36"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="65"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="64"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11" t="str">
         <f t="shared" si="75"/>
@@ -9509,17 +9969,17 @@
       <c r="A20" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="105" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="54"/>
-      <c r="E20" s="66">
+      <c r="B20" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="104" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="53"/>
+      <c r="E20" s="65">
         <v>43941</v>
       </c>
-      <c r="F20" s="66">
+      <c r="F20" s="65">
         <v>43942</v>
       </c>
       <c r="G20" s="11"/>
@@ -9677,17 +10137,17 @@
     </row>
     <row r="21" spans="1:155" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="27"/>
-      <c r="B21" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="105" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="54"/>
-      <c r="E21" s="66">
+      <c r="B21" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="104" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="53"/>
+      <c r="E21" s="65">
         <v>43926</v>
       </c>
-      <c r="F21" s="66">
+      <c r="F21" s="65">
         <v>43933</v>
       </c>
       <c r="G21" s="11"/>
@@ -9845,17 +10305,17 @@
     </row>
     <row r="22" spans="1:155" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="27"/>
-      <c r="B22" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="105" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="54"/>
-      <c r="E22" s="66">
+      <c r="B22" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="104" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="53"/>
+      <c r="E22" s="65">
         <v>43952</v>
       </c>
-      <c r="F22" s="66">
+      <c r="F22" s="65">
         <v>43968</v>
       </c>
       <c r="G22" s="11"/>
@@ -10013,17 +10473,17 @@
     </row>
     <row r="23" spans="1:155" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="27"/>
-      <c r="B23" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="105" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="54"/>
-      <c r="E23" s="66">
+      <c r="B23" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="104" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="53"/>
+      <c r="E23" s="65">
         <v>43926</v>
       </c>
-      <c r="F23" s="66">
+      <c r="F23" s="65">
         <v>43931</v>
       </c>
       <c r="G23" s="11"/>
@@ -10181,16 +10641,18 @@
     </row>
     <row r="24" spans="1:155" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="27"/>
-      <c r="B24" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="66">
+      <c r="B24" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="104" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="53"/>
+      <c r="E24" s="65">
         <f>E22</f>
         <v>43952</v>
       </c>
-      <c r="F24" s="66">
+      <c r="F24" s="65">
         <v>44000</v>
       </c>
       <c r="G24" s="11"/>
@@ -10348,15 +10810,17 @@
     </row>
     <row r="25" spans="1:155" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="27"/>
-      <c r="B25" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="37"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="66">
+      <c r="B25" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="104" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="53"/>
+      <c r="E25" s="65">
         <v>43941</v>
       </c>
-      <c r="F25" s="66">
+      <c r="F25" s="65">
         <v>44002</v>
       </c>
       <c r="G25" s="11"/>
@@ -10516,13 +10980,13 @@
       <c r="A26" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="67" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="68"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="71"/>
+      <c r="B26" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="67"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="70"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11" t="str">
         <f t="shared" si="75"/>
@@ -10678,15 +11142,15 @@
     </row>
     <row r="27" spans="1:155" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="27"/>
-      <c r="B27" s="72" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="73"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="75">
+      <c r="B27" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="72"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="74">
         <v>44007</v>
       </c>
-      <c r="F27" s="75">
+      <c r="F27" s="74">
         <f>E27</f>
         <v>44007</v>
       </c>
@@ -10845,15 +11309,15 @@
     </row>
     <row r="28" spans="1:155" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="27"/>
-      <c r="B28" s="72" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="73"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="75">
+      <c r="B28" s="71" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="72"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="74">
         <v>44007</v>
       </c>
-      <c r="F28" s="75">
+      <c r="F28" s="74">
         <v>44015</v>
       </c>
       <c r="G28" s="11"/>
@@ -11011,15 +11475,15 @@
     </row>
     <row r="29" spans="1:155" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="27"/>
-      <c r="B29" s="72" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="73"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="75">
+      <c r="B29" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="72"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="74">
         <v>44007</v>
       </c>
-      <c r="F29" s="75">
+      <c r="F29" s="74">
         <v>44011</v>
       </c>
       <c r="G29" s="11"/>
@@ -11177,15 +11641,15 @@
     </row>
     <row r="30" spans="1:155" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="27"/>
-      <c r="B30" s="72" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="73"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="75">
+      <c r="B30" s="71" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="72"/>
+      <c r="D30" s="73"/>
+      <c r="E30" s="74">
         <v>44007</v>
       </c>
-      <c r="F30" s="75">
+      <c r="F30" s="74">
         <v>44013</v>
       </c>
       <c r="G30" s="11"/>
@@ -11343,15 +11807,15 @@
     </row>
     <row r="31" spans="1:155" s="3" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="27"/>
-      <c r="B31" s="72" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="73"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="75">
+      <c r="B31" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="72"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="74">
         <v>44007</v>
       </c>
-      <c r="F31" s="75">
+      <c r="F31" s="74">
         <v>44015</v>
       </c>
       <c r="G31" s="11"/>
@@ -11511,13 +11975,13 @@
       <c r="A32" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="76" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="77"/>
-      <c r="D32" s="78"/>
-      <c r="E32" s="79"/>
-      <c r="F32" s="80"/>
+      <c r="B32" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="76"/>
+      <c r="D32" s="77"/>
+      <c r="E32" s="78"/>
+      <c r="F32" s="79"/>
       <c r="G32" s="11"/>
       <c r="H32" s="11" t="str">
         <f t="shared" si="75"/>
@@ -11675,948 +12139,943 @@
       <c r="A33" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="81" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" s="82"/>
-      <c r="D33" s="83"/>
-      <c r="E33" s="84">
-        <v>44018</v>
-      </c>
-      <c r="F33" s="84">
-        <v>44018</v>
-      </c>
-      <c r="G33" s="113"/>
-      <c r="H33" s="113">
+      <c r="B33" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="81"/>
+      <c r="D33" s="82"/>
+      <c r="E33" s="83">
+        <v>44032</v>
+      </c>
+      <c r="F33" s="83">
+        <v>44032</v>
+      </c>
+      <c r="G33" s="105"/>
+      <c r="H33" s="105">
         <f t="shared" si="75"/>
         <v>1</v>
       </c>
-      <c r="I33" s="114"/>
-      <c r="J33" s="114"/>
-      <c r="K33" s="114"/>
-      <c r="L33" s="114"/>
-      <c r="M33" s="114"/>
-      <c r="N33" s="114"/>
-      <c r="O33" s="114"/>
-      <c r="P33" s="114"/>
-      <c r="Q33" s="114"/>
-      <c r="R33" s="114"/>
-      <c r="S33" s="114"/>
-      <c r="T33" s="114"/>
-      <c r="U33" s="114"/>
-      <c r="V33" s="114"/>
-      <c r="W33" s="114"/>
-      <c r="X33" s="114"/>
-      <c r="Y33" s="114"/>
-      <c r="Z33" s="114"/>
-      <c r="AA33" s="114"/>
-      <c r="AB33" s="114"/>
-      <c r="AC33" s="114"/>
-      <c r="AD33" s="114"/>
-      <c r="AE33" s="114"/>
-      <c r="AF33" s="114"/>
-      <c r="AG33" s="114"/>
-      <c r="AH33" s="114"/>
-      <c r="AI33" s="114"/>
-      <c r="AJ33" s="114"/>
-      <c r="AK33" s="114"/>
-      <c r="AL33" s="114"/>
-      <c r="AM33" s="114"/>
-      <c r="AN33" s="114"/>
-      <c r="AO33" s="114"/>
-      <c r="AP33" s="114"/>
-      <c r="AQ33" s="114"/>
-      <c r="AR33" s="114"/>
-      <c r="AS33" s="114"/>
-      <c r="AT33" s="114"/>
-      <c r="AU33" s="114"/>
-      <c r="AV33" s="114"/>
-      <c r="AW33" s="114"/>
-      <c r="AX33" s="114"/>
-      <c r="AY33" s="114"/>
-      <c r="AZ33" s="114"/>
-      <c r="BA33" s="114"/>
-      <c r="BB33" s="114"/>
-      <c r="BC33" s="114"/>
-      <c r="BD33" s="114"/>
-      <c r="BE33" s="114"/>
-      <c r="BF33" s="114"/>
-      <c r="BG33" s="114"/>
-      <c r="BH33" s="114"/>
-      <c r="BI33" s="114"/>
-      <c r="BJ33" s="114"/>
-      <c r="BK33" s="114"/>
-      <c r="BL33" s="114"/>
-      <c r="BM33" s="114"/>
-      <c r="BN33" s="114"/>
-      <c r="BO33" s="114"/>
-      <c r="BP33" s="114"/>
-      <c r="BQ33" s="114"/>
-      <c r="BR33" s="114"/>
-      <c r="BS33" s="114"/>
-      <c r="BT33" s="114"/>
-      <c r="BU33" s="114"/>
-      <c r="BV33" s="114"/>
-      <c r="BW33" s="114"/>
-      <c r="BX33" s="114"/>
-      <c r="BY33" s="114"/>
-      <c r="BZ33" s="114"/>
-      <c r="CA33" s="114"/>
-      <c r="CB33" s="114"/>
-      <c r="CC33" s="114"/>
-      <c r="CD33" s="114"/>
-      <c r="CE33" s="114"/>
-      <c r="CF33" s="114"/>
-      <c r="CG33" s="114"/>
-      <c r="CH33" s="114"/>
-      <c r="CI33" s="114"/>
-      <c r="CJ33" s="114"/>
-      <c r="CK33" s="114"/>
-      <c r="CL33" s="114"/>
-      <c r="CM33" s="114"/>
-      <c r="CN33" s="114"/>
-      <c r="CO33" s="114"/>
-      <c r="CP33" s="114"/>
-      <c r="CQ33" s="114"/>
-      <c r="CR33" s="114"/>
-      <c r="CS33" s="114"/>
-      <c r="CT33" s="114"/>
-      <c r="CU33" s="114"/>
-      <c r="CV33" s="114"/>
-      <c r="CW33" s="114"/>
-      <c r="CX33" s="114"/>
-      <c r="CY33" s="114"/>
-      <c r="CZ33" s="114"/>
-      <c r="DA33" s="114"/>
-      <c r="DB33" s="114"/>
-      <c r="DC33" s="114"/>
-      <c r="DD33" s="114"/>
-      <c r="DE33" s="114"/>
-      <c r="DF33" s="114"/>
-      <c r="DG33" s="114"/>
-      <c r="DH33" s="114"/>
-      <c r="DI33" s="114"/>
-      <c r="DJ33" s="114"/>
-      <c r="DK33" s="114"/>
-      <c r="DL33" s="114"/>
-      <c r="DM33" s="114"/>
-      <c r="DN33" s="114"/>
-      <c r="DO33" s="114"/>
-      <c r="DP33" s="114"/>
-      <c r="DQ33" s="114"/>
-      <c r="DR33" s="114"/>
-      <c r="DS33" s="114"/>
-      <c r="DT33" s="114"/>
-      <c r="DU33" s="114"/>
-      <c r="DV33" s="114"/>
-      <c r="DW33" s="114"/>
-      <c r="DX33" s="114"/>
-      <c r="DY33" s="114"/>
-      <c r="DZ33" s="114"/>
-      <c r="EA33" s="114"/>
-      <c r="EB33" s="114"/>
-      <c r="EC33" s="114"/>
-      <c r="ED33" s="114"/>
-      <c r="EE33" s="114"/>
-      <c r="EF33" s="114"/>
-      <c r="EG33" s="114"/>
-      <c r="EH33" s="114"/>
-      <c r="EI33" s="114"/>
-      <c r="EJ33" s="114"/>
-      <c r="EK33" s="114"/>
-      <c r="EL33" s="114"/>
-      <c r="EM33" s="114"/>
-      <c r="EN33" s="114"/>
-      <c r="EO33" s="114"/>
-      <c r="EP33" s="114"/>
-      <c r="EQ33" s="114"/>
-      <c r="ER33" s="114"/>
-      <c r="ES33" s="114"/>
-      <c r="ET33" s="114"/>
-      <c r="EU33" s="114"/>
-      <c r="EV33" s="114"/>
-      <c r="EW33" s="114"/>
-      <c r="EX33" s="114"/>
-      <c r="EY33" s="114"/>
+      <c r="I33" s="106"/>
+      <c r="J33" s="106"/>
+      <c r="K33" s="106"/>
+      <c r="L33" s="106"/>
+      <c r="M33" s="106"/>
+      <c r="N33" s="106"/>
+      <c r="O33" s="106"/>
+      <c r="P33" s="106"/>
+      <c r="Q33" s="106"/>
+      <c r="R33" s="106"/>
+      <c r="S33" s="106"/>
+      <c r="T33" s="106"/>
+      <c r="U33" s="106"/>
+      <c r="V33" s="106"/>
+      <c r="W33" s="106"/>
+      <c r="X33" s="106"/>
+      <c r="Y33" s="106"/>
+      <c r="Z33" s="106"/>
+      <c r="AA33" s="106"/>
+      <c r="AB33" s="106"/>
+      <c r="AC33" s="106"/>
+      <c r="AD33" s="106"/>
+      <c r="AE33" s="106"/>
+      <c r="AF33" s="106"/>
+      <c r="AG33" s="106"/>
+      <c r="AH33" s="106"/>
+      <c r="AI33" s="106"/>
+      <c r="AJ33" s="106"/>
+      <c r="AK33" s="106"/>
+      <c r="AL33" s="106"/>
+      <c r="AM33" s="106"/>
+      <c r="AN33" s="106"/>
+      <c r="AO33" s="106"/>
+      <c r="AP33" s="106"/>
+      <c r="AQ33" s="106"/>
+      <c r="AR33" s="106"/>
+      <c r="AS33" s="106"/>
+      <c r="AT33" s="106"/>
+      <c r="AU33" s="106"/>
+      <c r="AV33" s="106"/>
+      <c r="AW33" s="106"/>
+      <c r="AX33" s="106"/>
+      <c r="AY33" s="106"/>
+      <c r="AZ33" s="106"/>
+      <c r="BA33" s="106"/>
+      <c r="BB33" s="106"/>
+      <c r="BC33" s="106"/>
+      <c r="BD33" s="106"/>
+      <c r="BE33" s="106"/>
+      <c r="BF33" s="106"/>
+      <c r="BG33" s="106"/>
+      <c r="BH33" s="106"/>
+      <c r="BI33" s="106"/>
+      <c r="BJ33" s="106"/>
+      <c r="BK33" s="106"/>
+      <c r="BL33" s="106"/>
+      <c r="BM33" s="106"/>
+      <c r="BN33" s="106"/>
+      <c r="BO33" s="106"/>
+      <c r="BP33" s="106"/>
+      <c r="BQ33" s="106"/>
+      <c r="BR33" s="106"/>
+      <c r="BS33" s="106"/>
+      <c r="BT33" s="106"/>
+      <c r="BU33" s="106"/>
+      <c r="BV33" s="106"/>
+      <c r="BW33" s="106"/>
+      <c r="BX33" s="106"/>
+      <c r="BY33" s="106"/>
+      <c r="BZ33" s="106"/>
+      <c r="CA33" s="106"/>
+      <c r="CB33" s="106"/>
+      <c r="CC33" s="106"/>
+      <c r="CD33" s="106"/>
+      <c r="CE33" s="106"/>
+      <c r="CF33" s="106"/>
+      <c r="CG33" s="106"/>
+      <c r="CH33" s="106"/>
+      <c r="CI33" s="106"/>
+      <c r="CJ33" s="106"/>
+      <c r="CK33" s="106"/>
+      <c r="CL33" s="106"/>
+      <c r="CM33" s="106"/>
+      <c r="CN33" s="106"/>
+      <c r="CO33" s="106"/>
+      <c r="CP33" s="106"/>
+      <c r="CQ33" s="106"/>
+      <c r="CR33" s="106"/>
+      <c r="CS33" s="106"/>
+      <c r="CT33" s="106"/>
+      <c r="CU33" s="106"/>
+      <c r="CV33" s="106"/>
+      <c r="CW33" s="106"/>
+      <c r="CX33" s="106"/>
+      <c r="CY33" s="106"/>
+      <c r="CZ33" s="106"/>
+      <c r="DA33" s="106"/>
+      <c r="DB33" s="106"/>
+      <c r="DC33" s="106"/>
+      <c r="DD33" s="106"/>
+      <c r="DE33" s="106"/>
+      <c r="DF33" s="106"/>
+      <c r="DG33" s="106"/>
+      <c r="DH33" s="106"/>
+      <c r="DI33" s="106"/>
+      <c r="DJ33" s="106"/>
+      <c r="DK33" s="106"/>
+      <c r="DL33" s="106"/>
+      <c r="DM33" s="106"/>
+      <c r="DN33" s="106"/>
+      <c r="DO33" s="106"/>
+      <c r="DP33" s="106"/>
+      <c r="DQ33" s="106"/>
+      <c r="DR33" s="106"/>
+      <c r="DS33" s="106"/>
+      <c r="DT33" s="106"/>
+      <c r="DU33" s="106"/>
+      <c r="DV33" s="106"/>
+      <c r="DW33" s="106"/>
+      <c r="DX33" s="106"/>
+      <c r="DY33" s="106"/>
+      <c r="DZ33" s="106"/>
+      <c r="EA33" s="106"/>
+      <c r="EB33" s="106"/>
+      <c r="EC33" s="106"/>
+      <c r="ED33" s="106"/>
+      <c r="EE33" s="106"/>
+      <c r="EF33" s="106"/>
+      <c r="EG33" s="106"/>
+      <c r="EH33" s="106"/>
+      <c r="EI33" s="106"/>
+      <c r="EJ33" s="106"/>
+      <c r="EK33" s="106"/>
+      <c r="EL33" s="106"/>
+      <c r="EM33" s="106"/>
+      <c r="EN33" s="106"/>
+      <c r="EO33" s="106"/>
+      <c r="EP33" s="106"/>
+      <c r="EQ33" s="106"/>
+      <c r="ER33" s="106"/>
+      <c r="ES33" s="106"/>
+      <c r="ET33" s="106"/>
+      <c r="EU33" s="106"/>
+      <c r="EV33" s="106"/>
+      <c r="EW33" s="106"/>
+      <c r="EX33" s="106"/>
+      <c r="EY33" s="106"/>
     </row>
     <row r="34" spans="1:155" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="91"/>
-      <c r="C34" s="92"/>
-      <c r="D34" s="93"/>
-      <c r="E34" s="94"/>
-      <c r="F34" s="94"/>
-      <c r="G34" s="89"/>
-      <c r="H34" s="89"/>
-      <c r="I34" s="90"/>
-      <c r="J34" s="90"/>
-      <c r="K34" s="90"/>
-      <c r="L34" s="90"/>
-      <c r="M34" s="90"/>
-      <c r="N34" s="90"/>
-      <c r="O34" s="90"/>
-      <c r="P34" s="90"/>
-      <c r="Q34" s="90"/>
-      <c r="R34" s="90"/>
-      <c r="S34" s="90"/>
-      <c r="T34" s="90"/>
-      <c r="U34" s="90"/>
-      <c r="V34" s="90"/>
-      <c r="W34" s="90"/>
-      <c r="X34" s="90"/>
-      <c r="Y34" s="90"/>
-      <c r="Z34" s="90"/>
-      <c r="AA34" s="90"/>
-      <c r="AB34" s="90"/>
-      <c r="AC34" s="90"/>
-      <c r="AD34" s="90"/>
-      <c r="AE34" s="90"/>
-      <c r="AF34" s="90"/>
-      <c r="AG34" s="90"/>
-      <c r="AH34" s="90"/>
-      <c r="AI34" s="90"/>
-      <c r="AJ34" s="90"/>
-      <c r="AK34" s="90"/>
-      <c r="AL34" s="90"/>
-      <c r="AM34" s="90"/>
-      <c r="AN34" s="90"/>
-      <c r="AO34" s="90"/>
-      <c r="AP34" s="90"/>
-      <c r="AQ34" s="90"/>
-      <c r="AR34" s="90"/>
-      <c r="AS34" s="90"/>
-      <c r="AT34" s="90"/>
-      <c r="AU34" s="90"/>
-      <c r="AV34" s="90"/>
-      <c r="AW34" s="90"/>
-      <c r="AX34" s="90"/>
-      <c r="AY34" s="90"/>
-      <c r="AZ34" s="90"/>
-      <c r="BA34" s="90"/>
-      <c r="BB34" s="90"/>
-      <c r="BC34" s="90"/>
-      <c r="BD34" s="90"/>
-      <c r="BE34" s="90"/>
-      <c r="BF34" s="90"/>
-      <c r="BG34" s="90"/>
-      <c r="BH34" s="90"/>
-      <c r="BI34" s="90"/>
-      <c r="BJ34" s="90"/>
-      <c r="BK34" s="90"/>
-      <c r="BL34" s="90"/>
-      <c r="BM34" s="90"/>
-      <c r="BN34" s="90"/>
-      <c r="BO34" s="90"/>
-      <c r="BP34" s="90"/>
-      <c r="BQ34" s="90"/>
-      <c r="BR34" s="90"/>
-      <c r="BS34" s="90"/>
-      <c r="BT34" s="90"/>
-      <c r="BU34" s="90"/>
-      <c r="BV34" s="90"/>
-      <c r="BW34" s="90"/>
-      <c r="BX34" s="90"/>
-      <c r="BY34" s="90"/>
-      <c r="BZ34" s="90"/>
-      <c r="CA34" s="90"/>
-      <c r="CB34" s="90"/>
-      <c r="CC34" s="90"/>
-      <c r="CD34" s="90"/>
-      <c r="CE34" s="90"/>
-      <c r="CF34" s="90"/>
-      <c r="CG34" s="90"/>
-      <c r="CH34" s="90"/>
-      <c r="CI34" s="90"/>
-      <c r="CJ34" s="90"/>
-      <c r="CK34" s="90"/>
-      <c r="CL34" s="90"/>
-      <c r="CM34" s="90"/>
-      <c r="CN34" s="90"/>
-      <c r="CO34" s="90"/>
-      <c r="CP34" s="90"/>
-      <c r="CQ34" s="90"/>
-      <c r="CR34" s="90"/>
-      <c r="CS34" s="90"/>
-      <c r="CT34" s="90"/>
-      <c r="CU34" s="90"/>
-      <c r="CV34" s="90"/>
-      <c r="CW34" s="90"/>
-      <c r="CX34" s="90"/>
-      <c r="CY34" s="90"/>
-      <c r="CZ34" s="90"/>
-      <c r="DA34" s="90"/>
-      <c r="DB34" s="90"/>
-      <c r="DC34" s="90"/>
-      <c r="DD34" s="90"/>
-      <c r="DE34" s="90"/>
-      <c r="DF34" s="90"/>
-      <c r="DG34" s="90"/>
-      <c r="DH34" s="90"/>
-      <c r="DI34" s="90"/>
-      <c r="DJ34" s="90"/>
-      <c r="DK34" s="90"/>
-      <c r="DL34" s="90"/>
-      <c r="DM34" s="90"/>
-      <c r="DN34" s="90"/>
-      <c r="DO34" s="90"/>
-      <c r="DP34" s="90"/>
-      <c r="DQ34" s="90"/>
-      <c r="DR34" s="90"/>
-      <c r="DS34" s="90"/>
-      <c r="DT34" s="90"/>
-      <c r="DU34" s="90"/>
-      <c r="DV34" s="90"/>
+      <c r="B34" s="90"/>
+      <c r="C34" s="91"/>
+      <c r="D34" s="92"/>
+      <c r="E34" s="93"/>
+      <c r="F34" s="93"/>
+      <c r="G34" s="88"/>
+      <c r="H34" s="88"/>
+      <c r="I34" s="89"/>
+      <c r="J34" s="89"/>
+      <c r="K34" s="89"/>
+      <c r="L34" s="89"/>
+      <c r="M34" s="89"/>
+      <c r="N34" s="89"/>
+      <c r="O34" s="89"/>
+      <c r="P34" s="89"/>
+      <c r="Q34" s="89"/>
+      <c r="R34" s="89"/>
+      <c r="S34" s="89"/>
+      <c r="T34" s="89"/>
+      <c r="U34" s="89"/>
+      <c r="V34" s="89"/>
+      <c r="W34" s="89"/>
+      <c r="X34" s="89"/>
+      <c r="Y34" s="89"/>
+      <c r="Z34" s="89"/>
+      <c r="AA34" s="89"/>
+      <c r="AB34" s="89"/>
+      <c r="AC34" s="89"/>
+      <c r="AD34" s="89"/>
+      <c r="AE34" s="89"/>
+      <c r="AF34" s="89"/>
+      <c r="AG34" s="89"/>
+      <c r="AH34" s="89"/>
+      <c r="AI34" s="89"/>
+      <c r="AJ34" s="89"/>
+      <c r="AK34" s="89"/>
+      <c r="AL34" s="89"/>
+      <c r="AM34" s="89"/>
+      <c r="AN34" s="89"/>
+      <c r="AO34" s="89"/>
+      <c r="AP34" s="89"/>
+      <c r="AQ34" s="89"/>
+      <c r="AR34" s="89"/>
+      <c r="AS34" s="89"/>
+      <c r="AT34" s="89"/>
+      <c r="AU34" s="89"/>
+      <c r="AV34" s="89"/>
+      <c r="AW34" s="89"/>
+      <c r="AX34" s="89"/>
+      <c r="AY34" s="89"/>
+      <c r="AZ34" s="89"/>
+      <c r="BA34" s="89"/>
+      <c r="BB34" s="89"/>
+      <c r="BC34" s="89"/>
+      <c r="BD34" s="89"/>
+      <c r="BE34" s="89"/>
+      <c r="BF34" s="89"/>
+      <c r="BG34" s="89"/>
+      <c r="BH34" s="89"/>
+      <c r="BI34" s="89"/>
+      <c r="BJ34" s="89"/>
+      <c r="BK34" s="89"/>
+      <c r="BL34" s="89"/>
+      <c r="BM34" s="89"/>
+      <c r="BN34" s="89"/>
+      <c r="BO34" s="89"/>
+      <c r="BP34" s="89"/>
+      <c r="BQ34" s="89"/>
+      <c r="BR34" s="89"/>
+      <c r="BS34" s="89"/>
+      <c r="BT34" s="89"/>
+      <c r="BU34" s="89"/>
+      <c r="BV34" s="89"/>
+      <c r="BW34" s="89"/>
+      <c r="BX34" s="89"/>
+      <c r="BY34" s="89"/>
+      <c r="BZ34" s="89"/>
+      <c r="CA34" s="89"/>
+      <c r="CB34" s="89"/>
+      <c r="CC34" s="89"/>
+      <c r="CD34" s="89"/>
+      <c r="CE34" s="89"/>
+      <c r="CF34" s="89"/>
+      <c r="CG34" s="89"/>
+      <c r="CH34" s="89"/>
+      <c r="CI34" s="89"/>
+      <c r="CJ34" s="89"/>
+      <c r="CK34" s="89"/>
+      <c r="CL34" s="89"/>
+      <c r="CM34" s="89"/>
+      <c r="CN34" s="89"/>
+      <c r="CO34" s="89"/>
+      <c r="CP34" s="89"/>
+      <c r="CQ34" s="89"/>
+      <c r="CR34" s="89"/>
+      <c r="CS34" s="89"/>
+      <c r="CT34" s="89"/>
+      <c r="CU34" s="89"/>
+      <c r="CV34" s="89"/>
+      <c r="CW34" s="89"/>
+      <c r="CX34" s="89"/>
+      <c r="CY34" s="89"/>
+      <c r="CZ34" s="89"/>
+      <c r="DA34" s="89"/>
+      <c r="DB34" s="89"/>
+      <c r="DC34" s="89"/>
+      <c r="DD34" s="89"/>
+      <c r="DE34" s="89"/>
+      <c r="DF34" s="89"/>
+      <c r="DG34" s="89"/>
+      <c r="DH34" s="89"/>
+      <c r="DI34" s="89"/>
+      <c r="DJ34" s="89"/>
+      <c r="DK34" s="89"/>
+      <c r="DL34" s="89"/>
+      <c r="DM34" s="89"/>
+      <c r="DN34" s="89"/>
+      <c r="DO34" s="89"/>
+      <c r="DP34" s="89"/>
+      <c r="DQ34" s="89"/>
+      <c r="DR34" s="89"/>
+      <c r="DS34" s="89"/>
+      <c r="DT34" s="89"/>
+      <c r="DU34" s="89"/>
+      <c r="DV34" s="89"/>
     </row>
     <row r="35" spans="1:155" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="95"/>
-      <c r="C35" s="86"/>
-      <c r="D35" s="87"/>
-      <c r="E35" s="96"/>
-      <c r="F35" s="97"/>
-      <c r="G35" s="89"/>
-      <c r="H35" s="89"/>
-      <c r="I35" s="90"/>
-      <c r="J35" s="90"/>
-      <c r="K35" s="90"/>
-      <c r="L35" s="90"/>
-      <c r="M35" s="90"/>
-      <c r="N35" s="90"/>
-      <c r="O35" s="90"/>
-      <c r="P35" s="90"/>
-      <c r="Q35" s="90"/>
-      <c r="R35" s="90"/>
-      <c r="S35" s="90"/>
-      <c r="T35" s="90"/>
-      <c r="U35" s="90"/>
-      <c r="V35" s="90"/>
-      <c r="W35" s="90"/>
-      <c r="X35" s="90"/>
-      <c r="Y35" s="90"/>
-      <c r="Z35" s="90"/>
-      <c r="AA35" s="90"/>
-      <c r="AB35" s="90"/>
-      <c r="AC35" s="90"/>
-      <c r="AD35" s="90"/>
-      <c r="AE35" s="90"/>
-      <c r="AF35" s="90"/>
-      <c r="AG35" s="90"/>
-      <c r="AH35" s="90"/>
-      <c r="AI35" s="90"/>
-      <c r="AJ35" s="90"/>
-      <c r="AK35" s="90"/>
-      <c r="AL35" s="90"/>
-      <c r="AM35" s="90"/>
-      <c r="AN35" s="90"/>
-      <c r="AO35" s="90"/>
-      <c r="AP35" s="90"/>
-      <c r="AQ35" s="90"/>
-      <c r="AR35" s="90"/>
-      <c r="AS35" s="90"/>
-      <c r="AT35" s="90"/>
-      <c r="AU35" s="90"/>
-      <c r="AV35" s="90"/>
-      <c r="AW35" s="90"/>
-      <c r="AX35" s="90"/>
-      <c r="AY35" s="90"/>
-      <c r="AZ35" s="90"/>
-      <c r="BA35" s="90"/>
-      <c r="BB35" s="90"/>
-      <c r="BC35" s="90"/>
-      <c r="BD35" s="90"/>
-      <c r="BE35" s="90"/>
-      <c r="BF35" s="90"/>
-      <c r="BG35" s="90"/>
-      <c r="BH35" s="90"/>
-      <c r="BI35" s="90"/>
-      <c r="BJ35" s="90"/>
-      <c r="BK35" s="90"/>
-      <c r="BL35" s="90"/>
-      <c r="BM35" s="90"/>
-      <c r="BN35" s="90"/>
-      <c r="BO35" s="90"/>
-      <c r="BP35" s="90"/>
-      <c r="BQ35" s="90"/>
-      <c r="BR35" s="90"/>
-      <c r="BS35" s="90"/>
-      <c r="BT35" s="90"/>
-      <c r="BU35" s="90"/>
-      <c r="BV35" s="90"/>
-      <c r="BW35" s="90"/>
-      <c r="BX35" s="90"/>
-      <c r="BY35" s="90"/>
-      <c r="BZ35" s="90"/>
-      <c r="CA35" s="90"/>
-      <c r="CB35" s="90"/>
-      <c r="CC35" s="90"/>
-      <c r="CD35" s="90"/>
-      <c r="CE35" s="90"/>
-      <c r="CF35" s="90"/>
-      <c r="CG35" s="90"/>
-      <c r="CH35" s="90"/>
-      <c r="CI35" s="90"/>
-      <c r="CJ35" s="90"/>
-      <c r="CK35" s="90"/>
-      <c r="CL35" s="90"/>
-      <c r="CM35" s="90"/>
-      <c r="CN35" s="90"/>
-      <c r="CO35" s="90"/>
-      <c r="CP35" s="90"/>
-      <c r="CQ35" s="90"/>
-      <c r="CR35" s="90"/>
-      <c r="CS35" s="90"/>
-      <c r="CT35" s="90"/>
-      <c r="CU35" s="90"/>
-      <c r="CV35" s="90"/>
-      <c r="CW35" s="90"/>
-      <c r="CX35" s="90"/>
-      <c r="CY35" s="90"/>
-      <c r="CZ35" s="90"/>
-      <c r="DA35" s="90"/>
-      <c r="DB35" s="90"/>
-      <c r="DC35" s="90"/>
-      <c r="DD35" s="90"/>
-      <c r="DE35" s="90"/>
-      <c r="DF35" s="90"/>
-      <c r="DG35" s="90"/>
-      <c r="DH35" s="90"/>
-      <c r="DI35" s="90"/>
-      <c r="DJ35" s="90"/>
-      <c r="DK35" s="90"/>
-      <c r="DL35" s="90"/>
-      <c r="DM35" s="90"/>
-      <c r="DN35" s="90"/>
-      <c r="DO35" s="90"/>
-      <c r="DP35" s="90"/>
-      <c r="DQ35" s="90"/>
-      <c r="DR35" s="90"/>
-      <c r="DS35" s="90"/>
-      <c r="DT35" s="90"/>
-      <c r="DU35" s="90"/>
-      <c r="DV35" s="90"/>
+      <c r="B35" s="94"/>
+      <c r="C35" s="85"/>
+      <c r="D35" s="86"/>
+      <c r="E35" s="95"/>
+      <c r="F35" s="96"/>
+      <c r="G35" s="88"/>
+      <c r="H35" s="88"/>
+      <c r="I35" s="89"/>
+      <c r="J35" s="89"/>
+      <c r="K35" s="89"/>
+      <c r="L35" s="89"/>
+      <c r="M35" s="89"/>
+      <c r="N35" s="89"/>
+      <c r="O35" s="89"/>
+      <c r="P35" s="89"/>
+      <c r="Q35" s="89"/>
+      <c r="R35" s="89"/>
+      <c r="S35" s="89"/>
+      <c r="T35" s="89"/>
+      <c r="U35" s="89"/>
+      <c r="V35" s="89"/>
+      <c r="W35" s="89"/>
+      <c r="X35" s="89"/>
+      <c r="Y35" s="89"/>
+      <c r="Z35" s="89"/>
+      <c r="AA35" s="89"/>
+      <c r="AB35" s="89"/>
+      <c r="AC35" s="89"/>
+      <c r="AD35" s="89"/>
+      <c r="AE35" s="89"/>
+      <c r="AF35" s="89"/>
+      <c r="AG35" s="89"/>
+      <c r="AH35" s="89"/>
+      <c r="AI35" s="89"/>
+      <c r="AJ35" s="89"/>
+      <c r="AK35" s="89"/>
+      <c r="AL35" s="89"/>
+      <c r="AM35" s="89"/>
+      <c r="AN35" s="89"/>
+      <c r="AO35" s="89"/>
+      <c r="AP35" s="89"/>
+      <c r="AQ35" s="89"/>
+      <c r="AR35" s="89"/>
+      <c r="AS35" s="89"/>
+      <c r="AT35" s="89"/>
+      <c r="AU35" s="89"/>
+      <c r="AV35" s="89"/>
+      <c r="AW35" s="89"/>
+      <c r="AX35" s="89"/>
+      <c r="AY35" s="89"/>
+      <c r="AZ35" s="89"/>
+      <c r="BA35" s="89"/>
+      <c r="BB35" s="89"/>
+      <c r="BC35" s="89"/>
+      <c r="BD35" s="89"/>
+      <c r="BE35" s="89"/>
+      <c r="BF35" s="89"/>
+      <c r="BG35" s="89"/>
+      <c r="BH35" s="89"/>
+      <c r="BI35" s="89"/>
+      <c r="BJ35" s="89"/>
+      <c r="BK35" s="89"/>
+      <c r="BL35" s="89"/>
+      <c r="BM35" s="89"/>
+      <c r="BN35" s="89"/>
+      <c r="BO35" s="89"/>
+      <c r="BP35" s="89"/>
+      <c r="BQ35" s="89"/>
+      <c r="BR35" s="89"/>
+      <c r="BS35" s="89"/>
+      <c r="BT35" s="89"/>
+      <c r="BU35" s="89"/>
+      <c r="BV35" s="89"/>
+      <c r="BW35" s="89"/>
+      <c r="BX35" s="89"/>
+      <c r="BY35" s="89"/>
+      <c r="BZ35" s="89"/>
+      <c r="CA35" s="89"/>
+      <c r="CB35" s="89"/>
+      <c r="CC35" s="89"/>
+      <c r="CD35" s="89"/>
+      <c r="CE35" s="89"/>
+      <c r="CF35" s="89"/>
+      <c r="CG35" s="89"/>
+      <c r="CH35" s="89"/>
+      <c r="CI35" s="89"/>
+      <c r="CJ35" s="89"/>
+      <c r="CK35" s="89"/>
+      <c r="CL35" s="89"/>
+      <c r="CM35" s="89"/>
+      <c r="CN35" s="89"/>
+      <c r="CO35" s="89"/>
+      <c r="CP35" s="89"/>
+      <c r="CQ35" s="89"/>
+      <c r="CR35" s="89"/>
+      <c r="CS35" s="89"/>
+      <c r="CT35" s="89"/>
+      <c r="CU35" s="89"/>
+      <c r="CV35" s="89"/>
+      <c r="CW35" s="89"/>
+      <c r="CX35" s="89"/>
+      <c r="CY35" s="89"/>
+      <c r="CZ35" s="89"/>
+      <c r="DA35" s="89"/>
+      <c r="DB35" s="89"/>
+      <c r="DC35" s="89"/>
+      <c r="DD35" s="89"/>
+      <c r="DE35" s="89"/>
+      <c r="DF35" s="89"/>
+      <c r="DG35" s="89"/>
+      <c r="DH35" s="89"/>
+      <c r="DI35" s="89"/>
+      <c r="DJ35" s="89"/>
+      <c r="DK35" s="89"/>
+      <c r="DL35" s="89"/>
+      <c r="DM35" s="89"/>
+      <c r="DN35" s="89"/>
+      <c r="DO35" s="89"/>
+      <c r="DP35" s="89"/>
+      <c r="DQ35" s="89"/>
+      <c r="DR35" s="89"/>
+      <c r="DS35" s="89"/>
+      <c r="DT35" s="89"/>
+      <c r="DU35" s="89"/>
+      <c r="DV35" s="89"/>
     </row>
     <row r="36" spans="1:155" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="85"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="87"/>
-      <c r="E36" s="88"/>
-      <c r="F36" s="88"/>
-      <c r="G36" s="89"/>
-      <c r="H36" s="89"/>
-      <c r="I36" s="90"/>
-      <c r="J36" s="90"/>
-      <c r="K36" s="90"/>
-      <c r="L36" s="90"/>
-      <c r="M36" s="90"/>
-      <c r="N36" s="90"/>
-      <c r="O36" s="90"/>
-      <c r="P36" s="90"/>
-      <c r="Q36" s="90"/>
-      <c r="R36" s="90"/>
-      <c r="S36" s="90"/>
-      <c r="T36" s="90"/>
-      <c r="U36" s="90"/>
-      <c r="V36" s="90"/>
-      <c r="W36" s="90"/>
-      <c r="X36" s="90"/>
-      <c r="Y36" s="90"/>
-      <c r="Z36" s="90"/>
-      <c r="AA36" s="90"/>
-      <c r="AB36" s="90"/>
-      <c r="AC36" s="90"/>
-      <c r="AD36" s="90"/>
-      <c r="AE36" s="90"/>
-      <c r="AF36" s="90"/>
-      <c r="AG36" s="90"/>
-      <c r="AH36" s="90"/>
-      <c r="AI36" s="90"/>
-      <c r="AJ36" s="90"/>
-      <c r="AK36" s="90"/>
-      <c r="AL36" s="90"/>
-      <c r="AM36" s="90"/>
-      <c r="AN36" s="90"/>
-      <c r="AO36" s="90"/>
-      <c r="AP36" s="90"/>
-      <c r="AQ36" s="90"/>
-      <c r="AR36" s="90"/>
-      <c r="AS36" s="90"/>
-      <c r="AT36" s="90"/>
-      <c r="AU36" s="90"/>
-      <c r="AV36" s="90"/>
-      <c r="AW36" s="90"/>
-      <c r="AX36" s="90"/>
-      <c r="AY36" s="90"/>
-      <c r="AZ36" s="90"/>
-      <c r="BA36" s="90"/>
-      <c r="BB36" s="90"/>
-      <c r="BC36" s="90"/>
-      <c r="BD36" s="90"/>
-      <c r="BE36" s="90"/>
-      <c r="BF36" s="90"/>
-      <c r="BG36" s="90"/>
-      <c r="BH36" s="90"/>
-      <c r="BI36" s="90"/>
-      <c r="BJ36" s="90"/>
-      <c r="BK36" s="90"/>
-      <c r="BL36" s="90"/>
-      <c r="BM36" s="90"/>
-      <c r="BN36" s="90"/>
-      <c r="BO36" s="90"/>
-      <c r="BP36" s="90"/>
-      <c r="BQ36" s="90"/>
-      <c r="BR36" s="90"/>
-      <c r="BS36" s="90"/>
-      <c r="BT36" s="90"/>
-      <c r="BU36" s="90"/>
-      <c r="BV36" s="90"/>
-      <c r="BW36" s="90"/>
-      <c r="BX36" s="90"/>
-      <c r="BY36" s="90"/>
-      <c r="BZ36" s="90"/>
-      <c r="CA36" s="90"/>
-      <c r="CB36" s="90"/>
-      <c r="CC36" s="90"/>
-      <c r="CD36" s="90"/>
-      <c r="CE36" s="90"/>
-      <c r="CF36" s="90"/>
-      <c r="CG36" s="90"/>
-      <c r="CH36" s="90"/>
-      <c r="CI36" s="90"/>
-      <c r="CJ36" s="90"/>
-      <c r="CK36" s="90"/>
-      <c r="CL36" s="90"/>
-      <c r="CM36" s="90"/>
-      <c r="CN36" s="90"/>
-      <c r="CO36" s="90"/>
-      <c r="CP36" s="90"/>
-      <c r="CQ36" s="90"/>
-      <c r="CR36" s="90"/>
-      <c r="CS36" s="90"/>
-      <c r="CT36" s="90"/>
-      <c r="CU36" s="90"/>
-      <c r="CV36" s="90"/>
-      <c r="CW36" s="90"/>
-      <c r="CX36" s="90"/>
-      <c r="CY36" s="90"/>
-      <c r="CZ36" s="90"/>
-      <c r="DA36" s="90"/>
-      <c r="DB36" s="90"/>
-      <c r="DC36" s="90"/>
-      <c r="DD36" s="90"/>
-      <c r="DE36" s="90"/>
-      <c r="DF36" s="90"/>
-      <c r="DG36" s="90"/>
-      <c r="DH36" s="90"/>
-      <c r="DI36" s="90"/>
-      <c r="DJ36" s="90"/>
-      <c r="DK36" s="90"/>
-      <c r="DL36" s="90"/>
-      <c r="DM36" s="90"/>
-      <c r="DN36" s="90"/>
-      <c r="DO36" s="90"/>
-      <c r="DP36" s="90"/>
-      <c r="DQ36" s="90"/>
-      <c r="DR36" s="90"/>
-      <c r="DS36" s="90"/>
-      <c r="DT36" s="90"/>
-      <c r="DU36" s="90"/>
-      <c r="DV36" s="90"/>
+      <c r="B36" s="84"/>
+      <c r="C36" s="85"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="87"/>
+      <c r="F36" s="87"/>
+      <c r="G36" s="88"/>
+      <c r="H36" s="88"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="89"/>
+      <c r="K36" s="89"/>
+      <c r="L36" s="89"/>
+      <c r="M36" s="89"/>
+      <c r="N36" s="89"/>
+      <c r="O36" s="89"/>
+      <c r="P36" s="89"/>
+      <c r="Q36" s="89"/>
+      <c r="R36" s="89"/>
+      <c r="S36" s="89"/>
+      <c r="T36" s="89"/>
+      <c r="U36" s="89"/>
+      <c r="V36" s="89"/>
+      <c r="W36" s="89"/>
+      <c r="X36" s="89"/>
+      <c r="Y36" s="89"/>
+      <c r="Z36" s="89"/>
+      <c r="AA36" s="89"/>
+      <c r="AB36" s="89"/>
+      <c r="AC36" s="89"/>
+      <c r="AD36" s="89"/>
+      <c r="AE36" s="89"/>
+      <c r="AF36" s="89"/>
+      <c r="AG36" s="89"/>
+      <c r="AH36" s="89"/>
+      <c r="AI36" s="89"/>
+      <c r="AJ36" s="89"/>
+      <c r="AK36" s="89"/>
+      <c r="AL36" s="89"/>
+      <c r="AM36" s="89"/>
+      <c r="AN36" s="89"/>
+      <c r="AO36" s="89"/>
+      <c r="AP36" s="89"/>
+      <c r="AQ36" s="89"/>
+      <c r="AR36" s="89"/>
+      <c r="AS36" s="89"/>
+      <c r="AT36" s="89"/>
+      <c r="AU36" s="89"/>
+      <c r="AV36" s="89"/>
+      <c r="AW36" s="89"/>
+      <c r="AX36" s="89"/>
+      <c r="AY36" s="89"/>
+      <c r="AZ36" s="89"/>
+      <c r="BA36" s="89"/>
+      <c r="BB36" s="89"/>
+      <c r="BC36" s="89"/>
+      <c r="BD36" s="89"/>
+      <c r="BE36" s="89"/>
+      <c r="BF36" s="89"/>
+      <c r="BG36" s="89"/>
+      <c r="BH36" s="89"/>
+      <c r="BI36" s="89"/>
+      <c r="BJ36" s="89"/>
+      <c r="BK36" s="89"/>
+      <c r="BL36" s="89"/>
+      <c r="BM36" s="89"/>
+      <c r="BN36" s="89"/>
+      <c r="BO36" s="89"/>
+      <c r="BP36" s="89"/>
+      <c r="BQ36" s="89"/>
+      <c r="BR36" s="89"/>
+      <c r="BS36" s="89"/>
+      <c r="BT36" s="89"/>
+      <c r="BU36" s="89"/>
+      <c r="BV36" s="89"/>
+      <c r="BW36" s="89"/>
+      <c r="BX36" s="89"/>
+      <c r="BY36" s="89"/>
+      <c r="BZ36" s="89"/>
+      <c r="CA36" s="89"/>
+      <c r="CB36" s="89"/>
+      <c r="CC36" s="89"/>
+      <c r="CD36" s="89"/>
+      <c r="CE36" s="89"/>
+      <c r="CF36" s="89"/>
+      <c r="CG36" s="89"/>
+      <c r="CH36" s="89"/>
+      <c r="CI36" s="89"/>
+      <c r="CJ36" s="89"/>
+      <c r="CK36" s="89"/>
+      <c r="CL36" s="89"/>
+      <c r="CM36" s="89"/>
+      <c r="CN36" s="89"/>
+      <c r="CO36" s="89"/>
+      <c r="CP36" s="89"/>
+      <c r="CQ36" s="89"/>
+      <c r="CR36" s="89"/>
+      <c r="CS36" s="89"/>
+      <c r="CT36" s="89"/>
+      <c r="CU36" s="89"/>
+      <c r="CV36" s="89"/>
+      <c r="CW36" s="89"/>
+      <c r="CX36" s="89"/>
+      <c r="CY36" s="89"/>
+      <c r="CZ36" s="89"/>
+      <c r="DA36" s="89"/>
+      <c r="DB36" s="89"/>
+      <c r="DC36" s="89"/>
+      <c r="DD36" s="89"/>
+      <c r="DE36" s="89"/>
+      <c r="DF36" s="89"/>
+      <c r="DG36" s="89"/>
+      <c r="DH36" s="89"/>
+      <c r="DI36" s="89"/>
+      <c r="DJ36" s="89"/>
+      <c r="DK36" s="89"/>
+      <c r="DL36" s="89"/>
+      <c r="DM36" s="89"/>
+      <c r="DN36" s="89"/>
+      <c r="DO36" s="89"/>
+      <c r="DP36" s="89"/>
+      <c r="DQ36" s="89"/>
+      <c r="DR36" s="89"/>
+      <c r="DS36" s="89"/>
+      <c r="DT36" s="89"/>
+      <c r="DU36" s="89"/>
+      <c r="DV36" s="89"/>
     </row>
     <row r="37" spans="1:155" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="85"/>
-      <c r="C37" s="86"/>
-      <c r="D37" s="87"/>
-      <c r="E37" s="88"/>
-      <c r="F37" s="88"/>
-      <c r="G37" s="89"/>
-      <c r="H37" s="89"/>
-      <c r="I37" s="90"/>
-      <c r="J37" s="90"/>
-      <c r="K37" s="90"/>
-      <c r="L37" s="90"/>
-      <c r="M37" s="90"/>
-      <c r="N37" s="90"/>
-      <c r="O37" s="90"/>
-      <c r="P37" s="90"/>
-      <c r="Q37" s="90"/>
-      <c r="R37" s="90"/>
-      <c r="S37" s="90"/>
-      <c r="T37" s="90"/>
-      <c r="U37" s="90"/>
-      <c r="V37" s="90"/>
-      <c r="W37" s="90"/>
-      <c r="X37" s="90"/>
-      <c r="Y37" s="90"/>
-      <c r="Z37" s="90"/>
-      <c r="AA37" s="90"/>
-      <c r="AB37" s="90"/>
-      <c r="AC37" s="90"/>
-      <c r="AD37" s="90"/>
-      <c r="AE37" s="90"/>
-      <c r="AF37" s="90"/>
-      <c r="AG37" s="90"/>
-      <c r="AH37" s="90"/>
-      <c r="AI37" s="90"/>
-      <c r="AJ37" s="90"/>
-      <c r="AK37" s="90"/>
-      <c r="AL37" s="90"/>
-      <c r="AM37" s="90"/>
-      <c r="AN37" s="90"/>
-      <c r="AO37" s="90"/>
-      <c r="AP37" s="90"/>
-      <c r="AQ37" s="90"/>
-      <c r="AR37" s="90"/>
-      <c r="AS37" s="90"/>
-      <c r="AT37" s="90"/>
-      <c r="AU37" s="90"/>
-      <c r="AV37" s="90"/>
-      <c r="AW37" s="90"/>
-      <c r="AX37" s="90"/>
-      <c r="AY37" s="90"/>
-      <c r="AZ37" s="90"/>
-      <c r="BA37" s="90"/>
-      <c r="BB37" s="90"/>
-      <c r="BC37" s="90"/>
-      <c r="BD37" s="90"/>
-      <c r="BE37" s="90"/>
-      <c r="BF37" s="90"/>
-      <c r="BG37" s="90"/>
-      <c r="BH37" s="90"/>
-      <c r="BI37" s="90"/>
-      <c r="BJ37" s="90"/>
-      <c r="BK37" s="90"/>
-      <c r="BL37" s="90"/>
-      <c r="BM37" s="90"/>
-      <c r="BN37" s="90"/>
-      <c r="BO37" s="90"/>
-      <c r="BP37" s="90"/>
-      <c r="BQ37" s="90"/>
-      <c r="BR37" s="90"/>
-      <c r="BS37" s="90"/>
-      <c r="BT37" s="90"/>
-      <c r="BU37" s="90"/>
-      <c r="BV37" s="90"/>
-      <c r="BW37" s="90"/>
-      <c r="BX37" s="90"/>
-      <c r="BY37" s="90"/>
-      <c r="BZ37" s="90"/>
-      <c r="CA37" s="90"/>
-      <c r="CB37" s="90"/>
-      <c r="CC37" s="90"/>
-      <c r="CD37" s="90"/>
-      <c r="CE37" s="90"/>
-      <c r="CF37" s="90"/>
-      <c r="CG37" s="90"/>
-      <c r="CH37" s="90"/>
-      <c r="CI37" s="90"/>
-      <c r="CJ37" s="90"/>
-      <c r="CK37" s="90"/>
-      <c r="CL37" s="90"/>
-      <c r="CM37" s="90"/>
-      <c r="CN37" s="90"/>
-      <c r="CO37" s="90"/>
-      <c r="CP37" s="90"/>
-      <c r="CQ37" s="90"/>
-      <c r="CR37" s="90"/>
-      <c r="CS37" s="90"/>
-      <c r="CT37" s="90"/>
-      <c r="CU37" s="90"/>
-      <c r="CV37" s="90"/>
-      <c r="CW37" s="90"/>
-      <c r="CX37" s="90"/>
-      <c r="CY37" s="90"/>
-      <c r="CZ37" s="90"/>
-      <c r="DA37" s="90"/>
-      <c r="DB37" s="90"/>
-      <c r="DC37" s="90"/>
-      <c r="DD37" s="90"/>
-      <c r="DE37" s="90"/>
-      <c r="DF37" s="90"/>
-      <c r="DG37" s="90"/>
-      <c r="DH37" s="90"/>
-      <c r="DI37" s="90"/>
-      <c r="DJ37" s="90"/>
-      <c r="DK37" s="90"/>
-      <c r="DL37" s="90"/>
-      <c r="DM37" s="90"/>
-      <c r="DN37" s="90"/>
-      <c r="DO37" s="90"/>
-      <c r="DP37" s="90"/>
-      <c r="DQ37" s="90"/>
-      <c r="DR37" s="90"/>
-      <c r="DS37" s="90"/>
-      <c r="DT37" s="90"/>
-      <c r="DU37" s="90"/>
-      <c r="DV37" s="90"/>
+      <c r="B37" s="84"/>
+      <c r="C37" s="85"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="87"/>
+      <c r="F37" s="87"/>
+      <c r="G37" s="88"/>
+      <c r="H37" s="88"/>
+      <c r="I37" s="89"/>
+      <c r="J37" s="89"/>
+      <c r="K37" s="89"/>
+      <c r="L37" s="89"/>
+      <c r="M37" s="89"/>
+      <c r="N37" s="89"/>
+      <c r="O37" s="89"/>
+      <c r="P37" s="89"/>
+      <c r="Q37" s="89"/>
+      <c r="R37" s="89"/>
+      <c r="S37" s="89"/>
+      <c r="T37" s="89"/>
+      <c r="U37" s="89"/>
+      <c r="V37" s="89"/>
+      <c r="W37" s="89"/>
+      <c r="X37" s="89"/>
+      <c r="Y37" s="89"/>
+      <c r="Z37" s="89"/>
+      <c r="AA37" s="89"/>
+      <c r="AB37" s="89"/>
+      <c r="AC37" s="89"/>
+      <c r="AD37" s="89"/>
+      <c r="AE37" s="89"/>
+      <c r="AF37" s="89"/>
+      <c r="AG37" s="89"/>
+      <c r="AH37" s="89"/>
+      <c r="AI37" s="89"/>
+      <c r="AJ37" s="89"/>
+      <c r="AK37" s="89"/>
+      <c r="AL37" s="89"/>
+      <c r="AM37" s="89"/>
+      <c r="AN37" s="89"/>
+      <c r="AO37" s="89"/>
+      <c r="AP37" s="89"/>
+      <c r="AQ37" s="89"/>
+      <c r="AR37" s="89"/>
+      <c r="AS37" s="89"/>
+      <c r="AT37" s="89"/>
+      <c r="AU37" s="89"/>
+      <c r="AV37" s="89"/>
+      <c r="AW37" s="89"/>
+      <c r="AX37" s="89"/>
+      <c r="AY37" s="89"/>
+      <c r="AZ37" s="89"/>
+      <c r="BA37" s="89"/>
+      <c r="BB37" s="89"/>
+      <c r="BC37" s="89"/>
+      <c r="BD37" s="89"/>
+      <c r="BE37" s="89"/>
+      <c r="BF37" s="89"/>
+      <c r="BG37" s="89"/>
+      <c r="BH37" s="89"/>
+      <c r="BI37" s="89"/>
+      <c r="BJ37" s="89"/>
+      <c r="BK37" s="89"/>
+      <c r="BL37" s="89"/>
+      <c r="BM37" s="89"/>
+      <c r="BN37" s="89"/>
+      <c r="BO37" s="89"/>
+      <c r="BP37" s="89"/>
+      <c r="BQ37" s="89"/>
+      <c r="BR37" s="89"/>
+      <c r="BS37" s="89"/>
+      <c r="BT37" s="89"/>
+      <c r="BU37" s="89"/>
+      <c r="BV37" s="89"/>
+      <c r="BW37" s="89"/>
+      <c r="BX37" s="89"/>
+      <c r="BY37" s="89"/>
+      <c r="BZ37" s="89"/>
+      <c r="CA37" s="89"/>
+      <c r="CB37" s="89"/>
+      <c r="CC37" s="89"/>
+      <c r="CD37" s="89"/>
+      <c r="CE37" s="89"/>
+      <c r="CF37" s="89"/>
+      <c r="CG37" s="89"/>
+      <c r="CH37" s="89"/>
+      <c r="CI37" s="89"/>
+      <c r="CJ37" s="89"/>
+      <c r="CK37" s="89"/>
+      <c r="CL37" s="89"/>
+      <c r="CM37" s="89"/>
+      <c r="CN37" s="89"/>
+      <c r="CO37" s="89"/>
+      <c r="CP37" s="89"/>
+      <c r="CQ37" s="89"/>
+      <c r="CR37" s="89"/>
+      <c r="CS37" s="89"/>
+      <c r="CT37" s="89"/>
+      <c r="CU37" s="89"/>
+      <c r="CV37" s="89"/>
+      <c r="CW37" s="89"/>
+      <c r="CX37" s="89"/>
+      <c r="CY37" s="89"/>
+      <c r="CZ37" s="89"/>
+      <c r="DA37" s="89"/>
+      <c r="DB37" s="89"/>
+      <c r="DC37" s="89"/>
+      <c r="DD37" s="89"/>
+      <c r="DE37" s="89"/>
+      <c r="DF37" s="89"/>
+      <c r="DG37" s="89"/>
+      <c r="DH37" s="89"/>
+      <c r="DI37" s="89"/>
+      <c r="DJ37" s="89"/>
+      <c r="DK37" s="89"/>
+      <c r="DL37" s="89"/>
+      <c r="DM37" s="89"/>
+      <c r="DN37" s="89"/>
+      <c r="DO37" s="89"/>
+      <c r="DP37" s="89"/>
+      <c r="DQ37" s="89"/>
+      <c r="DR37" s="89"/>
+      <c r="DS37" s="89"/>
+      <c r="DT37" s="89"/>
+      <c r="DU37" s="89"/>
+      <c r="DV37" s="89"/>
     </row>
     <row r="38" spans="1:155" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="85"/>
-      <c r="C38" s="86"/>
-      <c r="D38" s="87"/>
-      <c r="E38" s="88"/>
-      <c r="F38" s="88"/>
-      <c r="G38" s="89"/>
-      <c r="H38" s="89"/>
-      <c r="I38" s="90"/>
-      <c r="J38" s="90"/>
-      <c r="K38" s="90"/>
-      <c r="L38" s="90"/>
-      <c r="M38" s="90"/>
-      <c r="N38" s="90"/>
-      <c r="O38" s="90"/>
-      <c r="P38" s="90"/>
-      <c r="Q38" s="90"/>
-      <c r="R38" s="90"/>
-      <c r="S38" s="90"/>
-      <c r="T38" s="90"/>
-      <c r="U38" s="90"/>
-      <c r="V38" s="90"/>
-      <c r="W38" s="90"/>
-      <c r="X38" s="90"/>
-      <c r="Y38" s="90"/>
-      <c r="Z38" s="90"/>
-      <c r="AA38" s="90"/>
-      <c r="AB38" s="90"/>
-      <c r="AC38" s="90"/>
-      <c r="AD38" s="90"/>
-      <c r="AE38" s="90"/>
-      <c r="AF38" s="90"/>
-      <c r="AG38" s="90"/>
-      <c r="AH38" s="90"/>
-      <c r="AI38" s="90"/>
-      <c r="AJ38" s="90"/>
-      <c r="AK38" s="90"/>
-      <c r="AL38" s="90"/>
-      <c r="AM38" s="90"/>
-      <c r="AN38" s="90"/>
-      <c r="AO38" s="90"/>
-      <c r="AP38" s="90"/>
-      <c r="AQ38" s="90"/>
-      <c r="AR38" s="90"/>
-      <c r="AS38" s="90"/>
-      <c r="AT38" s="90"/>
-      <c r="AU38" s="90"/>
-      <c r="AV38" s="90"/>
-      <c r="AW38" s="90"/>
-      <c r="AX38" s="90"/>
-      <c r="AY38" s="90"/>
-      <c r="AZ38" s="90"/>
-      <c r="BA38" s="90"/>
-      <c r="BB38" s="90"/>
-      <c r="BC38" s="90"/>
-      <c r="BD38" s="90"/>
-      <c r="BE38" s="90"/>
-      <c r="BF38" s="90"/>
-      <c r="BG38" s="90"/>
-      <c r="BH38" s="90"/>
-      <c r="BI38" s="90"/>
-      <c r="BJ38" s="90"/>
-      <c r="BK38" s="90"/>
-      <c r="BL38" s="90"/>
-      <c r="BM38" s="90"/>
-      <c r="BN38" s="90"/>
-      <c r="BO38" s="90"/>
-      <c r="BP38" s="90"/>
-      <c r="BQ38" s="90"/>
-      <c r="BR38" s="90"/>
-      <c r="BS38" s="90"/>
-      <c r="BT38" s="90"/>
-      <c r="BU38" s="90"/>
-      <c r="BV38" s="90"/>
-      <c r="BW38" s="90"/>
-      <c r="BX38" s="90"/>
-      <c r="BY38" s="90"/>
-      <c r="BZ38" s="90"/>
-      <c r="CA38" s="90"/>
-      <c r="CB38" s="90"/>
-      <c r="CC38" s="90"/>
-      <c r="CD38" s="90"/>
-      <c r="CE38" s="90"/>
-      <c r="CF38" s="90"/>
-      <c r="CG38" s="90"/>
-      <c r="CH38" s="90"/>
-      <c r="CI38" s="90"/>
-      <c r="CJ38" s="90"/>
-      <c r="CK38" s="90"/>
-      <c r="CL38" s="90"/>
-      <c r="CM38" s="90"/>
-      <c r="CN38" s="90"/>
-      <c r="CO38" s="90"/>
-      <c r="CP38" s="90"/>
-      <c r="CQ38" s="90"/>
-      <c r="CR38" s="90"/>
-      <c r="CS38" s="90"/>
-      <c r="CT38" s="90"/>
-      <c r="CU38" s="90"/>
-      <c r="CV38" s="90"/>
-      <c r="CW38" s="90"/>
-      <c r="CX38" s="90"/>
-      <c r="CY38" s="90"/>
-      <c r="CZ38" s="90"/>
-      <c r="DA38" s="90"/>
-      <c r="DB38" s="90"/>
-      <c r="DC38" s="90"/>
-      <c r="DD38" s="90"/>
-      <c r="DE38" s="90"/>
-      <c r="DF38" s="90"/>
-      <c r="DG38" s="90"/>
-      <c r="DH38" s="90"/>
-      <c r="DI38" s="90"/>
-      <c r="DJ38" s="90"/>
-      <c r="DK38" s="90"/>
-      <c r="DL38" s="90"/>
-      <c r="DM38" s="90"/>
-      <c r="DN38" s="90"/>
-      <c r="DO38" s="90"/>
-      <c r="DP38" s="90"/>
-      <c r="DQ38" s="90"/>
-      <c r="DR38" s="90"/>
-      <c r="DS38" s="90"/>
-      <c r="DT38" s="90"/>
-      <c r="DU38" s="90"/>
-      <c r="DV38" s="90"/>
+      <c r="B38" s="84"/>
+      <c r="C38" s="85"/>
+      <c r="D38" s="86"/>
+      <c r="E38" s="87"/>
+      <c r="F38" s="87"/>
+      <c r="G38" s="88"/>
+      <c r="H38" s="88"/>
+      <c r="I38" s="89"/>
+      <c r="J38" s="89"/>
+      <c r="K38" s="89"/>
+      <c r="L38" s="89"/>
+      <c r="M38" s="89"/>
+      <c r="N38" s="89"/>
+      <c r="O38" s="89"/>
+      <c r="P38" s="89"/>
+      <c r="Q38" s="89"/>
+      <c r="R38" s="89"/>
+      <c r="S38" s="89"/>
+      <c r="T38" s="89"/>
+      <c r="U38" s="89"/>
+      <c r="V38" s="89"/>
+      <c r="W38" s="89"/>
+      <c r="X38" s="89"/>
+      <c r="Y38" s="89"/>
+      <c r="Z38" s="89"/>
+      <c r="AA38" s="89"/>
+      <c r="AB38" s="89"/>
+      <c r="AC38" s="89"/>
+      <c r="AD38" s="89"/>
+      <c r="AE38" s="89"/>
+      <c r="AF38" s="89"/>
+      <c r="AG38" s="89"/>
+      <c r="AH38" s="89"/>
+      <c r="AI38" s="89"/>
+      <c r="AJ38" s="89"/>
+      <c r="AK38" s="89"/>
+      <c r="AL38" s="89"/>
+      <c r="AM38" s="89"/>
+      <c r="AN38" s="89"/>
+      <c r="AO38" s="89"/>
+      <c r="AP38" s="89"/>
+      <c r="AQ38" s="89"/>
+      <c r="AR38" s="89"/>
+      <c r="AS38" s="89"/>
+      <c r="AT38" s="89"/>
+      <c r="AU38" s="89"/>
+      <c r="AV38" s="89"/>
+      <c r="AW38" s="89"/>
+      <c r="AX38" s="89"/>
+      <c r="AY38" s="89"/>
+      <c r="AZ38" s="89"/>
+      <c r="BA38" s="89"/>
+      <c r="BB38" s="89"/>
+      <c r="BC38" s="89"/>
+      <c r="BD38" s="89"/>
+      <c r="BE38" s="89"/>
+      <c r="BF38" s="89"/>
+      <c r="BG38" s="89"/>
+      <c r="BH38" s="89"/>
+      <c r="BI38" s="89"/>
+      <c r="BJ38" s="89"/>
+      <c r="BK38" s="89"/>
+      <c r="BL38" s="89"/>
+      <c r="BM38" s="89"/>
+      <c r="BN38" s="89"/>
+      <c r="BO38" s="89"/>
+      <c r="BP38" s="89"/>
+      <c r="BQ38" s="89"/>
+      <c r="BR38" s="89"/>
+      <c r="BS38" s="89"/>
+      <c r="BT38" s="89"/>
+      <c r="BU38" s="89"/>
+      <c r="BV38" s="89"/>
+      <c r="BW38" s="89"/>
+      <c r="BX38" s="89"/>
+      <c r="BY38" s="89"/>
+      <c r="BZ38" s="89"/>
+      <c r="CA38" s="89"/>
+      <c r="CB38" s="89"/>
+      <c r="CC38" s="89"/>
+      <c r="CD38" s="89"/>
+      <c r="CE38" s="89"/>
+      <c r="CF38" s="89"/>
+      <c r="CG38" s="89"/>
+      <c r="CH38" s="89"/>
+      <c r="CI38" s="89"/>
+      <c r="CJ38" s="89"/>
+      <c r="CK38" s="89"/>
+      <c r="CL38" s="89"/>
+      <c r="CM38" s="89"/>
+      <c r="CN38" s="89"/>
+      <c r="CO38" s="89"/>
+      <c r="CP38" s="89"/>
+      <c r="CQ38" s="89"/>
+      <c r="CR38" s="89"/>
+      <c r="CS38" s="89"/>
+      <c r="CT38" s="89"/>
+      <c r="CU38" s="89"/>
+      <c r="CV38" s="89"/>
+      <c r="CW38" s="89"/>
+      <c r="CX38" s="89"/>
+      <c r="CY38" s="89"/>
+      <c r="CZ38" s="89"/>
+      <c r="DA38" s="89"/>
+      <c r="DB38" s="89"/>
+      <c r="DC38" s="89"/>
+      <c r="DD38" s="89"/>
+      <c r="DE38" s="89"/>
+      <c r="DF38" s="89"/>
+      <c r="DG38" s="89"/>
+      <c r="DH38" s="89"/>
+      <c r="DI38" s="89"/>
+      <c r="DJ38" s="89"/>
+      <c r="DK38" s="89"/>
+      <c r="DL38" s="89"/>
+      <c r="DM38" s="89"/>
+      <c r="DN38" s="89"/>
+      <c r="DO38" s="89"/>
+      <c r="DP38" s="89"/>
+      <c r="DQ38" s="89"/>
+      <c r="DR38" s="89"/>
+      <c r="DS38" s="89"/>
+      <c r="DT38" s="89"/>
+      <c r="DU38" s="89"/>
+      <c r="DV38" s="89"/>
     </row>
     <row r="39" spans="1:155" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="98"/>
-      <c r="C39" s="98"/>
-      <c r="D39" s="98"/>
-      <c r="E39" s="99"/>
-      <c r="F39" s="98"/>
-      <c r="G39" s="98"/>
-      <c r="H39" s="98"/>
-      <c r="I39" s="98"/>
-      <c r="J39" s="98"/>
-      <c r="K39" s="98"/>
-      <c r="L39" s="98"/>
-      <c r="M39" s="98"/>
-      <c r="N39" s="98"/>
-      <c r="O39" s="98"/>
-      <c r="P39" s="98"/>
-      <c r="Q39" s="98"/>
-      <c r="R39" s="98"/>
-      <c r="S39" s="98"/>
-      <c r="T39" s="98"/>
-      <c r="U39" s="98"/>
-      <c r="V39" s="98"/>
-      <c r="W39" s="98"/>
-      <c r="X39" s="98"/>
-      <c r="Y39" s="98"/>
-      <c r="Z39" s="98"/>
-      <c r="AA39" s="98"/>
-      <c r="AB39" s="98"/>
-      <c r="AC39" s="98"/>
-      <c r="AD39" s="98"/>
-      <c r="AE39" s="98"/>
-      <c r="AF39" s="98"/>
-      <c r="AG39" s="98"/>
-      <c r="AH39" s="98"/>
-      <c r="AI39" s="98"/>
-      <c r="AJ39" s="98"/>
-      <c r="AK39" s="98"/>
-      <c r="AL39" s="98"/>
-      <c r="AM39" s="98"/>
-      <c r="AN39" s="98"/>
-      <c r="AO39" s="98"/>
-      <c r="AP39" s="98"/>
-      <c r="AQ39" s="98"/>
-      <c r="AR39" s="98"/>
-      <c r="AS39" s="98"/>
-      <c r="AT39" s="98"/>
-      <c r="AU39" s="98"/>
-      <c r="AV39" s="98"/>
-      <c r="AW39" s="98"/>
-      <c r="AX39" s="98"/>
-      <c r="AY39" s="98"/>
-      <c r="AZ39" s="98"/>
-      <c r="BA39" s="98"/>
-      <c r="BB39" s="98"/>
-      <c r="BC39" s="98"/>
-      <c r="BD39" s="98"/>
-      <c r="BE39" s="98"/>
-      <c r="BF39" s="98"/>
-      <c r="BG39" s="98"/>
-      <c r="BH39" s="98"/>
-      <c r="BI39" s="98"/>
-      <c r="BJ39" s="98"/>
-      <c r="BK39" s="98"/>
-      <c r="BL39" s="98"/>
-      <c r="BM39" s="98"/>
-      <c r="BN39" s="98"/>
-      <c r="BO39" s="98"/>
-      <c r="BP39" s="98"/>
-      <c r="BQ39" s="98"/>
-      <c r="BR39" s="98"/>
-      <c r="BS39" s="98"/>
-      <c r="BT39" s="98"/>
-      <c r="BU39" s="98"/>
-      <c r="BV39" s="98"/>
-      <c r="BW39" s="98"/>
-      <c r="BX39" s="98"/>
-      <c r="BY39" s="98"/>
-      <c r="BZ39" s="98"/>
-      <c r="CA39" s="98"/>
-      <c r="CB39" s="98"/>
-      <c r="CC39" s="98"/>
-      <c r="CD39" s="98"/>
-      <c r="CE39" s="98"/>
-      <c r="CF39" s="98"/>
-      <c r="CG39" s="98"/>
-      <c r="CH39" s="98"/>
-      <c r="CI39" s="98"/>
-      <c r="CJ39" s="98"/>
-      <c r="CK39" s="98"/>
-      <c r="CL39" s="98"/>
-      <c r="CM39" s="98"/>
-      <c r="CN39" s="98"/>
-      <c r="CO39" s="98"/>
-      <c r="CP39" s="98"/>
-      <c r="CQ39" s="98"/>
-      <c r="CR39" s="98"/>
-      <c r="CS39" s="98"/>
-      <c r="CT39" s="98"/>
-      <c r="CU39" s="98"/>
-      <c r="CV39" s="98"/>
-      <c r="CW39" s="98"/>
-      <c r="CX39" s="98"/>
-      <c r="CY39" s="98"/>
-      <c r="CZ39" s="98"/>
-      <c r="DA39" s="98"/>
-      <c r="DB39" s="98"/>
-      <c r="DC39" s="98"/>
-      <c r="DD39" s="98"/>
-      <c r="DE39" s="98"/>
-      <c r="DF39" s="98"/>
-      <c r="DG39" s="98"/>
-      <c r="DH39" s="98"/>
-      <c r="DI39" s="98"/>
-      <c r="DJ39" s="98"/>
-      <c r="DK39" s="98"/>
-      <c r="DL39" s="98"/>
-      <c r="DM39" s="98"/>
-      <c r="DN39" s="98"/>
-      <c r="DO39" s="98"/>
-      <c r="DP39" s="98"/>
-      <c r="DQ39" s="98"/>
-      <c r="DR39" s="98"/>
-      <c r="DS39" s="98"/>
-      <c r="DT39" s="98"/>
-      <c r="DU39" s="98"/>
-      <c r="DV39" s="98"/>
-      <c r="DW39" s="98"/>
+      <c r="B39" s="97"/>
+      <c r="C39" s="97"/>
+      <c r="D39" s="97"/>
+      <c r="E39" s="98"/>
+      <c r="F39" s="97"/>
+      <c r="G39" s="97"/>
+      <c r="H39" s="97"/>
+      <c r="I39" s="97"/>
+      <c r="J39" s="97"/>
+      <c r="K39" s="97"/>
+      <c r="L39" s="97"/>
+      <c r="M39" s="97"/>
+      <c r="N39" s="97"/>
+      <c r="O39" s="97"/>
+      <c r="P39" s="97"/>
+      <c r="Q39" s="97"/>
+      <c r="R39" s="97"/>
+      <c r="S39" s="97"/>
+      <c r="T39" s="97"/>
+      <c r="U39" s="97"/>
+      <c r="V39" s="97"/>
+      <c r="W39" s="97"/>
+      <c r="X39" s="97"/>
+      <c r="Y39" s="97"/>
+      <c r="Z39" s="97"/>
+      <c r="AA39" s="97"/>
+      <c r="AB39" s="97"/>
+      <c r="AC39" s="97"/>
+      <c r="AD39" s="97"/>
+      <c r="AE39" s="97"/>
+      <c r="AF39" s="97"/>
+      <c r="AG39" s="97"/>
+      <c r="AH39" s="97"/>
+      <c r="AI39" s="97"/>
+      <c r="AJ39" s="97"/>
+      <c r="AK39" s="97"/>
+      <c r="AL39" s="97"/>
+      <c r="AM39" s="97"/>
+      <c r="AN39" s="97"/>
+      <c r="AO39" s="97"/>
+      <c r="AP39" s="97"/>
+      <c r="AQ39" s="97"/>
+      <c r="AR39" s="97"/>
+      <c r="AS39" s="97"/>
+      <c r="AT39" s="97"/>
+      <c r="AU39" s="97"/>
+      <c r="AV39" s="97"/>
+      <c r="AW39" s="97"/>
+      <c r="AX39" s="97"/>
+      <c r="AY39" s="97"/>
+      <c r="AZ39" s="97"/>
+      <c r="BA39" s="97"/>
+      <c r="BB39" s="97"/>
+      <c r="BC39" s="97"/>
+      <c r="BD39" s="97"/>
+      <c r="BE39" s="97"/>
+      <c r="BF39" s="97"/>
+      <c r="BG39" s="97"/>
+      <c r="BH39" s="97"/>
+      <c r="BI39" s="97"/>
+      <c r="BJ39" s="97"/>
+      <c r="BK39" s="97"/>
+      <c r="BL39" s="97"/>
+      <c r="BM39" s="97"/>
+      <c r="BN39" s="97"/>
+      <c r="BO39" s="97"/>
+      <c r="BP39" s="97"/>
+      <c r="BQ39" s="97"/>
+      <c r="BR39" s="97"/>
+      <c r="BS39" s="97"/>
+      <c r="BT39" s="97"/>
+      <c r="BU39" s="97"/>
+      <c r="BV39" s="97"/>
+      <c r="BW39" s="97"/>
+      <c r="BX39" s="97"/>
+      <c r="BY39" s="97"/>
+      <c r="BZ39" s="97"/>
+      <c r="CA39" s="97"/>
+      <c r="CB39" s="97"/>
+      <c r="CC39" s="97"/>
+      <c r="CD39" s="97"/>
+      <c r="CE39" s="97"/>
+      <c r="CF39" s="97"/>
+      <c r="CG39" s="97"/>
+      <c r="CH39" s="97"/>
+      <c r="CI39" s="97"/>
+      <c r="CJ39" s="97"/>
+      <c r="CK39" s="97"/>
+      <c r="CL39" s="97"/>
+      <c r="CM39" s="97"/>
+      <c r="CN39" s="97"/>
+      <c r="CO39" s="97"/>
+      <c r="CP39" s="97"/>
+      <c r="CQ39" s="97"/>
+      <c r="CR39" s="97"/>
+      <c r="CS39" s="97"/>
+      <c r="CT39" s="97"/>
+      <c r="CU39" s="97"/>
+      <c r="CV39" s="97"/>
+      <c r="CW39" s="97"/>
+      <c r="CX39" s="97"/>
+      <c r="CY39" s="97"/>
+      <c r="CZ39" s="97"/>
+      <c r="DA39" s="97"/>
+      <c r="DB39" s="97"/>
+      <c r="DC39" s="97"/>
+      <c r="DD39" s="97"/>
+      <c r="DE39" s="97"/>
+      <c r="DF39" s="97"/>
+      <c r="DG39" s="97"/>
+      <c r="DH39" s="97"/>
+      <c r="DI39" s="97"/>
+      <c r="DJ39" s="97"/>
+      <c r="DK39" s="97"/>
+      <c r="DL39" s="97"/>
+      <c r="DM39" s="97"/>
+      <c r="DN39" s="97"/>
+      <c r="DO39" s="97"/>
+      <c r="DP39" s="97"/>
+      <c r="DQ39" s="97"/>
+      <c r="DR39" s="97"/>
+      <c r="DS39" s="97"/>
+      <c r="DT39" s="97"/>
+      <c r="DU39" s="97"/>
+      <c r="DV39" s="97"/>
+      <c r="DW39" s="97"/>
     </row>
     <row r="41" spans="1:155" ht="29.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="100"/>
+      <c r="B41" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="DX4:ED4"/>
-    <mergeCell ref="EE4:EK4"/>
-    <mergeCell ref="EL4:ER4"/>
-    <mergeCell ref="ES4:EY4"/>
-    <mergeCell ref="DQ4:DW4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="CV4:DB4"/>
-    <mergeCell ref="DC4:DI4"/>
-    <mergeCell ref="DJ4:DP4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B5:G5"/>
@@ -12627,11 +13086,16 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="CV4:DB4"/>
+    <mergeCell ref="DC4:DI4"/>
+    <mergeCell ref="DJ4:DP4"/>
+    <mergeCell ref="DX4:ED4"/>
+    <mergeCell ref="EE4:EK4"/>
+    <mergeCell ref="EL4:ER4"/>
+    <mergeCell ref="ES4:EY4"/>
+    <mergeCell ref="DQ4:DW4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D26">
     <cfRule type="dataBar" priority="460">
@@ -14436,14 +14900,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7420F1CA-32AB-4ACF-A4DB-C234D43D244C}">
+  <sheetPr codeName="Hoja3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.95" x14ac:dyDescent="0.3"/>
   <cols>
@@ -14451,97 +14917,69 @@
     <col min="2" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="1:2" ht="46.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="115"/>
+    </row>
     <row r="2" spans="1:2" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
-        <v>19</v>
-      </c>
+      <c r="A2" s="20"/>
       <c r="B2" s="20"/>
     </row>
     <row r="3" spans="1:2" s="25" customFormat="1" ht="27.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
-        <v>20</v>
-      </c>
+      <c r="A3" s="26"/>
       <c r="B3" s="26"/>
     </row>
     <row r="4" spans="1:2" s="22" customFormat="1" ht="26.05" x14ac:dyDescent="0.5">
-      <c r="A4" s="23" t="s">
-        <v>21</v>
+      <c r="A4" s="114" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="58.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
-        <v>23</v>
+      <c r="A6" s="114" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="19" customFormat="1" ht="223.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
-        <v>24</v>
-      </c>
+    <row r="7" spans="1:2" s="19" customFormat="1" ht="91.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="41"/>
     </row>
     <row r="8" spans="1:2" s="22" customFormat="1" ht="26.05" x14ac:dyDescent="0.5">
-      <c r="A8" s="23" t="s">
-        <v>25</v>
-      </c>
+      <c r="A8" s="23"/>
     </row>
-    <row r="9" spans="1:2" ht="58.1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
-        <v>26</v>
-      </c>
+    <row r="9" spans="1:2" ht="14.55" x14ac:dyDescent="0.3">
+      <c r="A9" s="24"/>
     </row>
     <row r="10" spans="1:2" s="19" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="43" t="s">
-        <v>27</v>
-      </c>
+      <c r="A10" s="42"/>
     </row>
     <row r="11" spans="1:2" s="22" customFormat="1" ht="26.05" x14ac:dyDescent="0.5">
-      <c r="A11" s="23" t="s">
-        <v>28</v>
-      </c>
+      <c r="A11" s="23"/>
     </row>
-    <row r="12" spans="1:2" ht="29.05" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
-        <v>29</v>
-      </c>
+    <row r="12" spans="1:2" ht="14.55" x14ac:dyDescent="0.3">
+      <c r="A12" s="24"/>
     </row>
     <row r="13" spans="1:2" s="19" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
-        <v>30</v>
-      </c>
+      <c r="A13" s="42"/>
     </row>
     <row r="14" spans="1:2" s="22" customFormat="1" ht="26.05" x14ac:dyDescent="0.5">
-      <c r="A14" s="23" t="s">
-        <v>31</v>
-      </c>
+      <c r="A14" s="23"/>
     </row>
     <row r="15" spans="1:2" ht="91.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24" t="s">
-        <v>32</v>
-      </c>
+      <c r="A15" s="24"/>
     </row>
-    <row r="16" spans="1:2" ht="87.15" x14ac:dyDescent="0.3">
-      <c r="A16" s="24" t="s">
-        <v>33</v>
-      </c>
+    <row r="16" spans="1:2" ht="14.55" x14ac:dyDescent="0.3">
+      <c r="A16" s="24"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A13" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A10" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="A2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-  </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId5"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>